<commit_message>
Nearly finalized cave upper level
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C20680-417A-42DB-9145-3C1A5C835171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D8462-E2DA-4F3B-B3DF-6E9FEDD6F052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="1920" windowWidth="15330" windowHeight="10890" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -58,9 +58,6 @@
     <t>225: House has been renovated (by Karl)</t>
   </si>
   <si>
-    <t>226: unused</t>
-  </si>
-  <si>
     <t>227: Wind gate has been built (by Karl)</t>
   </si>
   <si>
@@ -206,12 +203,6 @@
   </si>
   <si>
     <t>World map with isle of winds</t>
-  </si>
-  <si>
-    <t>Added teleport to renovated house (with condition)
-Added wind gate teleport (with condition)
-Added cave teleport (with condition)
-NPC Karl can create a wind gate there</t>
   </si>
   <si>
     <t>Added wind gate teleport to your house (with condition)
@@ -284,6 +275,25 @@
   </si>
   <si>
     <t>3x Healing Potion III, 3x Spell Potion III, 1x Healing Potion IV</t>
+  </si>
+  <si>
+    <t>Old dwarf mine</t>
+  </si>
+  <si>
+    <t>Global var 226 is now set when you open the treasure room</t>
+  </si>
+  <si>
+    <t>226: You opened the treasure room in dwarf mine</t>
+  </si>
+  <si>
+    <t>Added teleport to renovated house (with condition)
+Added wind gate teleport (with condition)
+Added cave teleport (deactivated at start)
+Made back tiles below later cave black
+NPC Karl can create a wind gate there</t>
+  </si>
+  <si>
+    <t>235: You fell through a cave hole so that it create a hole below as well</t>
   </si>
 </sst>
 </file>
@@ -659,16 +669,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -676,13 +686,13 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -690,13 +700,13 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -704,10 +714,10 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,10 +725,10 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -726,13 +736,13 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
         <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -744,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -755,13 +765,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,10 +779,10 @@
         <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -782,9 +792,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -829,47 +841,52 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -892,38 +909,38 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -946,23 +963,23 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -985,13 +1002,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -999,10 +1016,10 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1025,13 +1042,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,7 +1059,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1067,16 +1084,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1084,13 +1101,13 @@
         <v>403</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,13 +1115,13 @@
         <v>404</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1112,13 +1129,13 @@
         <v>405</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
         <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,13 +1143,13 @@
         <v>406</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1157,16 +1174,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,13 +1191,13 @@
         <v>456</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,13 +1205,13 @@
         <v>457</v>
       </c>
       <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
         <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,13 +1219,13 @@
         <v>458</v>
       </c>
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
         <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1221,7 +1238,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,24 +1249,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>157</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1257,10 +1274,10 @@
         <v>198</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1268,10 +1285,10 @@
         <v>259</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1279,10 +1296,10 @@
         <v>262</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1290,10 +1307,10 @@
         <v>263</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1301,16 +1318,22 @@
         <v>273</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="5">
+        <v>438</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>

</xml_diff>

<commit_message>
Finalized your cave upper level
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D8462-E2DA-4F3B-B3DF-6E9FEDD6F052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BA572D-2C8A-471B-B662-1493601747CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -294,6 +294,24 @@
   </si>
   <si>
     <t>235: You fell through a cave hole so that it create a hole below as well</t>
+  </si>
+  <si>
+    <t>Your Cave (459)</t>
+  </si>
+  <si>
+    <t>1x Levitation, 1x Healing Potion II</t>
+  </si>
+  <si>
+    <t>Your Cave (460)</t>
+  </si>
+  <si>
+    <t>3x Torch</t>
+  </si>
+  <si>
+    <t>2x Rope</t>
+  </si>
+  <si>
+    <t>1x Rope</t>
   </si>
 </sst>
 </file>
@@ -752,10 +770,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,6 +803,61 @@
         <v>78</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -794,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Last will is now an important item, cave end pile also contains some wishing coins
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81323086-4AEE-4D40-A968-7A08DFA6D217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E335A7-0DBB-4CB9-BD10-CB8ED971D771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -321,9 +321,6 @@
     <t>Powerful ring dropped by the spider at the end of your cave</t>
   </si>
   <si>
-    <t>1x Karl's Ring</t>
-  </si>
-  <si>
     <t>Riesenspinne</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>237: You played with your dog once</t>
+  </si>
+  <si>
+    <t>1x Karl's Ring, 1x Wishing Coins</t>
   </si>
 </sst>
 </file>
@@ -760,10 +760,10 @@
         <v>258</v>
       </c>
       <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
         <v>98</v>
-      </c>
-      <c r="C4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -966,14 +966,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="83" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1061,7 +1061,7 @@
         <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1074,7 +1074,7 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,17 +1165,17 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1479,7 +1479,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
@@ -1488,7 +1488,7 @@
         <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I1" t="s">
         <v>35</v>
@@ -1502,19 +1502,19 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2">
         <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added signs for tow new places in Spannenberg, adjusted some early chest contents
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E335A7-0DBB-4CB9-BD10-CB8ED971D771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC09EBD2-453D-4986-8F10-26C1F29DFEAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="MapChanges" sheetId="9" r:id="rId10"/>
     <sheet name="NPCs" sheetId="10" r:id="rId11"/>
     <sheet name="Chests" sheetId="11" r:id="rId12"/>
+    <sheet name="TextChanges" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="110">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -350,12 +351,36 @@
   <si>
     <t>1x Karl's Ring, 1x Wishing Coins</t>
   </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Changed Chests</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Grandpa's cellar (259)</t>
+  </si>
+  <si>
+    <t>Removed all scrolls, ropes, strengthen potion and spell potions. Added short sword, lockpicks and a lantern.</t>
+  </si>
+  <si>
+    <t>Map 259 Text 9</t>
+  </si>
+  <si>
+    <t>As there are no more scrolls the text is adjusted.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,8 +388,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,8 +410,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -401,11 +440,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -418,6 +483,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -964,19 +1036,21 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="83" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="98.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -986,8 +1060,12 @@
       <c r="C1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>132</v>
       </c>
@@ -997,8 +1075,17 @@
       <c r="C2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>133</v>
       </c>
@@ -1008,8 +1095,17 @@
       <c r="C3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>134</v>
       </c>
@@ -1020,7 +1116,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>135</v>
       </c>
@@ -1031,7 +1127,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>136</v>
       </c>
@@ -1042,7 +1138,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>137</v>
       </c>
@@ -1053,7 +1149,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>138</v>
       </c>
@@ -1065,7 +1161,45 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A23AD0D-3B64-4BEF-82E1-7DFFB5EA7471}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added more depth and details to the cave
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC09EBD2-453D-4986-8F10-26C1F29DFEAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7C9701-B676-4045-A419-4906FD064D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A23AD0D-3B64-4BEF-82E1-7DFFB5EA7471}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19:N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Slightly empowered thief equip
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7C9701-B676-4045-A419-4906FD064D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A98A598-DE8E-4DB9-808A-A1B0D9DB9B68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="116">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -374,6 +374,24 @@
   </si>
   <si>
     <t>As there are no more scrolls the text is adjusted.</t>
+  </si>
+  <si>
+    <t>Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
+  </si>
+  <si>
+    <t>Changed Items</t>
+  </si>
+  <si>
+    <t>Murder Blade</t>
+  </si>
+  <si>
+    <t>Shadow Belt</t>
+  </si>
+  <si>
+    <t>Number of charges (Blink) increased from 5 to 15</t>
+  </si>
+  <si>
+    <t>Atk increased from 10 to 11, MagicWeaponLevel from 0 to 1</t>
   </si>
 </sst>
 </file>
@@ -417,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -466,11 +484,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -490,6 +519,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -772,10 +804,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1207,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1492,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,9 +1543,10 @@
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1518,8 +1559,13 @@
       <c r="D1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>403</v>
       </c>
@@ -1532,8 +1578,17 @@
       <c r="D2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>404</v>
       </c>
@@ -1546,8 +1601,17 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>249</v>
+      </c>
+      <c r="G3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>405</v>
       </c>
@@ -1560,8 +1624,17 @@
       <c r="D4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>251</v>
+      </c>
+      <c r="G4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>406</v>
       </c>
@@ -1575,7 +1648,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>407</v>
       </c>
@@ -1590,6 +1663,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated Thalion, Valdyn, Targor and Leonaria
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEE75EC-1505-4683-B534-964CFA8A9FBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBDBC86-1153-4EA9-A45C-9F460752CC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,8 @@
     <sheet name="Chests" sheetId="11" r:id="rId12"/>
     <sheet name="TextChanges" sheetId="13" r:id="rId13"/>
     <sheet name="TileChangeEvents" sheetId="14" r:id="rId14"/>
-    <sheet name="Tiles" sheetId="15" r:id="rId15"/>
+    <sheet name="CharChanges" sheetId="16" r:id="rId15"/>
+    <sheet name="Tiles" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="132">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -409,6 +410,39 @@
   </si>
   <si>
     <t>Cobweb</t>
+  </si>
+  <si>
+    <t>Char</t>
+  </si>
+  <si>
+    <t>Leonaria</t>
+  </si>
+  <si>
+    <t>SLP/Lvl 10 -&gt; 20</t>
+  </si>
+  <si>
+    <t>Changed start spells</t>
+  </si>
+  <si>
+    <t>Targor</t>
+  </si>
+  <si>
+    <t>Start SLP 20 -&gt; 25</t>
+  </si>
+  <si>
+    <t>Replace some start items</t>
+  </si>
+  <si>
+    <t>Valdyn</t>
+  </si>
+  <si>
+    <t>Added Monster Knowledge spell scroll</t>
+  </si>
+  <si>
+    <t>Start SLP 16 -&gt; 10</t>
+  </si>
+  <si>
+    <t>Remove Monster Knowledge as start spell</t>
   </si>
 </sst>
 </file>
@@ -516,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -539,6 +573,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1264,7 +1300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAC578B-0798-484E-AD11-E9A5E47BA266}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1281,6 +1317,106 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42293419-9ED8-4D74-9E3B-F691567047C5}">
   <dimension ref="A1:I10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated Sabine, Gryban and reverted SLP for Tar and Nelvin
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBDBC86-1153-4EA9-A45C-9F460752CC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19259D93-46F5-4772-84EB-F095D9CF7A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="138">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -443,6 +443,24 @@
   </si>
   <si>
     <t>Remove Monster Knowledge as start spell</t>
+  </si>
+  <si>
+    <t>Sabine</t>
+  </si>
+  <si>
+    <t>Start SLP 4 -&gt; 15</t>
+  </si>
+  <si>
+    <t>SLP/Lvl 10 -&gt; 18</t>
+  </si>
+  <si>
+    <t>Gryban</t>
+  </si>
+  <si>
+    <t>SLP/Lvl 3 -&gt; 5</t>
+  </si>
+  <si>
+    <t>Start SLP 19 -&gt; 20</t>
   </si>
 </sst>
 </file>
@@ -1318,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,6 +1426,46 @@
       </c>
       <c r="B10" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted SLP values for all white, blue and green spells
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19259D93-46F5-4772-84EB-F095D9CF7A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC17881-7D38-4BDE-B358-EB261DA2D7D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="TileChangeEvents" sheetId="14" r:id="rId14"/>
     <sheet name="CharChanges" sheetId="16" r:id="rId15"/>
     <sheet name="Tiles" sheetId="15" r:id="rId16"/>
+    <sheet name="SpellChanges" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="211">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -461,6 +462,225 @@
   </si>
   <si>
     <t>Start SLP 19 -&gt; 20</t>
+  </si>
+  <si>
+    <t>- Charge Item: 20 -&gt; 60</t>
+  </si>
+  <si>
+    <t>- Repair Item: 15 -&gt; 45</t>
+  </si>
+  <si>
+    <t>- Duplicate Item: 25 -&gt; 75</t>
+  </si>
+  <si>
+    <t>- LP Stealer: 5 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- SP Stealer: 5 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Light: 2 -&gt; 5</t>
+  </si>
+  <si>
+    <t>- Magical Torch: 5 -&gt; 10</t>
+  </si>
+  <si>
+    <t>- Magical Lantern: 10 -&gt; 20</t>
+  </si>
+  <si>
+    <t>- Magical Sun: 15 -&gt; 35</t>
+  </si>
+  <si>
+    <t>- Ghost Weapon: 5 -&gt; 30</t>
+  </si>
+  <si>
+    <t>- Create Food: 10 -&gt; 15</t>
+  </si>
+  <si>
+    <t>- Blink: 5 -&gt; 15</t>
+  </si>
+  <si>
+    <t>- Jump: 10 -&gt; 50</t>
+  </si>
+  <si>
+    <t>- Word Of Marking: 20 -&gt; 70</t>
+  </si>
+  <si>
+    <t>- Word Of Returning: 20 -&gt; 80</t>
+  </si>
+  <si>
+    <t>- Magic Shield: 10 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Magic Wall: 15 -&gt; 35</t>
+  </si>
+  <si>
+    <t>- Magic Barrier: 20 -&gt; 45</t>
+  </si>
+  <si>
+    <t>- Magic Weapon: 10 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Magic Assault: 15 -&gt; 35</t>
+  </si>
+  <si>
+    <t>- Magic Attack: 20 -&gt; 45</t>
+  </si>
+  <si>
+    <t>- Levitation: 10 -&gt; 65</t>
+  </si>
+  <si>
+    <t>- Anti-Magic Wall: 5 -&gt; 30</t>
+  </si>
+  <si>
+    <t>- Anti-Magic Sphere: 15 -&gt; 50</t>
+  </si>
+  <si>
+    <t>- Alch. Globe: 25 -&gt; 120</t>
+  </si>
+  <si>
+    <t>- Hurry: 5 -&gt; 50</t>
+  </si>
+  <si>
+    <t>- Mass Hurry: 10 -&gt; 80</t>
+  </si>
+  <si>
+    <t>SLP Changes</t>
+  </si>
+  <si>
+    <t>- Monster Knowledge: 3 -&gt; 15</t>
+  </si>
+  <si>
+    <t>- Identification: 15 -&gt; 35</t>
+  </si>
+  <si>
+    <t>- Knowledge: 10 -&gt; 5</t>
+  </si>
+  <si>
+    <t>- Clairvoyance: 20 -&gt; 15</t>
+  </si>
+  <si>
+    <t>- Map View: 15 -&gt; 20</t>
+  </si>
+  <si>
+    <t>- Magical Compass: 2 -&gt; 5</t>
+  </si>
+  <si>
+    <t>- Find Traps: 10 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Find Monsters: 10 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Find Persons: 10 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Find Secret Doors: 10 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Mystical Mapping: 25 -&gt; 70</t>
+  </si>
+  <si>
+    <t>- Mystical Map I: 10 -&gt; 75</t>
+  </si>
+  <si>
+    <t>- Mystical Map II: 15 -&gt; 80</t>
+  </si>
+  <si>
+    <t>- Mystical Map III: 20 -&gt; 85</t>
+  </si>
+  <si>
+    <t>- Myst. Globe: 25 -&gt; 100</t>
+  </si>
+  <si>
+    <t>- Show Monster LP: 5 -&gt; 15</t>
+  </si>
+  <si>
+    <t>- Healing Hand: 1 -&gt; 5</t>
+  </si>
+  <si>
+    <t>- Remove Fear: 2 -&gt; 10</t>
+  </si>
+  <si>
+    <t>- Remove Panic: 5 -&gt; 20</t>
+  </si>
+  <si>
+    <t>- Remove Shadows: 3 -&gt; 10</t>
+  </si>
+  <si>
+    <t>- Remove Blindness: 8 -&gt; 20</t>
+  </si>
+  <si>
+    <t>- Remove Pain: 5 -&gt; 20</t>
+  </si>
+  <si>
+    <t>- Remove Disease: 10 -&gt; 30</t>
+  </si>
+  <si>
+    <t>- Small Healing: 5 -&gt; 20</t>
+  </si>
+  <si>
+    <t>- Remove Poison: 10 -&gt; 30</t>
+  </si>
+  <si>
+    <t>- Neutralize Poison: 12 -&gt; 45</t>
+  </si>
+  <si>
+    <t>- Medium Healing: 15 -&gt; 40</t>
+  </si>
+  <si>
+    <t>- Destroy Undead: 15 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Holy Word: 20 -&gt; 50</t>
+  </si>
+  <si>
+    <t>- Wake The Dead: 15 -&gt; 80</t>
+  </si>
+  <si>
+    <t>- Change Ashes: 20 -&gt; 50</t>
+  </si>
+  <si>
+    <t>- Change Dust: 25 -&gt; 50</t>
+  </si>
+  <si>
+    <t>- Great Healing: 30 -&gt; 75</t>
+  </si>
+  <si>
+    <t>- Mass Healing: 20 -&gt; 60</t>
+  </si>
+  <si>
+    <t>- Resurrection: 30 -&gt; 120</t>
+  </si>
+  <si>
+    <t>- Remove Rigidness: 5 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Remove Lamedness: 10 -&gt; 35</t>
+  </si>
+  <si>
+    <t>- Heal Aging: 12 -&gt; 15</t>
+  </si>
+  <si>
+    <t>- Stop Aging: 15 -&gt; 20</t>
+  </si>
+  <si>
+    <t>- Stone To Flesh: 20 -&gt; 55</t>
+  </si>
+  <si>
+    <t>- Wake Up: 5 -&gt; 10</t>
+  </si>
+  <si>
+    <t>- Remove Irritation: 5 -&gt; 25</t>
+  </si>
+  <si>
+    <t>- Remove Drugs: 10 -&gt; 15</t>
+  </si>
+  <si>
+    <t>- Remove Madness: 15 -&gt; 50</t>
+  </si>
+  <si>
+    <t>- Restore Stamina: 15 -&gt; 5</t>
   </si>
 </sst>
 </file>
@@ -568,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -582,6 +802,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -591,8 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -876,7 +1097,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,10 +1392,10 @@
       <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1338,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1349,10 +1570,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1489,16 +1710,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
-      <c r="G1" s="7" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="G1" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1685,6 +1906,389 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
+  <dimension ref="A1:A75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2005,11 +2609,11 @@
       <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>

<commit_message>
Prepared first sea creature quest
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC17881-7D38-4BDE-B358-EB261DA2D7D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3274496B-0732-4578-8679-FD8B300B1FD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="217">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -681,6 +681,24 @@
   </si>
   <si>
     <t>- Restore Stamina: 15 -&gt; 5</t>
+  </si>
+  <si>
+    <t>120: KARTE / MAP</t>
+  </si>
+  <si>
+    <t>121: KREATUREN DER SEE / SEA CREATURES</t>
+  </si>
+  <si>
+    <t>238: You got the journal (log) from Torle</t>
+  </si>
+  <si>
+    <t>Torle's Logbuch / Torle's Journal</t>
+  </si>
+  <si>
+    <t>Contains the coordinates and or hints to all sea creatures</t>
+  </si>
+  <si>
+    <t>Text of Torle's journal</t>
   </si>
 </sst>
 </file>
@@ -1914,7 +1932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
   <dimension ref="A1:A75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -2295,10 +2313,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,6 +2420,11 @@
         <v>100</v>
       </c>
     </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2409,10 +2432,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC73B1D-C705-4EA8-84D8-EC14D78F4581}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,6 +2477,16 @@
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2542,10 +2575,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6453DC1-51C9-48F1-850E-8100CA0FECA0}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,6 +2608,17 @@
         <v>34</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2582,15 +2626,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
@@ -2710,6 +2754,20 @@
       </c>
       <c r="D6" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>408</v>
+      </c>
+      <c r="B7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added first sea event
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3274496B-0732-4578-8679-FD8B300B1FD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DF3748-3803-4428-96F0-611BF6CDFF3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="218">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -699,6 +699,9 @@
   </si>
   <si>
     <t>Text of Torle's journal</t>
+  </si>
+  <si>
+    <t>239: Visited the giant turtle</t>
   </si>
 </sst>
 </file>
@@ -2313,10 +2316,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,6 +2426,11 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2577,7 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6453DC1-51C9-48F1-850E-8100CA0FECA0}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added sea snake event
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DF3748-3803-4428-96F0-611BF6CDFF3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C761D0-2C67-42A6-AA42-E6A5AC7FC0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15630" yWindow="9585" windowWidth="15330" windowHeight="10890" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,8 @@
     <sheet name="CharChanges" sheetId="16" r:id="rId15"/>
     <sheet name="Tiles" sheetId="15" r:id="rId16"/>
     <sheet name="SpellChanges" sheetId="17" r:id="rId17"/>
+    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId18"/>
+    <sheet name="Tabelle3" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="221">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -702,6 +704,15 @@
   </si>
   <si>
     <t>239: Visited the giant turtle</t>
+  </si>
+  <si>
+    <t>Turtle at 550,402</t>
+  </si>
+  <si>
+    <t>240: Visited the giant water snake</t>
+  </si>
+  <si>
+    <t>Snake at 773,313</t>
   </si>
 </sst>
 </file>
@@ -825,6 +836,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -834,7 +846,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1413,10 +1424,10 @@
       <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1731,16 +1742,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
-      <c r="G1" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="G1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1945,7 +1956,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2310,16 +2321,56 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A938DC3D-143F-4871-88FF-86347B3EB68B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBBD23D-83D2-4AFD-8FE1-B7316E06FB79}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2431,6 +2482,11 @@
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2661,11 +2717,11 @@
       <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>

<commit_message>
Added first maps for the sea quests
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,30 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C761D0-2C67-42A6-AA42-E6A5AC7FC0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBB1374-0E54-42F4-9693-3A0790A9F22C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15630" yWindow="9585" windowWidth="15330" windowHeight="10890" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="GlobalVars" sheetId="2" r:id="rId2"/>
-    <sheet name="Keywords" sheetId="3" r:id="rId3"/>
-    <sheet name="GotoPoints" sheetId="4" r:id="rId4"/>
-    <sheet name="Places" sheetId="5" r:id="rId5"/>
-    <sheet name="ObjectTexts" sheetId="6" r:id="rId6"/>
-    <sheet name="Items" sheetId="7" r:id="rId7"/>
-    <sheet name="Monsters" sheetId="12" r:id="rId8"/>
-    <sheet name="Maps" sheetId="8" r:id="rId9"/>
-    <sheet name="MapChanges" sheetId="9" r:id="rId10"/>
-    <sheet name="NPCs" sheetId="10" r:id="rId11"/>
-    <sheet name="Chests" sheetId="11" r:id="rId12"/>
-    <sheet name="TextChanges" sheetId="13" r:id="rId13"/>
-    <sheet name="TileChangeEvents" sheetId="14" r:id="rId14"/>
-    <sheet name="CharChanges" sheetId="16" r:id="rId15"/>
-    <sheet name="Tiles" sheetId="15" r:id="rId16"/>
-    <sheet name="SpellChanges" sheetId="17" r:id="rId17"/>
-    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId18"/>
-    <sheet name="Tabelle3" sheetId="19" r:id="rId19"/>
+    <sheet name="Todo" sheetId="20" r:id="rId2"/>
+    <sheet name="GlobalVars" sheetId="2" r:id="rId3"/>
+    <sheet name="Keywords" sheetId="3" r:id="rId4"/>
+    <sheet name="GotoPoints" sheetId="4" r:id="rId5"/>
+    <sheet name="Places" sheetId="5" r:id="rId6"/>
+    <sheet name="ObjectTexts" sheetId="6" r:id="rId7"/>
+    <sheet name="Items" sheetId="7" r:id="rId8"/>
+    <sheet name="Monsters" sheetId="12" r:id="rId9"/>
+    <sheet name="Maps" sheetId="8" r:id="rId10"/>
+    <sheet name="MapChanges" sheetId="9" r:id="rId11"/>
+    <sheet name="NPCs" sheetId="10" r:id="rId12"/>
+    <sheet name="Chests" sheetId="11" r:id="rId13"/>
+    <sheet name="TextChanges" sheetId="13" r:id="rId14"/>
+    <sheet name="TileChangeEvents" sheetId="14" r:id="rId15"/>
+    <sheet name="CharChanges" sheetId="16" r:id="rId16"/>
+    <sheet name="Tiles" sheetId="15" r:id="rId17"/>
+    <sheet name="SpellChanges" sheetId="17" r:id="rId18"/>
+    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId19"/>
+    <sheet name="Tabelle3" sheetId="19" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="233">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -192,13 +193,7 @@
     <t>Architektenbüro / Architect's Office</t>
   </si>
   <si>
-    <t>You can met Karl the architect here who can renovate your house, create a wind gate or a cave</t>
-  </si>
-  <si>
     <t>Tierhandlung / Pet Shop</t>
-  </si>
-  <si>
-    <t>You can met Ferdinand who sells you a cat and a dog, there is also a merchant for pet stuff</t>
   </si>
   <si>
     <t>Dein Haus / Your House</t>
@@ -713,6 +708,48 @@
   </si>
   <si>
     <t>Snake at 773,313</t>
+  </si>
+  <si>
+    <t>Auge des Strudels / Eye of the vortex</t>
+  </si>
+  <si>
+    <t>Deine Höhle - Obere Ebene / Your Cave - Upper Level</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>Deine Höhle - Untere Ebene / Your Cave - Lower Level</t>
+  </si>
+  <si>
+    <t>Small cave, Karl built for your</t>
+  </si>
+  <si>
+    <t>Map inside the vortex</t>
+  </si>
+  <si>
+    <t>Höhle der Meerjungfrau / Cave of the mermaid</t>
+  </si>
+  <si>
+    <t>You can meet the Mermaid here</t>
+  </si>
+  <si>
+    <t>You can meet Karl the architect here who can renovate your house, create a wind gate or a cave</t>
+  </si>
+  <si>
+    <t>You can meet Ferdinand who sells you a cat and a dog, there is also a merchant for pet stuff</t>
+  </si>
+  <si>
+    <t>Ship's end</t>
+  </si>
+  <si>
+    <t>Abandoned village inside the vortex</t>
+  </si>
+  <si>
+    <t>The wooden tree root, lizard, pile of trash and green liquid are not part of 3Objects.amb therefore they must be added there. Maybe smaller or even different versions.</t>
+  </si>
+  <si>
+    <t>the teleports to same map in Ship's End which use map index 0 seem to teleport to map 0. I guess index 372 is necessary there.</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1173,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1145,6 +1182,152 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD8B38F-295E-46BA-A316-56C9E4745E5F}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" customWidth="1"/>
+    <col min="4" max="4" width="85.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>456</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>457</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>458</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>459</v>
+      </c>
+      <c r="B5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>460</v>
+      </c>
+      <c r="B6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>370</v>
+      </c>
+      <c r="B7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>371</v>
+      </c>
+      <c r="B8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>372</v>
+      </c>
+      <c r="B9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8633A58-1CC4-49CC-A9EF-ED848DF63C3A}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -1174,10 +1357,10 @@
         <v>157</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1185,10 +1368,10 @@
         <v>198</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,10 +1379,10 @@
         <v>258</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,10 +1390,10 @@
         <v>259</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,10 +1401,10 @@
         <v>262</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1229,10 +1412,10 @@
         <v>263</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,10 +1423,10 @@
         <v>273</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1251,10 +1434,10 @@
         <v>438</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1301,7 +1484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1323,7 +1506,7 @@
         <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
         <v>33</v>
@@ -1334,13 +1517,13 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1348,13 +1531,13 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1362,10 +1545,10 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1373,10 +1556,10 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,13 +1567,13 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1398,7 +1581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1419,13 +1602,13 @@
         <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F1" s="12"/>
     </row>
@@ -1434,19 +1617,19 @@
         <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1454,19 +1637,19 @@
         <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E3">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1474,10 +1657,10 @@
         <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1485,10 +1668,10 @@
         <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1496,10 +1679,10 @@
         <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1507,10 +1690,10 @@
         <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1518,10 +1701,10 @@
         <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1532,7 +1715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A23AD0D-3B64-4BEF-82E1-7DFFB5EA7471}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1547,18 +1730,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1567,7 +1750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAC578B-0798-484E-AD11-E9A5E47BA266}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1579,7 +1762,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1587,7 +1770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -1603,122 +1786,122 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
         <v>122</v>
-      </c>
-      <c r="B3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
         <v>125</v>
-      </c>
-      <c r="B7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s">
         <v>128</v>
-      </c>
-      <c r="B9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
         <v>132</v>
-      </c>
-      <c r="B12" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" t="s">
         <v>135</v>
-      </c>
-      <c r="B15" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1727,7 +1910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42293419-9ED8-4D74-9E3B-F691567047C5}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -1743,19 +1926,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
       <c r="G1" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1764,7 +1947,7 @@
         <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -1781,7 +1964,7 @@
         <v>1193</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -1790,7 +1973,7 @@
         <v>1167</v>
       </c>
       <c r="I3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1801,7 +1984,7 @@
         <v>1194</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -1810,7 +1993,7 @@
         <v>1168</v>
       </c>
       <c r="I4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1821,7 +2004,7 @@
         <v>1195</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -1830,7 +2013,7 @@
         <v>1169</v>
       </c>
       <c r="I5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1841,7 +2024,7 @@
         <v>1196</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -1850,7 +2033,7 @@
         <v>1170</v>
       </c>
       <c r="I6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1861,7 +2044,7 @@
         <v>1197</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -1870,7 +2053,7 @@
         <v>1171</v>
       </c>
       <c r="I7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1881,7 +2064,7 @@
         <v>1198</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -1890,7 +2073,7 @@
         <v>1172</v>
       </c>
       <c r="I8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1901,7 +2084,7 @@
         <v>1199</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -1910,7 +2093,7 @@
         <v>1173</v>
       </c>
       <c r="I9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1921,7 +2104,7 @@
         <v>1200</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -1930,7 +2113,7 @@
         <v>1174</v>
       </c>
       <c r="I10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1942,7 +2125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
   <dimension ref="A1:A75"/>
   <sheetViews>
@@ -1957,367 +2140,367 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2325,11 +2508,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A938DC3D-143F-4871-88FF-86347B3EB68B}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2340,12 +2523,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2353,7 +2536,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBBD23D-83D2-4AFD-8FE1-B7316E06FB79}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2365,7 +2573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
   <dimension ref="A1:A23"/>
   <sheetViews>
@@ -2416,7 +2624,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -2461,32 +2669,32 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2494,7 +2702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC73B1D-C705-4EA8-84D8-EC14D78F4581}">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -2545,12 +2753,12 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2558,7 +2766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910D7988-B5EE-4331-AF20-D4792C0F4C16}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -2597,7 +2805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3244EE-9DE8-4394-8A72-E957F0B76A39}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2637,7 +2845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6453DC1-51C9-48F1-850E-8100CA0FECA0}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2680,7 +2888,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2688,7 +2896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -2718,7 +2926,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G1" s="11"/>
       <c r="H1" s="12"/>
@@ -2743,7 +2951,7 @@
         <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2763,10 +2971,10 @@
         <v>249</v>
       </c>
       <c r="G3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2786,10 +2994,10 @@
         <v>251</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2811,13 +3019,13 @@
         <v>407</v>
       </c>
       <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
         <v>89</v>
-      </c>
-      <c r="C6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2825,13 +3033,13 @@
         <v>408</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2842,7 +3050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -2861,7 +3069,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
@@ -2870,7 +3078,7 @@
         <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I1" t="s">
         <v>35</v>
@@ -2884,95 +3092,19 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
       </c>
       <c r="H2">
         <v>87</v>
       </c>
       <c r="I2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" t="s">
         <v>92</v>
-      </c>
-      <c r="J2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD8B38F-295E-46BA-A316-56C9E4745E5F}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>456</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>457</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>458</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed ship's end map
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBB1374-0E54-42F4-9693-3A0790A9F22C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83067D5-2046-4F15-943F-2DDDB4F4D94A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,10 +29,11 @@
     <sheet name="TextChanges" sheetId="13" r:id="rId14"/>
     <sheet name="TileChangeEvents" sheetId="14" r:id="rId15"/>
     <sheet name="CharChanges" sheetId="16" r:id="rId16"/>
-    <sheet name="Tiles" sheetId="15" r:id="rId17"/>
-    <sheet name="SpellChanges" sheetId="17" r:id="rId18"/>
-    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId19"/>
-    <sheet name="Tabelle3" sheetId="19" r:id="rId20"/>
+    <sheet name="New Object Graphics" sheetId="21" r:id="rId17"/>
+    <sheet name="Tiles" sheetId="15" r:id="rId18"/>
+    <sheet name="SpellChanges" sheetId="17" r:id="rId19"/>
+    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId20"/>
+    <sheet name="Tabelle3" sheetId="19" r:id="rId21"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="242">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -746,10 +747,37 @@
     <t>Abandoned village inside the vortex</t>
   </si>
   <si>
-    <t>The wooden tree root, lizard, pile of trash and green liquid are not part of 3Objects.amb therefore they must be added there. Maybe smaller or even different versions.</t>
-  </si>
-  <si>
-    <t>the teleports to same map in Ship's End which use map index 0 seem to teleport to map 0. I guess index 372 is necessary there.</t>
+    <t>Fix dog house tile icons in map 457</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Smaller version of the lizard</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>3Object3D.amb</t>
+  </si>
+  <si>
+    <t>New / Copy</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>Tree root</t>
+  </si>
+  <si>
+    <t>Green liquid</t>
+  </si>
+  <si>
+    <t>Pile of trash</t>
   </si>
 </sst>
 </file>
@@ -793,7 +821,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -853,11 +881,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -883,6 +956,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1911,6 +1987,111 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFAD946-A9D1-4502-A6CF-B93E446D51BE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42293419-9ED8-4D74-9E3B-F691567047C5}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -2125,7 +2306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
   <dimension ref="A1:A75"/>
   <sheetViews>
@@ -2508,7 +2689,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A938DC3D-143F-4871-88FF-86347B3EB68B}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2536,32 +2737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBBD23D-83D2-4AFD-8FE1-B7316E06FB79}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added new spider monsters and new 2D map 'abandoned hut'
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83067D5-2046-4F15-943F-2DDDB4F4D94A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D0EA91-D5B7-4935-92B0-A073015FF63F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="246">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -778,6 +778,18 @@
   </si>
   <si>
     <t>Pile of trash</t>
+  </si>
+  <si>
+    <t>Höhlenspinne</t>
+  </si>
+  <si>
+    <t>Monster in Ship's end</t>
+  </si>
+  <si>
+    <t>3x Höhlenspinne</t>
+  </si>
+  <si>
+    <t>4x Höhlenspinne</t>
   </si>
 </sst>
 </file>
@@ -2693,7 +2705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3228,10 +3240,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3283,6 +3295,31 @@
         <v>92</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s">
+        <v>245</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added life to the vortex map and improved some tiles
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D0EA91-D5B7-4935-92B0-A073015FF63F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0E9C32-32E4-423F-A60B-421C983D2A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="248">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -790,6 +790,12 @@
   </si>
   <si>
     <t>4x Höhlenspinne</t>
+  </si>
+  <si>
+    <t>Verlassene Hütte / Abandoned Hut</t>
+  </si>
+  <si>
+    <t>Abandoned hut in Ship's end</t>
   </si>
 </sst>
 </file>
@@ -1271,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD8B38F-295E-46BA-A316-56C9E4745E5F}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,6 +1414,20 @@
       </c>
       <c r="D9" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>373</v>
+      </c>
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3242,7 +3262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added all sea monster events and mermaid cave entering
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F4EDA4-7D2D-4A58-A9FE-D142A57D92E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920DAD24-B2E4-4B0B-853F-6ABF5D924066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="SpellChanges" sheetId="17" r:id="rId19"/>
     <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId20"/>
     <sheet name="Tabelle3" sheetId="19" r:id="rId21"/>
+    <sheet name="Tabelle2" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="264">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -702,15 +703,9 @@
     <t>239: Visited the giant turtle</t>
   </si>
   <si>
-    <t>Turtle at 550,402</t>
-  </si>
-  <si>
     <t>240: Visited the giant water snake</t>
   </si>
   <si>
-    <t>Snake at 773,313</t>
-  </si>
-  <si>
     <t>Auge des Strudels / Eye of the vortex</t>
   </si>
   <si>
@@ -814,6 +809,42 @@
   </si>
   <si>
     <t>1x Wind Pearl</t>
+  </si>
+  <si>
+    <t>242: Visited the giant whale</t>
+  </si>
+  <si>
+    <t>243: Visited the giant sword fish</t>
+  </si>
+  <si>
+    <t>244: Visited the giant piranha</t>
+  </si>
+  <si>
+    <t>Piranha at 311, 446 (map 135)</t>
+  </si>
+  <si>
+    <t>Turtle at 550,402 (map 139)</t>
+  </si>
+  <si>
+    <t>Mermaid at 126,530 (map 163)</t>
+  </si>
+  <si>
+    <t>Whale at 173, 773 (map 244)</t>
+  </si>
+  <si>
+    <t>Snake at 773,313 (map 112)</t>
+  </si>
+  <si>
+    <t>Swordfish at 621, 205 (map 77)</t>
+  </si>
+  <si>
+    <t>Finalize Torle's journal text</t>
+  </si>
+  <si>
+    <t>Finalize cave of the mermaid</t>
+  </si>
+  <si>
+    <t>Create manyeyes town and castle</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1364,7 @@
         <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,7 +1378,7 @@
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1369,13 +1400,13 @@
         <v>459</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" t="s">
         <v>221</v>
-      </c>
-      <c r="D5" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1383,13 +1414,13 @@
         <v>460</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" t="s">
         <v>221</v>
-      </c>
-      <c r="D6" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1397,13 +1428,13 @@
         <v>370</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C7" t="s">
         <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,13 +1442,13 @@
         <v>371</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C8" t="s">
         <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1425,13 +1456,13 @@
         <v>372</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,13 +1470,13 @@
         <v>373</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1711,7 +1742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1838,10 +1869,10 @@
         <v>139</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1849,10 +1880,10 @@
         <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1860,10 +1891,10 @@
         <v>141</v>
       </c>
       <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="s">
         <v>249</v>
-      </c>
-      <c r="C11" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1871,10 +1902,10 @@
         <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2096,19 +2127,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2116,16 +2147,16 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E2" t="s">
         <v>236</v>
-      </c>
-      <c r="E2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2133,16 +2164,16 @@
         <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" t="s">
         <v>236</v>
-      </c>
-      <c r="E3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2150,16 +2181,16 @@
         <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" t="s">
         <v>236</v>
-      </c>
-      <c r="E4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2167,16 +2198,16 @@
         <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E5" t="s">
         <v>236</v>
-      </c>
-      <c r="E5" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2785,17 +2816,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2805,10 +2851,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A938DC3D-143F-4871-88FF-86347B3EB68B}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,12 +2864,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2843,12 +2909,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303F205F-3A3D-43F3-9B99-BFC12608D1EA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,12 +3042,27 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>248</v>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3387,16 +3480,16 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H3">
         <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3404,7 +3497,7 @@
         <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added most parts of cavetown
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920DAD24-B2E4-4B0B-853F-6ABF5D924066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DEB2F9-21A3-452F-A3B4-8E8AD652E33A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="276">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -845,6 +845,42 @@
   </si>
   <si>
     <t>Create manyeyes town and castle</t>
+  </si>
+  <si>
+    <t>I guess I added wrong events to 372 or 373</t>
+  </si>
+  <si>
+    <t>79: Warenhändler / Good merchant (Cavetown)</t>
+  </si>
+  <si>
+    <t>80: Schmied / Blacksmith (Cavetown)</t>
+  </si>
+  <si>
+    <t>81: Cavetown Büro / Cavetown Office (Cavetown)</t>
+  </si>
+  <si>
+    <t>82: Vielauge-Schloss / Manyeyes' Castle (Cavetown)</t>
+  </si>
+  <si>
+    <t>83: Gasthaus / Tavern (Cavetown)</t>
+  </si>
+  <si>
+    <t>84: Badehaus / Bathhouse (Cavetown)</t>
+  </si>
+  <si>
+    <t>85: Flosshändler / Raft Dealer (Cavetown)</t>
+  </si>
+  <si>
+    <t>86: Gasthaus / Tavern (Cavetown) -- Second door</t>
+  </si>
+  <si>
+    <t>87: Stadthaus 1 / Townhouse 1 (Cavetown)</t>
+  </si>
+  <si>
+    <t>88: Stadthaus 2 / Townhouse 2 (Cavetown)</t>
+  </si>
+  <si>
+    <t>89: Stadthaus 3 / Townhouse 3 (Cavetown)</t>
   </si>
 </sst>
 </file>
@@ -1014,6 +1050,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1023,9 +1062,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1764,10 +1800,10 @@
       <c r="C1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="12"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -2126,19 +2162,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2231,16 +2267,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
-      <c r="G1" s="10" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="G1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="12"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2816,10 +2852,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2842,6 +2878,11 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3136,10 +3177,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910D7988-B5EE-4331-AF20-D4792C0F4C16}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,6 +3207,61 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3293,11 +3389,11 @@
       <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>

<commit_message>
Added life to cavetown
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DEB2F9-21A3-452F-A3B4-8E8AD652E33A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597DBA14-9A1A-4825-9D87-BE1422F68D79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="283">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -881,6 +881,27 @@
   </si>
   <si>
     <t>89: Stadthaus 3 / Townhouse 3 (Cavetown)</t>
+  </si>
+  <si>
+    <t>Blacksmith</t>
+  </si>
+  <si>
+    <t>Raft Dealer</t>
+  </si>
+  <si>
+    <t>Merchant Index 20: todo</t>
+  </si>
+  <si>
+    <t>A bit more expensive (35) than Burnville blacksmith (25)</t>
+  </si>
+  <si>
+    <t>A bit more expensive (20) than Burnville swim trainer (10)</t>
+  </si>
+  <si>
+    <t>Swim Trainer</t>
+  </si>
+  <si>
+    <t>350 Gold per raft, spawns east of Cavetown at the beach</t>
   </si>
 </sst>
 </file>
@@ -3179,7 +3200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910D7988-B5EE-4331-AF20-D4792C0F4C16}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3271,14 +3292,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3244EE-9DE8-4394-8A72-E957F0B76A39}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3302,6 +3324,50 @@
       </c>
       <c r="C2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed automap walls in hill caves, beast cave and newlake palace
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597DBA14-9A1A-4825-9D87-BE1422F68D79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D10627-FAE9-4404-A46A-2111CB4D535D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="284">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -844,9 +844,6 @@
     <t>Finalize cave of the mermaid</t>
   </si>
   <si>
-    <t>Create manyeyes town and castle</t>
-  </si>
-  <si>
     <t>I guess I added wrong events to 372 or 373</t>
   </si>
   <si>
@@ -902,6 +899,12 @@
   </si>
   <si>
     <t>350 Gold per raft, spawns east of Cavetown at the beach</t>
+  </si>
+  <si>
+    <t>Create manyeyes castle</t>
+  </si>
+  <si>
+    <t>Finish cavetown</t>
   </si>
 </sst>
 </file>
@@ -2873,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,12 +2901,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>264</v>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3232,57 +3240,57 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3294,8 +3302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3244EE-9DE8-4394-8A72-E957F0B76A39}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3334,7 +3342,7 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3342,10 +3350,10 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3353,10 +3361,10 @@
         <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3364,10 +3372,10 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved Karl cave quest
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D10627-FAE9-4404-A46A-2111CB4D535D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E480414-8D77-40CE-9F24-96F0C5CAFE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="286">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -280,15 +280,6 @@
   </si>
   <si>
     <t>3x Healing Potion III, 3x Spell Potion III, 1x Healing Potion IV</t>
-  </si>
-  <si>
-    <t>Old dwarf mine</t>
-  </si>
-  <si>
-    <t>Global var 226 is now set when you open the treasure room</t>
-  </si>
-  <si>
-    <t>226: You opened the treasure room in dwarf mine</t>
   </si>
   <si>
     <t>Added teleport to renovated house (with condition)
@@ -905,6 +896,21 @@
   </si>
   <si>
     <t>Finish cavetown</t>
+  </si>
+  <si>
+    <t>226: You visited the tavern in Snakesign</t>
+  </si>
+  <si>
+    <t>Tavern of the goddess</t>
+  </si>
+  <si>
+    <t>Snakesign</t>
+  </si>
+  <si>
+    <t>Added drunken NPC</t>
+  </si>
+  <si>
+    <t>Global var 226 is now set when you enter the tavern, added NPC who talks about Karl</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1382,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1424,7 +1430,7 @@
         <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,7 +1444,7 @@
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1460,13 +1466,13 @@
         <v>459</v>
       </c>
       <c r="B5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" t="s">
         <v>218</v>
-      </c>
-      <c r="C5" t="s">
-        <v>219</v>
-      </c>
-      <c r="D5" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1474,13 +1480,13 @@
         <v>460</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1488,13 +1494,13 @@
         <v>370</v>
       </c>
       <c r="B7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C7" t="s">
         <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1502,13 +1508,13 @@
         <v>371</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C8" t="s">
         <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1516,13 +1522,13 @@
         <v>372</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1530,13 +1536,13 @@
         <v>373</v>
       </c>
       <c r="B10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1548,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8633A58-1CC4-49CC-A9EF-ED848DF63C3A}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1583,7 @@
         <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1596,10 +1602,10 @@
         <v>258</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1648,19 +1654,25 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>283</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>421</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -1825,7 +1837,7 @@
         <v>75</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1846,7 +1858,7 @@
         <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1854,19 +1866,19 @@
         <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1874,10 +1886,10 @@
         <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1885,10 +1897,10 @@
         <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1896,10 +1908,10 @@
         <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1907,10 +1919,10 @@
         <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1918,10 +1930,10 @@
         <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1929,10 +1941,10 @@
         <v>139</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1940,10 +1952,10 @@
         <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1951,10 +1963,10 @@
         <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1962,10 +1974,10 @@
         <v>142</v>
       </c>
       <c r="B12" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" t="s">
         <v>247</v>
-      </c>
-      <c r="C12" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1991,18 +2003,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2023,7 +2035,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2047,122 +2059,122 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
         <v>126</v>
-      </c>
-      <c r="B10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2187,19 +2199,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>232</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2207,16 +2219,16 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" t="s">
         <v>231</v>
       </c>
-      <c r="C2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D2" t="s">
-        <v>234</v>
-      </c>
       <c r="E2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2224,16 +2236,16 @@
         <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2241,16 +2253,16 @@
         <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2258,16 +2270,16 @@
         <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2292,19 +2304,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="15"/>
       <c r="G1" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -2313,7 +2325,7 @@
         <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2330,7 +2342,7 @@
         <v>1193</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -2339,7 +2351,7 @@
         <v>1167</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2350,7 +2362,7 @@
         <v>1194</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -2359,7 +2371,7 @@
         <v>1168</v>
       </c>
       <c r="I4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2370,7 +2382,7 @@
         <v>1195</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2379,7 +2391,7 @@
         <v>1169</v>
       </c>
       <c r="I5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2390,7 +2402,7 @@
         <v>1196</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -2399,7 +2411,7 @@
         <v>1170</v>
       </c>
       <c r="I6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2410,7 +2422,7 @@
         <v>1197</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -2419,7 +2431,7 @@
         <v>1171</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2430,7 +2442,7 @@
         <v>1198</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -2439,7 +2451,7 @@
         <v>1172</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2450,7 +2462,7 @@
         <v>1199</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -2459,7 +2471,7 @@
         <v>1173</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2470,7 +2482,7 @@
         <v>1200</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -2479,7 +2491,7 @@
         <v>1174</v>
       </c>
       <c r="I10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2506,367 +2518,367 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2878,7 +2890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2886,32 +2898,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -2934,32 +2946,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2996,7 +3008,7 @@
   <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3042,7 +3054,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -3087,52 +3099,52 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3191,12 +3203,12 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3240,57 +3252,57 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3342,7 +3354,7 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3350,10 +3362,10 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" t="s">
         <v>275</v>
-      </c>
-      <c r="C4" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3361,10 +3373,10 @@
         <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3372,10 +3384,10 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -3426,7 +3438,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3464,7 +3476,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="15"/>
@@ -3489,7 +3501,7 @@
         <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3509,10 +3521,10 @@
         <v>249</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3532,10 +3544,10 @@
         <v>251</v>
       </c>
       <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
         <v>110</v>
-      </c>
-      <c r="H4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3557,13 +3569,13 @@
         <v>407</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3571,13 +3583,13 @@
         <v>408</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3607,7 +3619,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
@@ -3616,7 +3628,7 @@
         <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I1" t="s">
         <v>35</v>
@@ -3630,19 +3642,19 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H2">
         <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3650,16 +3662,16 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H3">
         <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3667,7 +3679,7 @@
         <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized most of cavetown inn
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2954086A-1112-4F87-B6B2-B45A665A7D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDE587F-62C0-45BD-9FCD-25ACECFEC9D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="305">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -960,6 +960,15 @@
   </si>
   <si>
     <t>Anti-Kater Mittel / Anti Hangover Drink</t>
+  </si>
+  <si>
+    <t>Ruben</t>
+  </si>
+  <si>
+    <t>Cavetown Inn (375)</t>
+  </si>
+  <si>
+    <t>Administrator of cavetown</t>
   </si>
 </sst>
 </file>
@@ -1792,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,6 +1889,20 @@
       </c>
       <c r="D6" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D7" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3572,7 +3595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added several keys, NPC Ruben and office door
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDE587F-62C0-45BD-9FCD-25ACECFEC9D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4515F88F-0E17-41D6-8D58-2F84B53CF946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,17 @@
     <sheet name="MapChanges" sheetId="9" r:id="rId11"/>
     <sheet name="NPCs" sheetId="10" r:id="rId12"/>
     <sheet name="Chests" sheetId="11" r:id="rId13"/>
-    <sheet name="TextChanges" sheetId="13" r:id="rId14"/>
-    <sheet name="TileChangeEvents" sheetId="14" r:id="rId15"/>
-    <sheet name="CharChanges" sheetId="16" r:id="rId16"/>
-    <sheet name="New Object Graphics" sheetId="21" r:id="rId17"/>
-    <sheet name="Tiles" sheetId="15" r:id="rId18"/>
-    <sheet name="SpellChanges" sheetId="17" r:id="rId19"/>
-    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId20"/>
-    <sheet name="Tabelle3" sheetId="19" r:id="rId21"/>
-    <sheet name="Tabelle2" sheetId="22" r:id="rId22"/>
-    <sheet name="Tabelle1" sheetId="23" r:id="rId23"/>
+    <sheet name="Doors" sheetId="24" r:id="rId14"/>
+    <sheet name="TextChanges" sheetId="13" r:id="rId15"/>
+    <sheet name="TileChangeEvents" sheetId="14" r:id="rId16"/>
+    <sheet name="CharChanges" sheetId="16" r:id="rId17"/>
+    <sheet name="New Object Graphics" sheetId="21" r:id="rId18"/>
+    <sheet name="Tiles" sheetId="15" r:id="rId19"/>
+    <sheet name="SpellChanges" sheetId="17" r:id="rId20"/>
+    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId21"/>
+    <sheet name="Tabelle3" sheetId="19" r:id="rId22"/>
+    <sheet name="Tabelle2" sheetId="22" r:id="rId23"/>
+    <sheet name="Tabelle1" sheetId="23" r:id="rId24"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="321">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -969,6 +970,54 @@
   </si>
   <si>
     <t>Administrator of cavetown</t>
+  </si>
+  <si>
+    <t>123: SCHLOSS / CASTLE</t>
+  </si>
+  <si>
+    <t>122: VIELAUGE / MANYEYES</t>
+  </si>
+  <si>
+    <t>245: Talked to Ruben once (got the office key)</t>
+  </si>
+  <si>
+    <t>124: BÜRO / OFFICE</t>
+  </si>
+  <si>
+    <t>Büroschlüssel / Office Key</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Opens the door to the cavetown office (Ruben gives it to you)</t>
+  </si>
+  <si>
+    <t>246: Door to Manyeyes' castle unlocked</t>
+  </si>
+  <si>
+    <t>Opens the first door in the gatekeeper house</t>
+  </si>
+  <si>
+    <t>Opens the second door in the gatekeeper house</t>
+  </si>
+  <si>
+    <t>Pförtnerschlüssel 1 / Gate Keeper's Key 1</t>
+  </si>
+  <si>
+    <t>Pförtnerschlüssel 2 / Gate Keeper's Key 2</t>
+  </si>
+  <si>
+    <t>DoorIndex</t>
+  </si>
+  <si>
+    <t>Door to the cavetown office</t>
+  </si>
+  <si>
+    <t>First gate keeper door</t>
+  </si>
+  <si>
+    <t>Second gate keeper door</t>
   </si>
 </sst>
 </file>
@@ -1803,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,6 +2138,56 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62C0FBA-1BDC-4EAA-90A2-D38035F594DC}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A23AD0D-3B64-4BEF-82E1-7DFFB5EA7471}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2123,7 +2222,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAC578B-0798-484E-AD11-E9A5E47BA266}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2143,7 +2242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -2283,7 +2382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFAD946-A9D1-4502-A6CF-B93E446D51BE}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2388,7 +2487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42293419-9ED8-4D74-9E3B-F691567047C5}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -2599,389 +2698,6 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
-  <dimension ref="A1:A75"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>205</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3032,6 +2748,389 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
+  <dimension ref="A1:A75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A938DC3D-143F-4871-88FF-86347B3EB68B}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -3079,7 +3178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBBD23D-83D2-4AFD-8FE1-B7316E06FB79}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3091,7 +3190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303F205F-3A3D-43F3-9B99-BFC12608D1EA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3103,7 +3202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18E140D-3A01-46A3-8908-6D1ECD214288}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3117,10 +3216,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3259,6 +3358,16 @@
         <v>251</v>
       </c>
     </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3266,10 +3375,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC73B1D-C705-4EA8-84D8-EC14D78F4581}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3321,6 +3430,21 @@
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3593,10 +3717,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,6 +3901,48 @@
       </c>
       <c r="D10" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>412</v>
+      </c>
+      <c r="B11" t="s">
+        <v>309</v>
+      </c>
+      <c r="C11" t="s">
+        <v>310</v>
+      </c>
+      <c r="D11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>413</v>
+      </c>
+      <c r="B12" t="s">
+        <v>315</v>
+      </c>
+      <c r="C12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D12" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>414</v>
+      </c>
+      <c r="B13" t="s">
+        <v>316</v>
+      </c>
+      <c r="C13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D13" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed Ruben to Tristan
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219A6DB9-A3E0-41FF-B2FC-738E04CF1826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCD26FE-5CC2-40C0-A181-ADE3AE497955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -960,9 +960,6 @@
     <t>Anti-Kater Mittel / Anti Hangover Drink</t>
   </si>
   <si>
-    <t>Ruben</t>
-  </si>
-  <si>
     <t>Cavetown Inn (375)</t>
   </si>
   <si>
@@ -975,9 +972,6 @@
     <t>122: VIELAUGE / MANYEYES</t>
   </si>
   <si>
-    <t>245: Talked to Ruben once (got the office key)</t>
-  </si>
-  <si>
     <t>124: BÜRO / OFFICE</t>
   </si>
   <si>
@@ -1033,6 +1027,12 @@
   </si>
   <si>
     <t>Add normal beds to tileset 8 and use them instead of the dwarf beds</t>
+  </si>
+  <si>
+    <t>245: Talked to Tristan once (got the office key)</t>
+  </si>
+  <si>
+    <t>Tristan</t>
   </si>
 </sst>
 </file>
@@ -1867,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,13 +1960,13 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" t="s">
         <v>301</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>302</v>
-      </c>
-      <c r="D7" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2149,10 +2149,10 @@
         <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C13" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2160,10 +2160,10 @@
         <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2171,10 +2171,10 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2200,7 +2200,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -2211,7 +2211,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2219,7 +2219,7 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2754,7 +2754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2772,12 +2772,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -3272,7 +3272,7 @@
   <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,12 +3413,12 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -3487,17 +3487,17 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -3961,13 +3961,13 @@
         <v>412</v>
       </c>
       <c r="B11" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" t="s">
+        <v>307</v>
+      </c>
+      <c r="D11" t="s">
         <v>308</v>
-      </c>
-      <c r="C11" t="s">
-        <v>309</v>
-      </c>
-      <c r="D11" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3975,13 +3975,13 @@
         <v>413</v>
       </c>
       <c r="B12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3989,13 +3989,13 @@
         <v>414</v>
       </c>
       <c r="B13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added prototype of manyeyes' castle
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCD26FE-5CC2-40C0-A181-ADE3AE497955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DC46B3-4425-40BA-8F3F-DBB935EB5E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="328">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>230: You have bought a cat from Ferdinand</t>
-  </si>
-  <si>
-    <t>229: You have created a wind chain</t>
   </si>
   <si>
     <t>231: You have bought a dog from Ferdinand</t>
@@ -1033,6 +1030,15 @@
   </si>
   <si>
     <t>Tristan</t>
+  </si>
+  <si>
+    <t>Vielauge's Schloss - 0 / Manyeyes' Castle - 0</t>
+  </si>
+  <si>
+    <t>Ground floor of Manyeyes' castle including the office</t>
+  </si>
+  <si>
+    <t>229: You have talked to Karl about his former trainee</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1510,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1514,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD8B38F-295E-46BA-A316-56C9E4745E5F}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,16 +1535,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1546,13 +1552,13 @@
         <v>456</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1560,13 +1566,13 @@
         <v>457</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1574,13 +1580,13 @@
         <v>458</v>
       </c>
       <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,13 +1594,13 @@
         <v>459</v>
       </c>
       <c r="B5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" t="s">
         <v>215</v>
       </c>
-      <c r="C5" t="s">
-        <v>216</v>
-      </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1602,13 +1608,13 @@
         <v>460</v>
       </c>
       <c r="B6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" t="s">
         <v>217</v>
-      </c>
-      <c r="C6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D6" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1616,13 +1622,13 @@
         <v>370</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,13 +1636,13 @@
         <v>371</v>
       </c>
       <c r="B8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
         <v>220</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,13 +1650,13 @@
         <v>372</v>
       </c>
       <c r="B9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" t="s">
         <v>224</v>
-      </c>
-      <c r="C9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D9" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1658,13 +1664,13 @@
         <v>373</v>
       </c>
       <c r="B10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
         <v>241</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1672,13 +1678,13 @@
         <v>374</v>
       </c>
       <c r="B11" t="s">
+        <v>284</v>
+      </c>
+      <c r="C11" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" t="s">
         <v>285</v>
-      </c>
-      <c r="C11" t="s">
-        <v>216</v>
-      </c>
-      <c r="D11" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1686,13 +1692,27 @@
         <v>375</v>
       </c>
       <c r="B12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
         <v>287</v>
       </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>288</v>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>461</v>
+      </c>
+      <c r="B13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C13" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -1716,13 +1736,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1730,10 +1750,10 @@
         <v>157</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1741,10 +1761,10 @@
         <v>198</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1752,10 +1772,10 @@
         <v>258</v>
       </c>
       <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
         <v>92</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1763,10 +1783,10 @@
         <v>259</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1774,10 +1794,10 @@
         <v>262</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1785,10 +1805,10 @@
         <v>263</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1796,10 +1816,10 @@
         <v>273</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1807,10 +1827,10 @@
         <v>420</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1818,10 +1838,10 @@
         <v>421</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1867,7 +1887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1879,16 +1899,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,13 +1916,13 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
         <v>62</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1910,13 +1930,13 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,10 +1944,10 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1935,10 +1955,10 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,13 +1966,13 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
         <v>72</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1960,13 +1980,13 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D7" t="s">
         <v>301</v>
-      </c>
-      <c r="D7" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -1992,16 +2012,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -2010,19 +2030,19 @@
         <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2030,19 +2050,19 @@
         <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3">
         <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" t="s">
         <v>101</v>
-      </c>
-      <c r="G3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2050,10 +2070,10 @@
         <v>134</v>
       </c>
       <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
         <v>78</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2061,10 +2081,10 @@
         <v>135</v>
       </c>
       <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
         <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2072,10 +2092,10 @@
         <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2083,10 +2103,10 @@
         <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2094,10 +2114,10 @@
         <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2105,10 +2125,10 @@
         <v>139</v>
       </c>
       <c r="B9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" t="s">
         <v>244</v>
-      </c>
-      <c r="C9" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2116,10 +2136,10 @@
         <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,10 +2147,10 @@
         <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2138,10 +2158,10 @@
         <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2149,10 +2169,10 @@
         <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2160,10 +2180,10 @@
         <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2171,10 +2191,10 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2200,10 +2220,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2211,7 +2231,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2219,7 +2239,7 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2227,7 +2247,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -2250,18 +2270,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
-      </c>
-      <c r="B2" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2282,7 +2302,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2306,122 +2326,122 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
         <v>117</v>
-      </c>
-      <c r="B2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
         <v>120</v>
-      </c>
-      <c r="B4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" t="s">
         <v>123</v>
-      </c>
-      <c r="B8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
         <v>127</v>
-      </c>
-      <c r="B11" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" t="s">
         <v>130</v>
-      </c>
-      <c r="B14" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2446,19 +2466,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>230</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2466,16 +2486,16 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2483,16 +2503,16 @@
         <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2500,16 +2520,16 @@
         <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2517,16 +2537,16 @@
         <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2551,34 +2571,34 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="15"/>
       <c r="G1" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2589,7 +2609,7 @@
         <v>1193</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -2598,7 +2618,7 @@
         <v>1167</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2609,7 +2629,7 @@
         <v>1194</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -2618,7 +2638,7 @@
         <v>1168</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2629,7 +2649,7 @@
         <v>1195</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2638,7 +2658,7 @@
         <v>1169</v>
       </c>
       <c r="I5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2649,7 +2669,7 @@
         <v>1196</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -2658,7 +2678,7 @@
         <v>1170</v>
       </c>
       <c r="I6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2669,7 +2689,7 @@
         <v>1197</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -2678,7 +2698,7 @@
         <v>1171</v>
       </c>
       <c r="I7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2689,7 +2709,7 @@
         <v>1198</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -2698,7 +2718,7 @@
         <v>1172</v>
       </c>
       <c r="I8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2709,7 +2729,7 @@
         <v>1199</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -2718,7 +2738,7 @@
         <v>1173</v>
       </c>
       <c r="I9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2729,7 +2749,7 @@
         <v>1200</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -2738,7 +2758,7 @@
         <v>1174</v>
       </c>
       <c r="I10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2762,37 +2782,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2815,367 +2835,367 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3198,32 +3218,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3271,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,7 +3338,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -3333,7 +3353,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3343,82 +3363,82 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3441,63 +3461,63 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3520,78 +3540,78 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -3615,13 +3635,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3629,10 +3649,10 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3640,10 +3660,10 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3651,10 +3671,10 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3662,10 +3682,10 @@
         <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3673,10 +3693,10 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3684,10 +3704,10 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7" t="s">
         <v>289</v>
-      </c>
-      <c r="C7" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3695,10 +3715,10 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3706,10 +3726,10 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C9" t="s">
         <v>291</v>
-      </c>
-      <c r="C9" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3732,13 +3752,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3749,7 +3769,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3760,7 +3780,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3786,19 +3806,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="15"/>
@@ -3808,22 +3828,22 @@
         <v>403</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3831,22 +3851,22 @@
         <v>404</v>
       </c>
       <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3">
         <v>249</v>
       </c>
       <c r="G3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" t="s">
         <v>108</v>
-      </c>
-      <c r="H3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3854,22 +3874,22 @@
         <v>405</v>
       </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
         <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
       </c>
       <c r="F4">
         <v>251</v>
       </c>
       <c r="G4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3877,13 +3897,13 @@
         <v>406</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3891,13 +3911,13 @@
         <v>407</v>
       </c>
       <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>85</v>
-      </c>
-      <c r="D6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3905,13 +3925,13 @@
         <v>408</v>
       </c>
       <c r="B7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>209</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3919,13 +3939,13 @@
         <v>409</v>
       </c>
       <c r="B8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C8" t="s">
         <v>294</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>295</v>
-      </c>
-      <c r="D8" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3933,13 +3953,13 @@
         <v>410</v>
       </c>
       <c r="B9" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
         <v>297</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3947,13 +3967,13 @@
         <v>411</v>
       </c>
       <c r="B10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3961,13 +3981,13 @@
         <v>412</v>
       </c>
       <c r="B11" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" t="s">
         <v>306</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>307</v>
-      </c>
-      <c r="D11" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3975,13 +3995,13 @@
         <v>413</v>
       </c>
       <c r="B12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3989,13 +4009,13 @@
         <v>414</v>
       </c>
       <c r="B13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -4025,22 +4045,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -4048,19 +4068,19 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2">
         <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4068,16 +4088,16 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" t="s">
         <v>237</v>
-      </c>
-      <c r="C3" t="s">
-        <v>238</v>
       </c>
       <c r="H3">
         <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -4085,7 +4105,7 @@
         <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished manyeyes' castle level 1
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DC46B3-4425-40BA-8F3F-DBB935EB5E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879EDD5F-796A-43BA-8648-98DD30BB53DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="334">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1039,6 +1039,24 @@
   </si>
   <si>
     <t>229: You have talked to Karl about his former trainee</t>
+  </si>
+  <si>
+    <t>Monster in Manyeyes' castle</t>
+  </si>
+  <si>
+    <t>Untoter Krieger</t>
+  </si>
+  <si>
+    <t>Untoter Magier</t>
+  </si>
+  <si>
+    <t>2x Untoter Krieger, 1x Untoter Magier</t>
+  </si>
+  <si>
+    <t>2x Untoter Krieger</t>
+  </si>
+  <si>
+    <t>3x Untoter Krieger, 2x Untoter Magier</t>
   </si>
 </sst>
 </file>
@@ -3291,8 +3309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4028,17 +4046,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="22.42578125" customWidth="1"/>
   </cols>
@@ -4101,11 +4119,53 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" t="s">
+        <v>328</v>
+      </c>
       <c r="H4">
         <v>89</v>
       </c>
       <c r="I4" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C5" t="s">
+        <v>328</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
+      <c r="I5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>91</v>
+      </c>
+      <c r="I6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized manyeyes' castle level 1
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879EDD5F-796A-43BA-8648-98DD30BB53DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720695F-4E90-4096-B9AC-63217568360C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="341">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1008,9 +1008,6 @@
     <t>Second gate keeper door</t>
   </si>
   <si>
-    <t>1x Stamina Potion, 3x Bitter</t>
-  </si>
-  <si>
     <t>1x Shovel, 2x Rope</t>
   </si>
   <si>
@@ -1057,6 +1054,30 @@
   </si>
   <si>
     <t>3x Untoter Krieger, 2x Untoter Magier</t>
+  </si>
+  <si>
+    <t>Manyeyes'c castle 1 (461)</t>
+  </si>
+  <si>
+    <t>1x Dark Dagger</t>
+  </si>
+  <si>
+    <t>1x Holy Horn, 1x Horned Helmet, 1x Scimitar, 800 Gold</t>
+  </si>
+  <si>
+    <t>1x Silver Cutlery, 3 Healing Potion III, 2 Spell Potion IV, 1 Healing Potion IV, 250 Gold</t>
+  </si>
+  <si>
+    <t>1x Stamina Potion, 3x Bitter, 5x Food</t>
+  </si>
+  <si>
+    <t>Dunkle Klinge / Dark Blade</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Cursed weapon from manyeyes' castle</t>
   </si>
 </sst>
 </file>
@@ -1724,13 +1745,13 @@
         <v>461</v>
       </c>
       <c r="B13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C13" t="s">
         <v>215</v>
       </c>
       <c r="D13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -1998,7 +2019,7 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C7" t="s">
         <v>300</v>
@@ -2014,10 +2035,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,10 +2208,10 @@
         <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C13" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2198,10 +2219,10 @@
         <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2209,10 +2230,43 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C15" t="s">
-        <v>319</v>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>146</v>
+      </c>
+      <c r="B16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C16" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>147</v>
+      </c>
+      <c r="B17" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>148</v>
+      </c>
+      <c r="B18" t="s">
+        <v>333</v>
+      </c>
+      <c r="C18" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -2810,12 +2864,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -3310,7 +3364,7 @@
   <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3371,7 +3425,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3451,7 +3505,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -3808,10 +3862,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4036,6 +4090,20 @@
         <v>310</v>
       </c>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>415</v>
+      </c>
+      <c r="B14" t="s">
+        <v>338</v>
+      </c>
+      <c r="C14" t="s">
+        <v>339</v>
+      </c>
+      <c r="D14" t="s">
+        <v>340</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:H1"/>
@@ -4048,7 +4116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -4123,10 +4191,10 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H4">
         <v>89</v>
@@ -4140,16 +4208,16 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H5">
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4157,7 +4225,7 @@
         <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4165,7 +4233,7 @@
         <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ancient key and chests for manyeyes' castle 2
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720695F-4E90-4096-B9AC-63217568360C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39CAF63-A7EA-4C86-B799-A4BFADF2740F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="347">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -888,9 +888,6 @@
     <t>350 Gold per raft, spawns east of Cavetown at the beach</t>
   </si>
   <si>
-    <t>Create manyeyes castle</t>
-  </si>
-  <si>
     <t>Finish cavetown</t>
   </si>
   <si>
@@ -1017,9 +1014,6 @@
     <t>Gatekeeper's house (376)</t>
   </si>
   <si>
-    <t>Add gatekeeper chests (to savegame)</t>
-  </si>
-  <si>
     <t>Add normal beds to tileset 8 and use them instead of the dwarf beds</t>
   </si>
   <si>
@@ -1077,7 +1071,31 @@
     <t>Weapon</t>
   </si>
   <si>
-    <t>Cursed weapon from manyeyes' castle</t>
+    <t>Add gatekeeper chests</t>
+  </si>
+  <si>
+    <t>Finish manyeyes castle</t>
+  </si>
+  <si>
+    <t>Alter Schlüssel / Ancient Key</t>
+  </si>
+  <si>
+    <t>Opens the boss room in manyeyes' castle 2</t>
+  </si>
+  <si>
+    <t>Cursed weapon from manyeyes' castle 1</t>
+  </si>
+  <si>
+    <t>Manyeyes'c castle 2 (462)</t>
+  </si>
+  <si>
+    <t>1x Ancient Key</t>
+  </si>
+  <si>
+    <t>2x Healing Potion II, 2x Spell Potion III, 4x Antidot</t>
+  </si>
+  <si>
+    <t>10x Healing Potion I, 5x Spell Potion I, 1x Firebrand, 150 Gold</t>
   </si>
 </sst>
 </file>
@@ -1717,13 +1735,13 @@
         <v>374</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C11" t="s">
         <v>215</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1731,13 +1749,13 @@
         <v>375</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,13 +1763,13 @@
         <v>461</v>
       </c>
       <c r="B13" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C13" t="s">
         <v>215</v>
       </c>
       <c r="D13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -1866,10 +1884,10 @@
         <v>420</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1877,10 +1895,10 @@
         <v>421</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2019,13 +2037,13 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" t="s">
         <v>300</v>
-      </c>
-      <c r="D7" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2035,10 +2053,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,10 +2226,10 @@
         <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C13" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2219,10 +2237,10 @@
         <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2230,10 +2248,10 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2241,10 +2259,10 @@
         <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2252,10 +2270,10 @@
         <v>147</v>
       </c>
       <c r="B17" t="s">
+        <v>331</v>
+      </c>
+      <c r="C17" t="s">
         <v>333</v>
-      </c>
-      <c r="C17" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2263,10 +2281,43 @@
         <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C18" t="s">
-        <v>336</v>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>149</v>
+      </c>
+      <c r="B19" t="s">
+        <v>343</v>
+      </c>
+      <c r="C19" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>150</v>
+      </c>
+      <c r="B20" t="s">
+        <v>343</v>
+      </c>
+      <c r="C20" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>151</v>
+      </c>
+      <c r="B21" t="s">
+        <v>343</v>
+      </c>
+      <c r="C21" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2343,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -2303,7 +2354,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2311,7 +2362,7 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2319,7 +2370,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -2847,7 +2898,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,17 +2915,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>320</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -2884,7 +2935,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3410,7 +3461,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -3425,7 +3476,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3505,12 +3556,12 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3579,17 +3630,17 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -3776,10 +3827,10 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C7" t="s">
         <v>288</v>
-      </c>
-      <c r="C7" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3790,7 +3841,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3798,10 +3849,10 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" t="s">
         <v>290</v>
-      </c>
-      <c r="C9" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -3862,10 +3913,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4011,13 +4062,13 @@
         <v>409</v>
       </c>
       <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" t="s">
         <v>293</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>294</v>
-      </c>
-      <c r="D8" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4025,13 +4076,13 @@
         <v>410</v>
       </c>
       <c r="B9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4039,13 +4090,13 @@
         <v>411</v>
       </c>
       <c r="B10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4053,13 +4104,13 @@
         <v>412</v>
       </c>
       <c r="B11" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" t="s">
         <v>305</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>306</v>
-      </c>
-      <c r="D11" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4067,13 +4118,13 @@
         <v>413</v>
       </c>
       <c r="B12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4081,13 +4132,13 @@
         <v>414</v>
       </c>
       <c r="B13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4095,13 +4146,27 @@
         <v>415</v>
       </c>
       <c r="B14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D14" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>416</v>
+      </c>
+      <c r="B15" t="s">
         <v>340</v>
+      </c>
+      <c r="C15" t="s">
+        <v>305</v>
+      </c>
+      <c r="D15" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -4191,10 +4256,10 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H4">
         <v>89</v>
@@ -4208,16 +4273,16 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H5">
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4225,7 +4290,7 @@
         <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4233,7 +4298,7 @@
         <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added teleport, chests and door to manyeyes' castle 2
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39CAF63-A7EA-4C86-B799-A4BFADF2740F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6A6592-EDAE-42E9-990A-CDBA92B9A528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="349">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1096,6 +1096,12 @@
   </si>
   <si>
     <t>10x Healing Potion I, 5x Spell Potion I, 1x Firebrand, 150 Gold</t>
+  </si>
+  <si>
+    <t>Manyeyes' upper boos door</t>
+  </si>
+  <si>
+    <t>Ladder teleport event to manyeyes' castle 2</t>
   </si>
 </sst>
 </file>
@@ -2055,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,10 +2336,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62C0FBA-1BDC-4EAA-90A2-D38035F594DC}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,6 +2377,14 @@
       </c>
       <c r="B4" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2895,10 +2909,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,6 +2950,11 @@
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mostly finished manyeyes' cellar
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6A6592-EDAE-42E9-990A-CDBA92B9A528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8005D0AD-A6E3-4A3C-AE55-5E2FC57C352C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <sheet name="Tiles" sheetId="15" r:id="rId19"/>
     <sheet name="SpellChanges" sheetId="17" r:id="rId20"/>
     <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId21"/>
-    <sheet name="Tabelle3" sheetId="19" r:id="rId22"/>
-    <sheet name="Tabelle2" sheetId="22" r:id="rId23"/>
-    <sheet name="Tabelle1" sheetId="23" r:id="rId24"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="366">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1101,7 +1098,58 @@
     <t>Manyeyes' upper boos door</t>
   </si>
   <si>
-    <t>Ladder teleport event to manyeyes' castle 2</t>
+    <t>Fix 462 event icons (after opening the door, it is a closed chest …)</t>
+  </si>
+  <si>
+    <t>1x Untoter Lord, 1x Untoter Krieger, 3x Untoter Magier</t>
+  </si>
+  <si>
+    <t>Untoter Lord</t>
+  </si>
+  <si>
+    <t>Boss in Manyeyes' castle</t>
+  </si>
+  <si>
+    <t>247: Upper boss in Manyeyes' castle killed</t>
+  </si>
+  <si>
+    <t>2Object3D.amb</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Undead (that works with sky, pal4)</t>
+  </si>
+  <si>
+    <t>Manyeyes' castle 2</t>
+  </si>
+  <si>
+    <t>Also added two overlays 92 and 93 for the door in Manyeyes' castle 2</t>
+  </si>
+  <si>
+    <t>Change small lizard sprite to not include the sky color!</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Reward from first manyeyes' castle boss</t>
+  </si>
+  <si>
+    <t>Schwert der Ahnen / Ancestral Sword</t>
+  </si>
+  <si>
+    <t>Rüstung der Ahnen / Ancestral Armour</t>
+  </si>
+  <si>
+    <t>Manyeyes'c cellar (463)</t>
+  </si>
+  <si>
+    <t>1x Strength Potion, 1x Intelligence Potion, 2x Antidot, 5x Healing Potion IV, 3x Spell Potion III</t>
+  </si>
+  <si>
+    <t>100 Gold, 6 Rationen</t>
   </si>
 </sst>
 </file>
@@ -2059,10 +2107,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,6 +2372,28 @@
       </c>
       <c r="C21" t="s">
         <v>346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
+        <v>363</v>
+      </c>
+      <c r="C22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>153</v>
+      </c>
+      <c r="B23" t="s">
+        <v>363</v>
+      </c>
+      <c r="C23" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -2589,19 +2659,20 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFAD946-A9D1-4502-A6CF-B93E446D51BE}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>226</v>
       </c>
@@ -2617,8 +2688,11 @@
       <c r="E1" s="12" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>39</v>
       </c>
@@ -2635,7 +2709,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>153</v>
       </c>
@@ -2652,7 +2726,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>86</v>
       </c>
@@ -2669,7 +2743,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>154</v>
       </c>
@@ -2684,6 +2758,23 @@
       </c>
       <c r="E5" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>374</v>
+      </c>
+      <c r="B6" t="s">
+        <v>355</v>
+      </c>
+      <c r="C6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" t="s">
+        <v>353</v>
+      </c>
+      <c r="E6" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -2909,10 +3000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2955,6 +3046,11 @@
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -3393,48 +3489,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBBD23D-83D2-4AFD-8FE1-B7316E06FB79}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303F205F-3A3D-43F3-9B99-BFC12608D1EA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18E140D-3A01-46A3-8908-6D1ECD214288}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3581,6 +3641,11 @@
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3932,10 +3997,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4188,6 +4253,34 @@
         <v>341</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>417</v>
+      </c>
+      <c r="B16" t="s">
+        <v>361</v>
+      </c>
+      <c r="C16" t="s">
+        <v>337</v>
+      </c>
+      <c r="D16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>418</v>
+      </c>
+      <c r="B17" t="s">
+        <v>362</v>
+      </c>
+      <c r="C17" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:H1"/>
@@ -4198,10 +4291,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4305,6 +4398,15 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>351</v>
+      </c>
       <c r="H6">
         <v>91</v>
       </c>
@@ -4318,6 +4420,14 @@
       </c>
       <c r="I7" t="s">
         <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing automaps, fixed some spell elements
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13ACB6F5-4367-43DC-BE42-318B06F0B397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F59CE63-221D-4F4A-A756-9EE7FBA6417F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="376">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1020,9 +1020,6 @@
     <t>Tristan</t>
   </si>
   <si>
-    <t>Vielauge's Schloss - 0 / Manyeyes' Castle - 0</t>
-  </si>
-  <si>
     <t>Ground floor of Manyeyes' castle including the office</t>
   </si>
   <si>
@@ -1165,13 +1162,31 @@
   </si>
   <si>
     <t>3x Einauge (Typ 1), 2x Einauge (Typ 2)</t>
+  </si>
+  <si>
+    <t>Vielauge's Schloss 1 / Manyeyes' Castle 1</t>
+  </si>
+  <si>
+    <t>Vielauge's Schloss 2 / Manyeyes' Castle 2</t>
+  </si>
+  <si>
+    <t>Vielauge's Keller / Manyeyes' Cellar</t>
+  </si>
+  <si>
+    <t>Cellar of Manyeyes' castle</t>
+  </si>
+  <si>
+    <t>Upper floor of Manyeyes' castle</t>
+  </si>
+  <si>
+    <t>Manyeyes' cellar, the disappearing wall in the upper left should add 2 torches left and right as the walls are bright</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1183,6 +1198,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1646,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD8B38F-295E-46BA-A316-56C9E4745E5F}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,16 +1853,45 @@
         <v>461</v>
       </c>
       <c r="B13" t="s">
-        <v>322</v>
+        <v>370</v>
       </c>
       <c r="C13" t="s">
         <v>215</v>
       </c>
       <c r="D13" t="s">
-        <v>323</v>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>462</v>
+      </c>
+      <c r="B14" t="s">
+        <v>371</v>
+      </c>
+      <c r="C14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>463</v>
+      </c>
+      <c r="B15" t="s">
+        <v>372</v>
+      </c>
+      <c r="C15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2298,7 +2348,7 @@
         <v>318</v>
       </c>
       <c r="C13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2328,10 +2378,10 @@
         <v>146</v>
       </c>
       <c r="B16" t="s">
+        <v>331</v>
+      </c>
+      <c r="C16" t="s">
         <v>332</v>
-      </c>
-      <c r="C16" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2339,10 +2389,10 @@
         <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2350,10 +2400,10 @@
         <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2361,10 +2411,10 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
+        <v>343</v>
+      </c>
+      <c r="C19" t="s">
         <v>344</v>
-      </c>
-      <c r="C19" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2372,10 +2422,10 @@
         <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2383,10 +2433,10 @@
         <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2394,10 +2444,10 @@
         <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2405,10 +2455,10 @@
         <v>153</v>
       </c>
       <c r="B23" t="s">
+        <v>363</v>
+      </c>
+      <c r="C23" t="s">
         <v>364</v>
-      </c>
-      <c r="C23" t="s">
-        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -2469,7 +2519,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2704,7 +2754,7 @@
         <v>231</v>
       </c>
       <c r="I1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2780,16 +2830,16 @@
         <v>374</v>
       </c>
       <c r="B6" t="s">
+        <v>355</v>
+      </c>
+      <c r="C6" t="s">
         <v>356</v>
       </c>
-      <c r="C6" t="s">
-        <v>357</v>
-      </c>
       <c r="D6" t="s">
+        <v>353</v>
+      </c>
+      <c r="E6" t="s">
         <v>354</v>
-      </c>
-      <c r="E6" t="s">
-        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -3015,10 +3065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3035,7 +3085,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -3045,7 +3095,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -3060,12 +3110,17 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>359</v>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3570,7 +3625,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3660,7 +3715,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4245,13 +4300,13 @@
         <v>415</v>
       </c>
       <c r="B14" t="s">
+        <v>336</v>
+      </c>
+      <c r="C14" t="s">
         <v>337</v>
       </c>
-      <c r="C14" t="s">
-        <v>338</v>
-      </c>
       <c r="D14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4259,13 +4314,13 @@
         <v>416</v>
       </c>
       <c r="B15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C15" t="s">
         <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4273,13 +4328,13 @@
         <v>417</v>
       </c>
       <c r="B16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D16" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4287,13 +4342,13 @@
         <v>418</v>
       </c>
       <c r="B17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C17" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" t="s">
         <v>360</v>
-      </c>
-      <c r="D17" t="s">
-        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -4308,8 +4363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4383,10 +4438,10 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H4">
         <v>89</v>
@@ -4400,16 +4455,16 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H5">
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4417,16 +4472,16 @@
         <v>61</v>
       </c>
       <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
         <v>351</v>
-      </c>
-      <c r="C6" t="s">
-        <v>352</v>
       </c>
       <c r="H6">
         <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4434,16 +4489,16 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H7">
         <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -4451,16 +4506,16 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H8">
         <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -4468,16 +4523,16 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C9" t="s">
         <v>325</v>
-      </c>
-      <c r="C9" t="s">
-        <v>326</v>
       </c>
       <c r="H9">
         <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -4485,7 +4540,7 @@
         <v>95</v>
       </c>
       <c r="I10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -4493,7 +4548,7 @@
         <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added monsters for manyeyes' cellar
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F59CE63-221D-4F4A-A756-9EE7FBA6417F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548FA2DD-84FE-4BDA-A007-EE253B0EA77C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="379">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1180,6 +1180,15 @@
   </si>
   <si>
     <t>Manyeyes' cellar, the disappearing wall in the upper left should add 2 torches left and right as the walls are bright</t>
+  </si>
+  <si>
+    <t>Falling through the upper floor does not work for Amiga. Screen is dark. Better add a second event when you walk to the door after the boss is dead. Adjust positions of the holes/events also in the lower levels!</t>
+  </si>
+  <si>
+    <t>The black man statue is not drawn correctly for Amiga. Maybe gfx is missing?</t>
+  </si>
+  <si>
+    <t>Singleeye: Improve gfx (battle field and sprite) and make them smaller, improve animations, fix spells (bits must be one higher)</t>
   </si>
 </sst>
 </file>
@@ -3065,10 +3074,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3121,6 +3130,21 @@
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added monsters to cellar
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548FA2DD-84FE-4BDA-A007-EE253B0EA77C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8498ABBB-5321-4775-B4D4-24991615B4C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="385">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1189,6 +1189,24 @@
   </si>
   <si>
     <t>Singleeye: Improve gfx (battle field and sprite) and make them smaller, improve animations, fix spells (bits must be one higher)</t>
+  </si>
+  <si>
+    <t>248: Fallen through roof of Manyeyes' castle once</t>
+  </si>
+  <si>
+    <t>249: Manyeyes' curse was banished (wall removed)</t>
+  </si>
+  <si>
+    <t>5x Spell Potion V, 1x Stamina Potion, 1x Ghost Orb, 1x Speed Ring, 1x Zielbrosche</t>
+  </si>
+  <si>
+    <t>Geisterkugel / Ghost Orb</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>In a chest in the secret room in manyeyes' cellar</t>
   </si>
 </sst>
 </file>
@@ -2181,10 +2199,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2468,6 +2486,17 @@
       </c>
       <c r="C23" t="s">
         <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>154</v>
+      </c>
+      <c r="B24" t="s">
+        <v>363</v>
+      </c>
+      <c r="C24" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -3076,7 +3105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -3585,10 +3614,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3740,6 +3769,16 @@
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4091,10 +4130,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4373,6 +4412,20 @@
       </c>
       <c r="D17" t="s">
         <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>419</v>
+      </c>
+      <c r="B18" t="s">
+        <v>382</v>
+      </c>
+      <c r="C18" t="s">
+        <v>383</v>
+      </c>
+      <c r="D18" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished monster single eye
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8498ABBB-5321-4775-B4D4-24991615B4C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE9A6EB-05E0-4FDF-B86B-AB252179E391}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="388">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1071,9 +1071,6 @@
     <t>Add gatekeeper chests</t>
   </si>
   <si>
-    <t>Finish manyeyes castle</t>
-  </si>
-  <si>
     <t>Alter Schlüssel / Ancient Key</t>
   </si>
   <si>
@@ -1179,9 +1176,6 @@
     <t>Upper floor of Manyeyes' castle</t>
   </si>
   <si>
-    <t>Manyeyes' cellar, the disappearing wall in the upper left should add 2 torches left and right as the walls are bright</t>
-  </si>
-  <si>
     <t>Falling through the upper floor does not work for Amiga. Screen is dark. Better add a second event when you walk to the door after the boss is dead. Adjust positions of the holes/events also in the lower levels!</t>
   </si>
   <si>
@@ -1207,13 +1201,28 @@
   </si>
   <si>
     <t>In a chest in the secret room in manyeyes' cellar</t>
+  </si>
+  <si>
+    <t>Reduced food from 39 to 20</t>
+  </si>
+  <si>
+    <t>Replaced shortsword by a dagger</t>
+  </si>
+  <si>
+    <t>Changed Monster</t>
+  </si>
+  <si>
+    <t>Ghul</t>
+  </si>
+  <si>
+    <t>Element changed from None to Undead</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1230,13 +1239,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1253,6 +1269,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1362,10 +1383,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1394,8 +1416,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1880,7 +1906,7 @@
         <v>461</v>
       </c>
       <c r="B13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C13" t="s">
         <v>215</v>
@@ -1894,13 +1920,13 @@
         <v>462</v>
       </c>
       <c r="B14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C14" t="s">
         <v>215</v>
       </c>
       <c r="D14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1908,17 +1934,17 @@
         <v>463</v>
       </c>
       <c r="B15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C15" t="s">
         <v>215</v>
       </c>
       <c r="D15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2202,7 +2228,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,6 +2304,15 @@
       <c r="C4" t="s">
         <v>78</v>
       </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2289,6 +2324,15 @@
       <c r="C5" t="s">
         <v>80</v>
       </c>
+      <c r="E5">
+        <v>124</v>
+      </c>
+      <c r="F5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2438,10 +2482,10 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
+        <v>342</v>
+      </c>
+      <c r="C19" t="s">
         <v>343</v>
-      </c>
-      <c r="C19" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2449,10 +2493,10 @@
         <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2460,10 +2504,10 @@
         <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C21" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2471,10 +2515,10 @@
         <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2482,10 +2526,10 @@
         <v>153</v>
       </c>
       <c r="B23" t="s">
+        <v>362</v>
+      </c>
+      <c r="C23" t="s">
         <v>363</v>
-      </c>
-      <c r="C23" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2493,10 +2537,10 @@
         <v>154</v>
       </c>
       <c r="B24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C24" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2557,7 +2601,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2792,7 +2836,7 @@
         <v>231</v>
       </c>
       <c r="I1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2868,16 +2912,16 @@
         <v>374</v>
       </c>
       <c r="B6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C6" t="s">
         <v>355</v>
       </c>
-      <c r="C6" t="s">
-        <v>356</v>
-      </c>
       <c r="D6" t="s">
+        <v>352</v>
+      </c>
+      <c r="E6" t="s">
         <v>353</v>
-      </c>
-      <c r="E6" t="s">
-        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3106,7 +3150,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,11 +3175,6 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>339</v>
-      </c>
-    </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>258</v>
@@ -3148,32 +3187,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -3768,17 +3802,17 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -4132,7 +4166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -4369,7 +4403,7 @@
         <v>337</v>
       </c>
       <c r="D14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4377,13 +4411,13 @@
         <v>416</v>
       </c>
       <c r="B15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C15" t="s">
         <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4391,13 +4425,13 @@
         <v>417</v>
       </c>
       <c r="B16" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C16" t="s">
         <v>337</v>
       </c>
       <c r="D16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4405,13 +4439,13 @@
         <v>418</v>
       </c>
       <c r="B17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C17" t="s">
+        <v>358</v>
+      </c>
+      <c r="D17" t="s">
         <v>359</v>
-      </c>
-      <c r="D17" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4419,13 +4453,13 @@
         <v>419</v>
       </c>
       <c r="B18" t="s">
+        <v>380</v>
+      </c>
+      <c r="C18" t="s">
+        <v>381</v>
+      </c>
+      <c r="D18" t="s">
         <v>382</v>
-      </c>
-      <c r="C18" t="s">
-        <v>383</v>
-      </c>
-      <c r="D18" t="s">
-        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -4438,10 +4472,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4453,7 +4487,7 @@
     <col min="10" max="10" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -4472,8 +4506,13 @@
       <c r="J1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N1" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>50</v>
       </c>
@@ -4492,8 +4531,17 @@
       <c r="J2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>58</v>
       </c>
@@ -4509,8 +4557,17 @@
       <c r="I3" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>386</v>
+      </c>
+      <c r="P3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>59</v>
       </c>
@@ -4527,7 +4584,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>60</v>
       </c>
@@ -4544,15 +4601,15 @@
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>61</v>
       </c>
       <c r="B6" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" t="s">
         <v>350</v>
-      </c>
-      <c r="C6" t="s">
-        <v>351</v>
       </c>
       <c r="H6">
         <v>91</v>
@@ -4561,15 +4618,15 @@
         <v>328</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H7">
         <v>92</v>
@@ -4578,24 +4635,24 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H8">
         <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>64</v>
       </c>
@@ -4609,26 +4666,29 @@
         <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H10">
         <v>95</v>
       </c>
       <c r="I10" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H11">
         <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N1:P1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished most of manyeyes' castle
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE9A6EB-05E0-4FDF-B86B-AB252179E391}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6BEC9C-654F-424A-B519-A656505FE439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="387">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1176,15 +1176,9 @@
     <t>Upper floor of Manyeyes' castle</t>
   </si>
   <si>
-    <t>Falling through the upper floor does not work for Amiga. Screen is dark. Better add a second event when you walk to the door after the boss is dead. Adjust positions of the holes/events also in the lower levels!</t>
-  </si>
-  <si>
     <t>The black man statue is not drawn correctly for Amiga. Maybe gfx is missing?</t>
   </si>
   <si>
-    <t>Singleeye: Improve gfx (battle field and sprite) and make them smaller, improve animations, fix spells (bits must be one higher)</t>
-  </si>
-  <si>
     <t>248: Fallen through roof of Manyeyes' castle once</t>
   </si>
   <si>
@@ -1216,6 +1210,9 @@
   </si>
   <si>
     <t>Element changed from None to Undead</t>
+  </si>
+  <si>
+    <t>Door in upper manyeyes' level looks wrong (the one with hammer is shown and without the correct overlays)</t>
   </si>
 </sst>
 </file>
@@ -2311,7 +2308,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2331,7 +2328,7 @@
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2540,7 +2537,7 @@
         <v>362</v>
       </c>
       <c r="C24" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -3149,8 +3146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3195,19 +3192,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>374</v>
-      </c>
-    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -3807,12 +3799,12 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -4453,13 +4445,13 @@
         <v>419</v>
       </c>
       <c r="B18" t="s">
+        <v>378</v>
+      </c>
+      <c r="C18" t="s">
+        <v>379</v>
+      </c>
+      <c r="D18" t="s">
         <v>380</v>
-      </c>
-      <c r="C18" t="s">
-        <v>381</v>
-      </c>
-      <c r="D18" t="s">
-        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4474,7 +4466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -4507,7 +4499,7 @@
         <v>32</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
@@ -4561,10 +4553,10 @@
         <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="P3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved small lizard sprite, added normal beds to cavetown houses
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6BEC9C-654F-424A-B519-A656505FE439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726130D4-5327-4D6F-824A-35E09DEC90BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="385">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1011,9 +1011,6 @@
     <t>Gatekeeper's house (376)</t>
   </si>
   <si>
-    <t>Add normal beds to tileset 8 and use them instead of the dwarf beds</t>
-  </si>
-  <si>
     <t>245: Talked to Tristan once (got the office key)</t>
   </si>
   <si>
@@ -1068,9 +1065,6 @@
     <t>Weapon</t>
   </si>
   <si>
-    <t>Add gatekeeper chests</t>
-  </si>
-  <si>
     <t>Alter Schlüssel / Ancient Key</t>
   </si>
   <si>
@@ -1095,9 +1089,6 @@
     <t>Manyeyes' upper boos door</t>
   </si>
   <si>
-    <t>Fix 462 event icons (after opening the door, it is a closed chest …)</t>
-  </si>
-  <si>
     <t>1x Untoter Lord, 1x Untoter Krieger, 3x Untoter Magier</t>
   </si>
   <si>
@@ -1125,9 +1116,6 @@
     <t>Also added two overlays 92 and 93 for the door in Manyeyes' castle 2</t>
   </si>
   <si>
-    <t>Change small lizard sprite to not include the sky color!</t>
-  </si>
-  <si>
     <t>Armor</t>
   </si>
   <si>
@@ -1213,6 +1201,12 @@
   </si>
   <si>
     <t>Door in upper manyeyes' level looks wrong (the one with hammer is shown and without the correct overlays)</t>
+  </si>
+  <si>
+    <t>Pressure plate in gatekeeper house can be activated by eye cursor!</t>
+  </si>
+  <si>
+    <t>Add gatekeeper chests (or fix them)</t>
   </si>
 </sst>
 </file>
@@ -1903,13 +1897,13 @@
         <v>461</v>
       </c>
       <c r="B13" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C13" t="s">
         <v>215</v>
       </c>
       <c r="D13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1917,13 +1911,13 @@
         <v>462</v>
       </c>
       <c r="B14" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C14" t="s">
         <v>215</v>
       </c>
       <c r="D14" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1931,13 +1925,13 @@
         <v>463</v>
       </c>
       <c r="B15" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C15" t="s">
         <v>215</v>
       </c>
       <c r="D15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -2206,7 +2200,7 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C7" t="s">
         <v>299</v>
@@ -2308,7 +2302,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2328,7 +2322,7 @@
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2416,7 +2410,7 @@
         <v>318</v>
       </c>
       <c r="C13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2446,10 +2440,10 @@
         <v>146</v>
       </c>
       <c r="B16" t="s">
+        <v>330</v>
+      </c>
+      <c r="C16" t="s">
         <v>331</v>
-      </c>
-      <c r="C16" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2457,10 +2451,10 @@
         <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2468,10 +2462,10 @@
         <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2479,10 +2473,10 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2490,10 +2484,10 @@
         <v>150</v>
       </c>
       <c r="B20" t="s">
+        <v>340</v>
+      </c>
+      <c r="C20" t="s">
         <v>342</v>
-      </c>
-      <c r="C20" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2501,10 +2495,10 @@
         <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C21" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2512,10 +2506,10 @@
         <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C22" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2523,10 +2517,10 @@
         <v>153</v>
       </c>
       <c r="B23" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C23" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2534,10 +2528,10 @@
         <v>154</v>
       </c>
       <c r="B24" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C24" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -2598,7 +2592,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -2833,7 +2827,7 @@
         <v>231</v>
       </c>
       <c r="I1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2909,16 +2903,16 @@
         <v>374</v>
       </c>
       <c r="B6" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C6" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D6" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E6" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3144,10 +3138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3164,42 +3158,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>338</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>319</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>277</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>347</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3704,7 +3688,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3784,7 +3768,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -3794,17 +3778,17 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -4389,13 +4373,13 @@
         <v>415</v>
       </c>
       <c r="B14" t="s">
+        <v>335</v>
+      </c>
+      <c r="C14" t="s">
         <v>336</v>
       </c>
-      <c r="C14" t="s">
-        <v>337</v>
-      </c>
       <c r="D14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4403,13 +4387,13 @@
         <v>416</v>
       </c>
       <c r="B15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C15" t="s">
         <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4417,13 +4401,13 @@
         <v>417</v>
       </c>
       <c r="B16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D16" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,13 +4415,13 @@
         <v>418</v>
       </c>
       <c r="B17" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C17" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D17" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4445,13 +4429,13 @@
         <v>419</v>
       </c>
       <c r="B18" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C18" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D18" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -4499,7 +4483,7 @@
         <v>32</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
@@ -4553,10 +4537,10 @@
         <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="P3" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4564,10 +4548,10 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H4">
         <v>89</v>
@@ -4581,16 +4565,16 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H5">
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -4598,16 +4582,16 @@
         <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C6" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H6">
         <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -4615,16 +4599,16 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H7">
         <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4632,16 +4616,16 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H8">
         <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -4649,16 +4633,16 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
+        <v>323</v>
+      </c>
+      <c r="C9" t="s">
         <v>324</v>
-      </c>
-      <c r="C9" t="s">
-        <v>325</v>
       </c>
       <c r="H9">
         <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -4666,7 +4650,7 @@
         <v>95</v>
       </c>
       <c r="I10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -4674,7 +4658,7 @@
         <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added NPC for Alex
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726130D4-5327-4D6F-824A-35E09DEC90BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4727CB-ED76-4BF9-92D1-E59CC0E4A9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="388">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -885,9 +885,6 @@
     <t>350 Gold per raft, spawns east of Cavetown at the beach</t>
   </si>
   <si>
-    <t>Finish cavetown</t>
-  </si>
-  <si>
     <t>226: You visited the tavern in Snakesign</t>
   </si>
   <si>
@@ -1207,6 +1204,18 @@
   </si>
   <si>
     <t>Add gatekeeper chests (or fix them)</t>
+  </si>
+  <si>
+    <t>Finish cavetown (add NPCs in town and houses)</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Thalion Office (257)</t>
+  </si>
+  <si>
+    <t>Alex Holland</t>
   </si>
 </sst>
 </file>
@@ -1869,13 +1878,13 @@
         <v>374</v>
       </c>
       <c r="B11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C11" t="s">
         <v>215</v>
       </c>
       <c r="D11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1883,13 +1892,13 @@
         <v>375</v>
       </c>
       <c r="B12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,13 +1906,13 @@
         <v>461</v>
       </c>
       <c r="B13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C13" t="s">
         <v>215</v>
       </c>
       <c r="D13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1911,13 +1920,13 @@
         <v>462</v>
       </c>
       <c r="B14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C14" t="s">
         <v>215</v>
       </c>
       <c r="D14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1925,13 +1934,13 @@
         <v>463</v>
       </c>
       <c r="B15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C15" t="s">
         <v>215</v>
       </c>
       <c r="D15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -2047,10 +2056,10 @@
         <v>420</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2058,10 +2067,10 @@
         <v>421</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2105,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,13 +2209,27 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C7" t="s">
+        <v>298</v>
+      </c>
+      <c r="D7" t="s">
         <v>299</v>
       </c>
-      <c r="D7" t="s">
-        <v>300</v>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>385</v>
+      </c>
+      <c r="C8" t="s">
+        <v>386</v>
+      </c>
+      <c r="D8" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -2302,7 +2325,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2322,7 +2345,7 @@
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2407,10 +2430,10 @@
         <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2418,10 +2441,10 @@
         <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2429,10 +2452,10 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2440,10 +2463,10 @@
         <v>146</v>
       </c>
       <c r="B16" t="s">
+        <v>329</v>
+      </c>
+      <c r="C16" t="s">
         <v>330</v>
-      </c>
-      <c r="C16" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2451,10 +2474,10 @@
         <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2462,10 +2485,10 @@
         <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2473,10 +2496,10 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
+        <v>339</v>
+      </c>
+      <c r="C19" t="s">
         <v>340</v>
-      </c>
-      <c r="C19" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2484,10 +2507,10 @@
         <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2495,10 +2518,10 @@
         <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2506,10 +2529,10 @@
         <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2517,10 +2540,10 @@
         <v>153</v>
       </c>
       <c r="B23" t="s">
+        <v>357</v>
+      </c>
+      <c r="C23" t="s">
         <v>358</v>
-      </c>
-      <c r="C23" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2528,10 +2551,10 @@
         <v>154</v>
       </c>
       <c r="B24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C24" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -2557,7 +2580,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -2568,7 +2591,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2576,7 +2599,7 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2584,7 +2607,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2592,7 +2615,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2827,7 +2850,7 @@
         <v>231</v>
       </c>
       <c r="I1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2903,16 +2926,16 @@
         <v>374</v>
       </c>
       <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
         <v>351</v>
       </c>
-      <c r="C6" t="s">
-        <v>352</v>
-      </c>
       <c r="D6" t="s">
+        <v>348</v>
+      </c>
+      <c r="E6" t="s">
         <v>349</v>
-      </c>
-      <c r="E6" t="s">
-        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3141,7 +3164,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3158,7 +3181,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -3168,22 +3191,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -3673,7 +3696,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -3688,7 +3711,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3768,27 +3791,27 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -3857,17 +3880,17 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -4054,10 +4077,10 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" t="s">
         <v>287</v>
-      </c>
-      <c r="C7" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4068,7 +4091,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4076,10 +4099,10 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" t="s">
         <v>289</v>
-      </c>
-      <c r="C9" t="s">
-        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4289,13 +4312,13 @@
         <v>409</v>
       </c>
       <c r="B8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" t="s">
         <v>292</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>293</v>
-      </c>
-      <c r="D8" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4303,13 +4326,13 @@
         <v>410</v>
       </c>
       <c r="B9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4317,13 +4340,13 @@
         <v>411</v>
       </c>
       <c r="B10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4331,13 +4354,13 @@
         <v>412</v>
       </c>
       <c r="B11" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" t="s">
         <v>304</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>305</v>
-      </c>
-      <c r="D11" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4345,13 +4368,13 @@
         <v>413</v>
       </c>
       <c r="B12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4359,13 +4382,13 @@
         <v>414</v>
       </c>
       <c r="B13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4373,13 +4396,13 @@
         <v>415</v>
       </c>
       <c r="B14" t="s">
+        <v>334</v>
+      </c>
+      <c r="C14" t="s">
         <v>335</v>
       </c>
-      <c r="C14" t="s">
-        <v>336</v>
-      </c>
       <c r="D14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4387,13 +4410,13 @@
         <v>416</v>
       </c>
       <c r="B15" t="s">
+        <v>336</v>
+      </c>
+      <c r="C15" t="s">
+        <v>304</v>
+      </c>
+      <c r="D15" t="s">
         <v>337</v>
-      </c>
-      <c r="C15" t="s">
-        <v>305</v>
-      </c>
-      <c r="D15" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4401,13 +4424,13 @@
         <v>417</v>
       </c>
       <c r="B16" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4415,13 +4438,13 @@
         <v>418</v>
       </c>
       <c r="B17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C17" t="s">
+        <v>353</v>
+      </c>
+      <c r="D17" t="s">
         <v>354</v>
-      </c>
-      <c r="D17" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4429,13 +4452,13 @@
         <v>419</v>
       </c>
       <c r="B18" t="s">
+        <v>373</v>
+      </c>
+      <c r="C18" t="s">
         <v>374</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>375</v>
-      </c>
-      <c r="D18" t="s">
-        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -4483,7 +4506,7 @@
         <v>32</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
@@ -4537,10 +4560,10 @@
         <v>19</v>
       </c>
       <c r="O3" t="s">
+        <v>379</v>
+      </c>
+      <c r="P3" t="s">
         <v>380</v>
-      </c>
-      <c r="P3" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4548,10 +4571,10 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H4">
         <v>89</v>
@@ -4565,16 +4588,16 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H5">
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -4582,16 +4605,16 @@
         <v>61</v>
       </c>
       <c r="B6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C6" t="s">
         <v>346</v>
-      </c>
-      <c r="C6" t="s">
-        <v>347</v>
       </c>
       <c r="H6">
         <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -4599,16 +4622,16 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H7">
         <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4616,16 +4639,16 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H8">
         <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -4633,16 +4656,16 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C9" t="s">
         <v>323</v>
-      </c>
-      <c r="C9" t="s">
-        <v>324</v>
       </c>
       <c r="H9">
         <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -4650,7 +4673,7 @@
         <v>95</v>
       </c>
       <c r="I10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -4658,7 +4681,7 @@
         <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved Tristan text, fixed chests in gatekeeper's house
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4727CB-ED76-4BF9-92D1-E59CC0E4A9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87009E14-FFA9-4636-B52A-A6BA539E7166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="389">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1203,9 +1203,6 @@
     <t>Pressure plate in gatekeeper house can be activated by eye cursor!</t>
   </si>
   <si>
-    <t>Add gatekeeper chests (or fix them)</t>
-  </si>
-  <si>
     <t>Finish cavetown (add NPCs in town and houses)</t>
   </si>
   <si>
@@ -1216,6 +1213,12 @@
   </si>
   <si>
     <t>Alex Holland</t>
+  </si>
+  <si>
+    <t>Pförtnerhaus / Gatekeeper's House</t>
+  </si>
+  <si>
+    <t>3 houses in cavetown</t>
   </si>
 </sst>
 </file>
@@ -1720,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD8B38F-295E-46BA-A316-56C9E4745E5F}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,43 +1906,57 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>461</v>
+        <v>376</v>
       </c>
       <c r="B13" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
       <c r="C13" t="s">
-        <v>215</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>320</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C14" t="s">
         <v>215</v>
       </c>
       <c r="D14" t="s">
-        <v>368</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C15" t="s">
         <v>215</v>
       </c>
       <c r="D15" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>463</v>
+      </c>
+      <c r="B16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -2223,13 +2240,13 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C8" t="s">
         <v>385</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>386</v>
-      </c>
-      <c r="D8" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -2242,7 +2259,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3164,7 +3181,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3179,11 +3196,6 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>383</v>
-      </c>
-    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>258</v>
@@ -3191,7 +3203,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -3997,7 +4009,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed/finalized a bunch of stuff, added gatekeeper NPCs
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87009E14-FFA9-4636-B52A-A6BA539E7166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E790E7-35B4-42DA-971E-5A8A288C8FA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,28 +24,37 @@
     <sheet name="Monsters" sheetId="12" r:id="rId9"/>
     <sheet name="Maps" sheetId="8" r:id="rId10"/>
     <sheet name="MapChanges" sheetId="9" r:id="rId11"/>
-    <sheet name="NPCs" sheetId="10" r:id="rId12"/>
-    <sheet name="Chests" sheetId="11" r:id="rId13"/>
-    <sheet name="Doors" sheetId="24" r:id="rId14"/>
-    <sheet name="TextChanges" sheetId="13" r:id="rId15"/>
-    <sheet name="TileChangeEvents" sheetId="14" r:id="rId16"/>
-    <sheet name="CharChanges" sheetId="16" r:id="rId17"/>
-    <sheet name="New Object Graphics" sheetId="21" r:id="rId18"/>
-    <sheet name="Tiles" sheetId="15" r:id="rId19"/>
-    <sheet name="SpellChanges" sheetId="17" r:id="rId20"/>
-    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId21"/>
+    <sheet name="ElementChanges" sheetId="26" r:id="rId12"/>
+    <sheet name="NPCs" sheetId="10" r:id="rId13"/>
+    <sheet name="Chests" sheetId="11" r:id="rId14"/>
+    <sheet name="Doors" sheetId="24" r:id="rId15"/>
+    <sheet name="TextChanges" sheetId="13" r:id="rId16"/>
+    <sheet name="TileChangeEvents" sheetId="14" r:id="rId17"/>
+    <sheet name="CharChanges" sheetId="16" r:id="rId18"/>
+    <sheet name="New Object Graphics" sheetId="21" r:id="rId19"/>
+    <sheet name="Tiles" sheetId="15" r:id="rId20"/>
+    <sheet name="SpellChanges" sheetId="17" r:id="rId21"/>
+    <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId22"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="444">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -762,9 +771,6 @@
     <t>Pile of trash</t>
   </si>
   <si>
-    <t>Höhlenspinne</t>
-  </si>
-  <si>
     <t>Monster in Ship's end</t>
   </si>
   <si>
@@ -828,9 +834,6 @@
     <t>Finalize Torle's journal text</t>
   </si>
   <si>
-    <t>I guess I added wrong events to 372 or 373</t>
-  </si>
-  <si>
     <t>79: Warenhändler / Good merchant (Cavetown)</t>
   </si>
   <si>
@@ -870,9 +873,6 @@
     <t>Raft Dealer</t>
   </si>
   <si>
-    <t>Merchant Index 20: todo</t>
-  </si>
-  <si>
     <t>A bit more expensive (35) than Burnville blacksmith (25)</t>
   </si>
   <si>
@@ -1200,12 +1200,6 @@
     <t>Door in upper manyeyes' level looks wrong (the one with hammer is shown and without the correct overlays)</t>
   </si>
   <si>
-    <t>Pressure plate in gatekeeper house can be activated by eye cursor!</t>
-  </si>
-  <si>
-    <t>Finish cavetown (add NPCs in town and houses)</t>
-  </si>
-  <si>
     <t>Alex</t>
   </si>
   <si>
@@ -1219,6 +1213,186 @@
   </si>
   <si>
     <t>3 houses in cavetown</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>Gatekeeper's House (376)</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>Gatekeeper in middle house who wants a drink for the key</t>
+  </si>
+  <si>
+    <t>Gatekeeper in the right house who wants a treasure</t>
+  </si>
+  <si>
+    <t>Merchant Index 20: unlimited Torches (130), 1x Scimitar, 1x Zweihander, 1x Morning Star, 1x Trident, 1x Whip, 1x Murder Blade, 1x Compass, 1x Magic Picture, 1x Wind Pearl, 5x Shovel, 25x Rope, 2x Horn Helm, 1x Steel Helm, 1x Banded Armour, 1x Round Shield, 99x Magic Arrow, 1x Wishing Coins, 3x Lantern, 1x Holy Horn, 50x Magic Bolts, 5x Heal Paralyze Potion</t>
+  </si>
+  <si>
+    <t>250: Gave booze to Jeff the gatekeeper</t>
+  </si>
+  <si>
+    <t>251: Gave treasure map to Luke</t>
+  </si>
+  <si>
+    <t>1x Old Treasure Map</t>
+  </si>
+  <si>
+    <t>Finish cavetown (add NPCs in town)</t>
+  </si>
+  <si>
+    <t>Abandoned Hut (373)</t>
+  </si>
+  <si>
+    <t>1x Shovel</t>
+  </si>
+  <si>
+    <t>Altes Tagebuch / Old Diary</t>
+  </si>
+  <si>
+    <t>Found in the abandoned hut in Ship's End</t>
+  </si>
+  <si>
+    <t>1x Old Diary, 1x Ring of Sobek</t>
+  </si>
+  <si>
+    <t>Erdspinne</t>
+  </si>
+  <si>
+    <t>408 Windschrein: Event mit globvar raus</t>
+  </si>
+  <si>
+    <t>Rework NPC 37 (Karl) events</t>
+  </si>
+  <si>
+    <t>- Remove trainee in map 421 after building the wind gate</t>
+  </si>
+  <si>
+    <t>Add skeleton of trainee to cave</t>
+  </si>
+  <si>
+    <t>Rename Karl's ring to Apprentice's ring</t>
+  </si>
+  <si>
+    <t>- New introduction when you met the trainee (based on globvar)</t>
+  </si>
+  <si>
+    <t>- Merged texts</t>
+  </si>
+  <si>
+    <t>- Remove wind chain stuff</t>
+  </si>
+  <si>
+    <t>Element fixes:</t>
+  </si>
+  <si>
+    <t>Mystical Globe: Physical (4) -&gt; Mental (1)</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (ger): 0x4414F</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (ger): 0x46E9F</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (eng): 0x4413F</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (eng): 0x46E8F</t>
+  </si>
+  <si>
+    <t>Show Monster LP: Undead (8) -&gt; Mental (1)</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (ger): 0x44154</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (ger): 0x46EA4</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (eng): 0x44144</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (eng): 0x46E94</t>
+  </si>
+  <si>
+    <t>Whirlwind: None (0) -&gt; Wind (32)</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (ger): 0x44203</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (ger): 0x46F53</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (eng): 0x441F3</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (eng): 0x46F43</t>
+  </si>
+  <si>
+    <t>LP Stealer: Physical (4) -&gt; Undead (8)</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (ger): 0x440F5</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (ger): 0x46E45</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (eng): 0x440E5</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (eng): 0x46E35</t>
+  </si>
+  <si>
+    <t>Dispell Undead: Undead (8) -&gt; None (0)</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (ger): 0x4400F</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (ger): 0x46D5F</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (eng): 0x43FFF</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (eng): 0x46D4F</t>
+  </si>
+  <si>
+    <t>Destroy Undead: Undead (8) -&gt; None (0)</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (ger): 0x44014</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (ger): 0x46D64</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (eng): 0x44004</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (eng): 0x46D54</t>
+  </si>
+  <si>
+    <t>Holy Word: Undead (8) -&gt; None (0)</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (ger): 0x44019</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (ger): 0x46D69</t>
+  </si>
+  <si>
+    <t>- AM2_CPU (eng): 0x44009</t>
+  </si>
+  <si>
+    <t>- AM2_BLIT (eng): 0x46D59</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1422,6 +1596,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1867,13 +2042,13 @@
         <v>373</v>
       </c>
       <c r="B10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1881,13 +2056,13 @@
         <v>374</v>
       </c>
       <c r="B11" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C11" t="s">
         <v>215</v>
       </c>
       <c r="D11" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1895,13 +2070,13 @@
         <v>375</v>
       </c>
       <c r="B12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,13 +2084,13 @@
         <v>376</v>
       </c>
       <c r="B13" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1923,13 +2098,13 @@
         <v>461</v>
       </c>
       <c r="B14" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C14" t="s">
         <v>215</v>
       </c>
       <c r="D14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1937,13 +2112,13 @@
         <v>462</v>
       </c>
       <c r="B15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C15" t="s">
         <v>215</v>
       </c>
       <c r="D15" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1951,13 +2126,13 @@
         <v>463</v>
       </c>
       <c r="B16" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C16" t="s">
         <v>215</v>
       </c>
       <c r="D16" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -2073,10 +2248,10 @@
         <v>420</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2084,10 +2259,10 @@
         <v>421</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2130,123 +2305,193 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D8139E-327A-4885-8257-94E3A09DB943}">
+  <dimension ref="A1:A43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>319</v>
-      </c>
-      <c r="C7" t="s">
-        <v>298</v>
-      </c>
-      <c r="D7" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>384</v>
-      </c>
-      <c r="C8" t="s">
-        <v>385</v>
-      </c>
-      <c r="D8" t="s">
-        <v>386</v>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -2255,11 +2500,164 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C8" t="s">
+        <v>380</v>
+      </c>
+      <c r="D8" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>386</v>
+      </c>
+      <c r="C9" t="s">
+        <v>385</v>
+      </c>
+      <c r="D9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>384</v>
+      </c>
+      <c r="C10" t="s">
+        <v>385</v>
+      </c>
+      <c r="D10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2740,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2362,7 +2760,7 @@
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2403,10 +2801,10 @@
         <v>139</v>
       </c>
       <c r="B9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" t="s">
         <v>243</v>
-      </c>
-      <c r="C9" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2414,10 +2812,10 @@
         <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2425,10 +2823,10 @@
         <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2436,10 +2834,10 @@
         <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2447,10 +2845,10 @@
         <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C13" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2458,10 +2856,10 @@
         <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2469,10 +2867,10 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C15" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2480,10 +2878,10 @@
         <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C16" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2491,10 +2889,10 @@
         <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2502,10 +2900,10 @@
         <v>148</v>
       </c>
       <c r="B18" t="s">
+        <v>326</v>
+      </c>
+      <c r="C18" t="s">
         <v>329</v>
-      </c>
-      <c r="C18" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2513,10 +2911,10 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C19" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2524,10 +2922,10 @@
         <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C20" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2535,10 +2933,10 @@
         <v>151</v>
       </c>
       <c r="B21" t="s">
+        <v>336</v>
+      </c>
+      <c r="C21" t="s">
         <v>339</v>
-      </c>
-      <c r="C21" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2546,10 +2944,10 @@
         <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2557,10 +2955,10 @@
         <v>153</v>
       </c>
       <c r="B23" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C23" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2568,10 +2966,43 @@
         <v>154</v>
       </c>
       <c r="B24" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C24" t="s">
-        <v>372</v>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>155</v>
+      </c>
+      <c r="B25" t="s">
+        <v>242</v>
+      </c>
+      <c r="C25" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>156</v>
+      </c>
+      <c r="B26" t="s">
+        <v>394</v>
+      </c>
+      <c r="C26" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>157</v>
+      </c>
+      <c r="B27" t="s">
+        <v>394</v>
+      </c>
+      <c r="C27" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -2582,7 +3013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62C0FBA-1BDC-4EAA-90A2-D38035F594DC}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2597,7 +3028,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -2608,7 +3039,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2616,7 +3047,7 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2624,7 +3055,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2632,7 +3063,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2640,7 +3071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A23AD0D-3B64-4BEF-82E1-7DFFB5EA7471}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2675,7 +3106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAC578B-0798-484E-AD11-E9A5E47BA266}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2695,7 +3126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -2835,7 +3266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFAD946-A9D1-4502-A6CF-B93E446D51BE}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -2867,7 +3298,7 @@
         <v>231</v>
       </c>
       <c r="I1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2943,16 +3374,16 @@
         <v>374</v>
       </c>
       <c r="B6" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C6" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D6" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E6" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2961,7 +3392,87 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>404</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42293419-9ED8-4D74-9E3B-F691567047C5}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -3176,57 +3687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>381</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
   <dimension ref="A1:A75"/>
   <sheetViews>
@@ -3609,7 +4070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A938DC3D-143F-4871-88FF-86347B3EB68B}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -3624,32 +4085,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3659,10 +4120,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C25D-ED95-40AF-978F-1BDF8D4F496C}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3708,7 +4169,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -3723,7 +4184,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3783,47 +4244,57 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>371</v>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -3892,17 +4363,17 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3946,57 +4417,57 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4009,7 +4480,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4048,7 +4519,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>272</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4056,10 +4527,10 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C4" t="s">
         <v>270</v>
-      </c>
-      <c r="C4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4067,10 +4538,10 @@
         <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4078,10 +4549,10 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4089,10 +4560,10 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4103,7 +4574,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4111,10 +4582,10 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C9" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4175,10 +4646,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660A265-43B2-4101-9AAE-C44C4935A3ED}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4324,13 +4795,13 @@
         <v>409</v>
       </c>
       <c r="B8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4338,13 +4809,13 @@
         <v>410</v>
       </c>
       <c r="B9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4352,13 +4823,13 @@
         <v>411</v>
       </c>
       <c r="B10" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D10" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4366,13 +4837,13 @@
         <v>412</v>
       </c>
       <c r="B11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D11" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4380,13 +4851,13 @@
         <v>413</v>
       </c>
       <c r="B12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D12" t="s">
         <v>304</v>
-      </c>
-      <c r="D12" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4394,13 +4865,13 @@
         <v>414</v>
       </c>
       <c r="B13" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C13" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D13" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4408,13 +4879,13 @@
         <v>415</v>
       </c>
       <c r="B14" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D14" t="s">
         <v>335</v>
-      </c>
-      <c r="D14" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4422,13 +4893,13 @@
         <v>416</v>
       </c>
       <c r="B15" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C15" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D15" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4436,13 +4907,13 @@
         <v>417</v>
       </c>
       <c r="B16" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C16" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D16" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4450,13 +4921,13 @@
         <v>418</v>
       </c>
       <c r="B17" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C17" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D17" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4464,13 +4935,27 @@
         <v>419</v>
       </c>
       <c r="B18" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C18" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D18" t="s">
-        <v>375</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>420</v>
+      </c>
+      <c r="B19" t="s">
+        <v>396</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -4486,7 +4971,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4518,7 +5003,7 @@
         <v>32</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
@@ -4557,25 +5042,25 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" t="s">
         <v>236</v>
-      </c>
-      <c r="C3" t="s">
-        <v>237</v>
       </c>
       <c r="H3">
         <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N3">
         <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="P3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4583,16 +5068,16 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H4">
         <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -4600,16 +5085,16 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H5">
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -4617,16 +5102,16 @@
         <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C6" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H6">
         <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -4634,16 +5119,16 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H7">
         <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4651,16 +5136,16 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C8" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H8">
         <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -4668,16 +5153,16 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C9" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H9">
         <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -4685,7 +5170,7 @@
         <v>95</v>
       </c>
       <c r="I10" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -4693,7 +5178,7 @@
         <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted Karl and his apprentice
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E790E7-35B4-42DA-971E-5A8A288C8FA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826EFD83-8B2E-4B31-9C0B-9EA22819618D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="443">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1263,9 +1263,6 @@
     <t>Erdspinne</t>
   </si>
   <si>
-    <t>408 Windschrein: Event mit globvar raus</t>
-  </si>
-  <si>
     <t>Rework NPC 37 (Karl) events</t>
   </si>
   <si>
@@ -1278,15 +1275,6 @@
     <t>Rename Karl's ring to Apprentice's ring</t>
   </si>
   <si>
-    <t>- New introduction when you met the trainee (based on globvar)</t>
-  </si>
-  <si>
-    <t>- Merged texts</t>
-  </si>
-  <si>
-    <t>- Remove wind chain stuff</t>
-  </si>
-  <si>
     <t>Element fixes:</t>
   </si>
   <si>
@@ -1393,6 +1381,15 @@
   </si>
   <si>
     <t>- AM2_BLIT (eng): 0x46D59</t>
+  </si>
+  <si>
+    <t>Gustav</t>
+  </si>
+  <si>
+    <t>Tavern of the goddess (421)</t>
+  </si>
+  <si>
+    <t>Former apprentice of Karl</t>
   </si>
 </sst>
 </file>
@@ -2316,182 +2313,182 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -2501,16 +2498,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2645,6 +2642,20 @@
       </c>
       <c r="D10" t="s">
         <v>388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>440</v>
+      </c>
+      <c r="C11" t="s">
+        <v>441</v>
+      </c>
+      <c r="D11" t="s">
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -3394,10 +3405,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3427,45 +3438,28 @@
         <v>378</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>400</v>
-      </c>
-    </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>405</v>
-      </c>
-    </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>406</v>
+      <c r="A13" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>404</v>
-      </c>
+      <c r="A14" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4123,7 +4117,7 @@
   <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4307,7 +4301,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed dog hut tiles
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5DD101-CD83-459D-B850-2FF88993AA9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819025D2-2D4C-41A3-90E1-929D086025E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="442">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1233,9 +1233,6 @@
     <t>1x Old Treasure Map</t>
   </si>
   <si>
-    <t>Finish cavetown (add NPCs in town)</t>
-  </si>
-  <si>
     <t>Abandoned Hut (373)</t>
   </si>
   <si>
@@ -1254,12 +1251,6 @@
     <t>Erdspinne</t>
   </si>
   <si>
-    <t>Add skeleton of trainee to cave</t>
-  </si>
-  <si>
-    <t>Rename Karl's ring to Apprentice's ring</t>
-  </si>
-  <si>
     <t>Element fixes:</t>
   </si>
   <si>
@@ -1393,6 +1384,9 @@
   </si>
   <si>
     <t>1x Gustav's Ring, 1x Wishing Coins</t>
+  </si>
+  <si>
+    <t>Maybe make old woman a bit smaller in Cavetown</t>
   </si>
 </sst>
 </file>
@@ -2316,182 +2310,182 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -2504,7 +2498,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,13 +2646,13 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C11" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D11" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -2670,7 +2664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2807,7 +2801,7 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3002,10 +2996,10 @@
         <v>156</v>
       </c>
       <c r="B26" t="s">
+        <v>390</v>
+      </c>
+      <c r="C26" t="s">
         <v>391</v>
-      </c>
-      <c r="C26" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3013,10 +3007,10 @@
         <v>157</v>
       </c>
       <c r="B27" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -3410,8 +3404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3428,27 +3422,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>390</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>398</v>
+        <v>441</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -4365,17 +4349,17 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -4769,13 +4753,13 @@
         <v>407</v>
       </c>
       <c r="B6" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C6" t="s">
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4951,13 +4935,13 @@
         <v>420</v>
       </c>
       <c r="B19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -5044,7 +5028,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C3" t="s">
         <v>233</v>

</xml_diff>

<commit_message>
Changed black damage spells' damage values
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0E45B6-6ECF-4603-9945-F376941E2107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA51666-50DC-4DF1-83D4-D48FB134CBB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="458">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1381,6 +1381,60 @@
   </si>
   <si>
     <t>Amiga: Door in upper manyeyes' level looks wrong (the one with hammer is shown and without the correct overlays)</t>
+  </si>
+  <si>
+    <t>Damage Changes</t>
+  </si>
+  <si>
+    <t>Mudsling | 4-8 | 5-10</t>
+  </si>
+  <si>
+    <t>Rockfall | 10-25 | 12-25</t>
+  </si>
+  <si>
+    <t>Earthslide | 8-16 | 10-20</t>
+  </si>
+  <si>
+    <t>Earthquake | 8-22 | 8-18</t>
+  </si>
+  <si>
+    <t>Winddevil | 8-16 | 20-35</t>
+  </si>
+  <si>
+    <t>Windhowler | 16-48 | 30-50</t>
+  </si>
+  <si>
+    <t>Thunderbolt | 20-32 | 25-45</t>
+  </si>
+  <si>
+    <t>Whirlwind | 20-35 | 20-40</t>
+  </si>
+  <si>
+    <t>Firebeam | 20-30 | 45-75</t>
+  </si>
+  <si>
+    <t>Fireball | 40-85 | 70-120</t>
+  </si>
+  <si>
+    <t>Firestorm | 35-65 | 65-110</t>
+  </si>
+  <si>
+    <t>Firepillar | 40-70 | 60-100</t>
+  </si>
+  <si>
+    <t>Waterfall | 32-60 | 110-150</t>
+  </si>
+  <si>
+    <t>Iceball | 90-180 | 150-200</t>
+  </si>
+  <si>
+    <t>Icestorm | 64-128 | 130-180</t>
+  </si>
+  <si>
+    <t>Iceshower | 128-256 | 125-175</t>
+  </si>
+  <si>
+    <t>Name | Old | New</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1585,6 +1639,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -3398,7 +3456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -3644,10 +3702,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
-  <dimension ref="A1:A75"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3655,157 +3713,217 @@
     <col min="1" max="1" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>441</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>159</v>
       </c>
@@ -4021,7 +4139,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Lame spell is now only available in witch house
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA51666-50DC-4DF1-83D4-D48FB134CBB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA038569-2C64-4568-9627-FB079D2F60AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="465">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1435,6 +1435,27 @@
   </si>
   <si>
     <t>Name | Old | New</t>
+  </si>
+  <si>
+    <t>Witch house (411)</t>
+  </si>
+  <si>
+    <t>Replaced 29x Magic Projectile spell scrolls with 15x Lame scrolls</t>
+  </si>
+  <si>
+    <t>Change merchants</t>
+  </si>
+  <si>
+    <t>Replaced Lame scrolls by Magic Projectile scrolls</t>
+  </si>
+  <si>
+    <t>Nalven's Magical School</t>
+  </si>
+  <si>
+    <t>Zombiemaster</t>
+  </si>
+  <si>
+    <t>Now drops Sleep scroll instead of Lame scroll</t>
   </si>
 </sst>
 </file>
@@ -2717,7 +2738,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,6 +2853,15 @@
       </c>
       <c r="C6" t="s">
         <v>82</v>
+      </c>
+      <c r="E6">
+        <v>84</v>
+      </c>
+      <c r="F6" t="s">
+        <v>458</v>
+      </c>
+      <c r="G6" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3704,13 +3734,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5819E0-6767-42B1-A03F-190E8B90AA2C}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4569,15 +4601,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3244EE-9DE8-4394-8A72-E957F0B76A39}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="99.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4678,6 +4710,22 @@
       </c>
       <c r="C9" t="s">
         <v>281</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>462</v>
+      </c>
+      <c r="C24" t="s">
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -5062,8 +5110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5961762D-6D3E-4C96-84C7-B754C8917FD8}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5073,6 +5121,7 @@
     <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -5170,6 +5219,15 @@
       </c>
       <c r="I4" t="s">
         <v>234</v>
+      </c>
+      <c r="N4">
+        <v>8</v>
+      </c>
+      <c r="O4" t="s">
+        <v>463</v>
+      </c>
+      <c r="P4" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed some issues with 3D labdata
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9AAEAB-19C6-4DF0-85CB-C42B671CE627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515B6A9E-5FD8-4F49-A5E3-6DAE8B9B7132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="477">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1146,9 +1146,6 @@
     <t>Upper floor of Manyeyes' castle</t>
   </si>
   <si>
-    <t>The black man statue is not drawn correctly for Amiga. Maybe gfx is missing?</t>
-  </si>
-  <si>
     <t>248: Fallen through roof of Manyeyes' castle once</t>
   </si>
   <si>
@@ -1377,9 +1374,6 @@
     <t>1x Gustav's Ring, 1x Wishing Coins</t>
   </si>
   <si>
-    <t>Amiga: Door in upper manyeyes' level looks wrong (the one with hammer is shown and without the correct overlays)</t>
-  </si>
-  <si>
     <t>Damage Changes</t>
   </si>
   <si>
@@ -1485,9 +1479,6 @@
     <t>252: Removed magic flying disc in eye of vortex</t>
   </si>
   <si>
-    <t>Raft is above the beach in center</t>
-  </si>
-  <si>
     <t>1x Magic Flying Disc</t>
   </si>
   <si>
@@ -1497,7 +1488,10 @@
     <t>254: Just removed magic flying disc in the event chain</t>
   </si>
   <si>
-    <t>1x Wishing Coins, 20 Gold</t>
+    <t>1x Wishing Coins</t>
+  </si>
+  <si>
+    <t>Dark Blade has +234 damage on Amiga</t>
   </si>
 </sst>
 </file>
@@ -2193,13 +2187,13 @@
         <v>376</v>
       </c>
       <c r="B13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2425,182 +2419,182 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2719,13 +2713,13 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>372</v>
+      </c>
+      <c r="C8" t="s">
         <v>373</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>374</v>
-      </c>
-      <c r="D8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2733,13 +2727,13 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C9" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" t="s">
         <v>380</v>
-      </c>
-      <c r="C9" t="s">
-        <v>379</v>
-      </c>
-      <c r="D9" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2747,13 +2741,13 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
+        <v>377</v>
+      </c>
+      <c r="C10" t="s">
         <v>378</v>
       </c>
-      <c r="C10" t="s">
-        <v>379</v>
-      </c>
       <c r="D10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2761,13 +2755,13 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
+        <v>428</v>
+      </c>
+      <c r="C11" t="s">
         <v>429</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>430</v>
-      </c>
-      <c r="D11" t="s">
-        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -2779,7 +2773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E1CF46-42F9-4EAE-9733-88B0C19839E5}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -2863,7 +2857,7 @@
         <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2883,7 +2877,7 @@
         <v>97</v>
       </c>
       <c r="G5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2900,10 +2894,10 @@
         <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2920,10 +2914,10 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G7" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2934,16 +2928,16 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E8">
         <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3119,7 +3113,7 @@
         <v>349</v>
       </c>
       <c r="C24" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3130,7 +3124,7 @@
         <v>238</v>
       </c>
       <c r="C25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3138,10 +3132,10 @@
         <v>156</v>
       </c>
       <c r="B26" t="s">
+        <v>386</v>
+      </c>
+      <c r="C26" t="s">
         <v>387</v>
-      </c>
-      <c r="C26" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3149,10 +3143,10 @@
         <v>157</v>
       </c>
       <c r="B27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C27" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3163,7 +3157,7 @@
         <v>238</v>
       </c>
       <c r="C28" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3174,7 +3168,7 @@
         <v>238</v>
       </c>
       <c r="C29" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3185,7 +3179,7 @@
         <v>238</v>
       </c>
       <c r="C30" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -3579,25 +3573,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -3843,7 +3825,7 @@
         <v>156</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="15"/>
@@ -3853,7 +3835,7 @@
         <v>129</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="21"/>
@@ -3863,7 +3845,7 @@
         <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -3873,7 +3855,7 @@
         <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3881,7 +3863,7 @@
         <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3889,7 +3871,7 @@
         <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3897,7 +3879,7 @@
         <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3905,7 +3887,7 @@
         <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3913,7 +3895,7 @@
         <v>136</v>
       </c>
       <c r="C9" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3921,7 +3903,7 @@
         <v>137</v>
       </c>
       <c r="C10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3929,7 +3911,7 @@
         <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3937,7 +3919,7 @@
         <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3945,7 +3927,7 @@
         <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3953,7 +3935,7 @@
         <v>141</v>
       </c>
       <c r="C14" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3961,7 +3943,7 @@
         <v>142</v>
       </c>
       <c r="C15" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3969,7 +3951,7 @@
         <v>143</v>
       </c>
       <c r="C16" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3977,7 +3959,7 @@
         <v>144</v>
       </c>
       <c r="C17" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3985,7 +3967,7 @@
         <v>145</v>
       </c>
       <c r="C18" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4481,37 +4463,37 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -4595,17 +4577,17 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -4751,7 +4733,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4822,7 +4804,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4830,10 +4812,10 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C24" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4841,10 +4823,10 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C25" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -5026,13 +5008,13 @@
         <v>407</v>
       </c>
       <c r="B6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C6" t="s">
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5194,13 +5176,13 @@
         <v>419</v>
       </c>
       <c r="B18" t="s">
+        <v>364</v>
+      </c>
+      <c r="C18" t="s">
         <v>365</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>366</v>
-      </c>
-      <c r="D18" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5208,13 +5190,13 @@
         <v>420</v>
       </c>
       <c r="B19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -5263,7 +5245,7 @@
         <v>32</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
@@ -5302,7 +5284,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C3" t="s">
         <v>232</v>
@@ -5317,10 +5299,10 @@
         <v>19</v>
       </c>
       <c r="O3" t="s">
+        <v>370</v>
+      </c>
+      <c r="P3" t="s">
         <v>371</v>
-      </c>
-      <c r="P3" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -5343,10 +5325,10 @@
         <v>8</v>
       </c>
       <c r="O4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="P4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -5369,10 +5351,10 @@
         <v>21</v>
       </c>
       <c r="O5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="P5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed some german texts
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515B6A9E-5FD8-4F49-A5E3-6DAE8B9B7132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D27FD19-6821-4B41-B8EE-7474F12B6448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="475">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -874,12 +874,6 @@
   </si>
   <si>
     <t>Tavern of the goddess</t>
-  </si>
-  <si>
-    <t>Snakesign</t>
-  </si>
-  <si>
-    <t>Added drunken NPC</t>
   </si>
   <si>
     <t>Global var 226 is now set when you enter the tavern, added NPC who talks about Karl</t>
@@ -2159,13 +2153,13 @@
         <v>374</v>
       </c>
       <c r="B11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
         <v>212</v>
       </c>
       <c r="D11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2173,13 +2167,13 @@
         <v>375</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2187,13 +2181,13 @@
         <v>376</v>
       </c>
       <c r="B13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2201,13 +2195,13 @@
         <v>461</v>
       </c>
       <c r="B14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C14" t="s">
         <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2215,13 +2209,13 @@
         <v>462</v>
       </c>
       <c r="B15" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C15" t="s">
         <v>212</v>
       </c>
       <c r="D15" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2229,13 +2223,13 @@
         <v>463</v>
       </c>
       <c r="B16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C16" t="s">
         <v>212</v>
       </c>
       <c r="D16" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -2248,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8633A58-1CC4-49CC-A9EF-ED848DF63C3A}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,26 +2340,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>421</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2419,182 +2402,182 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -2699,13 +2682,13 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2713,13 +2696,13 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C8" t="s">
+        <v>371</v>
+      </c>
+      <c r="D8" t="s">
         <v>372</v>
-      </c>
-      <c r="C8" t="s">
-        <v>373</v>
-      </c>
-      <c r="D8" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2727,13 +2710,13 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C9" t="s">
+        <v>376</v>
+      </c>
+      <c r="D9" t="s">
         <v>378</v>
-      </c>
-      <c r="D9" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2741,13 +2724,13 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2755,13 +2738,13 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" t="s">
+        <v>427</v>
+      </c>
+      <c r="D11" t="s">
         <v>428</v>
-      </c>
-      <c r="C11" t="s">
-        <v>429</v>
-      </c>
-      <c r="D11" t="s">
-        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -2774,7 +2757,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2857,7 +2840,7 @@
         <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2877,7 +2860,7 @@
         <v>97</v>
       </c>
       <c r="G5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2894,10 +2877,10 @@
         <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2914,10 +2897,10 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2928,16 +2911,16 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E8">
         <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2989,10 +2972,10 @@
         <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3000,10 +2983,10 @@
         <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3011,10 +2994,10 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3022,10 +3005,10 @@
         <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3033,10 +3016,10 @@
         <v>147</v>
       </c>
       <c r="B17" t="s">
+        <v>319</v>
+      </c>
+      <c r="C17" t="s">
         <v>321</v>
-      </c>
-      <c r="C17" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3044,10 +3027,10 @@
         <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3055,10 +3038,10 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3066,10 +3049,10 @@
         <v>150</v>
       </c>
       <c r="B20" t="s">
+        <v>329</v>
+      </c>
+      <c r="C20" t="s">
         <v>331</v>
-      </c>
-      <c r="C20" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3077,10 +3060,10 @@
         <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C21" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3088,10 +3071,10 @@
         <v>152</v>
       </c>
       <c r="B22" t="s">
+        <v>347</v>
+      </c>
+      <c r="C22" t="s">
         <v>349</v>
-      </c>
-      <c r="C22" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3099,10 +3082,10 @@
         <v>153</v>
       </c>
       <c r="B23" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C23" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3110,10 +3093,10 @@
         <v>154</v>
       </c>
       <c r="B24" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C24" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3124,7 +3107,7 @@
         <v>238</v>
       </c>
       <c r="C25" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3132,10 +3115,10 @@
         <v>156</v>
       </c>
       <c r="B26" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C26" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3143,10 +3126,10 @@
         <v>157</v>
       </c>
       <c r="B27" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C27" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3157,7 +3140,7 @@
         <v>238</v>
       </c>
       <c r="C28" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3168,7 +3151,7 @@
         <v>238</v>
       </c>
       <c r="C29" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3179,7 +3162,7 @@
         <v>238</v>
       </c>
       <c r="C30" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -3205,7 +3188,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -3216,7 +3199,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3224,7 +3207,7 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3232,7 +3215,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3240,7 +3223,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -3475,7 +3458,7 @@
         <v>227</v>
       </c>
       <c r="I1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3551,16 +3534,16 @@
         <v>374</v>
       </c>
       <c r="B6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -3573,13 +3556,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914EDC47-D4FD-4B0B-A76D-17F07014FD7F}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -3825,7 +3810,7 @@
         <v>156</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="15"/>
@@ -3835,7 +3820,7 @@
         <v>129</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="21"/>
@@ -3845,7 +3830,7 @@
         <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -3855,7 +3840,7 @@
         <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3863,7 +3848,7 @@
         <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3871,7 +3856,7 @@
         <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3879,7 +3864,7 @@
         <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3887,7 +3872,7 @@
         <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3895,7 +3880,7 @@
         <v>136</v>
       </c>
       <c r="C9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3903,7 +3888,7 @@
         <v>137</v>
       </c>
       <c r="C10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3911,7 +3896,7 @@
         <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3919,7 +3904,7 @@
         <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3927,7 +3912,7 @@
         <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3935,7 +3920,7 @@
         <v>141</v>
       </c>
       <c r="C14" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3943,7 +3928,7 @@
         <v>142</v>
       </c>
       <c r="C15" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3951,7 +3936,7 @@
         <v>143</v>
       </c>
       <c r="C16" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3959,7 +3944,7 @@
         <v>144</v>
       </c>
       <c r="C17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3967,7 +3952,7 @@
         <v>145</v>
       </c>
       <c r="C18" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4368,7 +4353,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -4448,52 +4433,52 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -4562,32 +4547,32 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -4733,7 +4718,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4774,10 +4759,10 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4788,7 +4773,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4796,15 +4781,15 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4812,10 +4797,10 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C24" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4823,10 +4808,10 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C25" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -4890,7 +4875,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5008,13 +4993,13 @@
         <v>407</v>
       </c>
       <c r="B6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C6" t="s">
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5036,13 +5021,13 @@
         <v>409</v>
       </c>
       <c r="B8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D8" t="s">
         <v>283</v>
-      </c>
-      <c r="C8" t="s">
-        <v>284</v>
-      </c>
-      <c r="D8" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5050,13 +5035,13 @@
         <v>410</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5064,13 +5049,13 @@
         <v>411</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5078,13 +5063,13 @@
         <v>412</v>
       </c>
       <c r="B11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C11" t="s">
+        <v>294</v>
+      </c>
+      <c r="D11" t="s">
         <v>295</v>
-      </c>
-      <c r="C11" t="s">
-        <v>296</v>
-      </c>
-      <c r="D11" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5092,13 +5077,13 @@
         <v>413</v>
       </c>
       <c r="B12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5106,13 +5091,13 @@
         <v>414</v>
       </c>
       <c r="B13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D13" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5120,13 +5105,13 @@
         <v>415</v>
       </c>
       <c r="B14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5134,13 +5119,13 @@
         <v>416</v>
       </c>
       <c r="B15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D15" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5148,13 +5133,13 @@
         <v>417</v>
       </c>
       <c r="B16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5162,13 +5147,13 @@
         <v>418</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C17" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5176,13 +5161,13 @@
         <v>419</v>
       </c>
       <c r="B18" t="s">
+        <v>362</v>
+      </c>
+      <c r="C18" t="s">
+        <v>363</v>
+      </c>
+      <c r="D18" t="s">
         <v>364</v>
-      </c>
-      <c r="C18" t="s">
-        <v>365</v>
-      </c>
-      <c r="D18" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5190,13 +5175,13 @@
         <v>420</v>
       </c>
       <c r="B19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -5245,7 +5230,7 @@
         <v>32</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
@@ -5284,7 +5269,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C3" t="s">
         <v>232</v>
@@ -5299,10 +5284,10 @@
         <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="P3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -5310,10 +5295,10 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H4">
         <v>89</v>
@@ -5325,10 +5310,10 @@
         <v>8</v>
       </c>
       <c r="O4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="P4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -5336,25 +5321,25 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H5">
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="N5">
         <v>21</v>
       </c>
       <c r="O5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="P5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -5362,16 +5347,16 @@
         <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H6">
         <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -5379,16 +5364,16 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H7">
         <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -5396,16 +5381,16 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H8">
         <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -5413,16 +5398,16 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C9" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H9">
         <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -5430,7 +5415,7 @@
         <v>95</v>
       </c>
       <c r="I10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -5438,7 +5423,7 @@
         <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increased Egil's TP/lvl from 5 to 6
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3179484-0F92-4A49-BC9B-852CFFECB649}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2769A8BB-3DC8-4E1A-9BB1-0405D53C48A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="486">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1513,6 +1513,12 @@
   </si>
   <si>
     <t>Added sea quest events</t>
+  </si>
+  <si>
+    <t>Egil</t>
+  </si>
+  <si>
+    <t>TP/Lvl 8 -&gt; 6</t>
   </si>
 </sst>
 </file>
@@ -1704,6 +1710,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1716,11 +1727,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2687,7 +2693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491449B-92A2-40E4-A53E-51EAF196F725}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
@@ -2910,10 +2916,10 @@
       <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -3428,10 +3434,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3558,6 +3564,14 @@
       </c>
       <c r="B15" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>484</v>
+      </c>
+      <c r="B16" t="s">
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -3701,7 +3715,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3723,16 +3737,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="G1" s="13" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="G1" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3942,21 +3956,21 @@
       <c r="A1" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="18" t="s">
         <v>435</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3965,8 +3979,8 @@
       <c r="C3" t="s">
         <v>436</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -5043,11 +5057,11 @@
       <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -5373,11 +5387,11 @@
       <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="21" t="s">
         <v>368</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>

<commit_message>
Adjusted level factors and start exp (see excel file)
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2769A8BB-3DC8-4E1A-9BB1-0405D53C48A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE40E04-619E-4758-A17E-80A90CF3037E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="516">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1519,6 +1519,96 @@
   </si>
   <si>
     <t>TP/Lvl 8 -&gt; 6</t>
+  </si>
+  <si>
+    <t>Exp factors are given in AM2_*. Just search for the sequence 00 4B 00 96 00 B4 00 64 00 7D 00 5A 00 5A 00 5A 00 5F 7F FF.</t>
+  </si>
+  <si>
+    <t>Exp Factors</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>Thalion</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Adventurer</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Paladin</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Healer</t>
+  </si>
+  <si>
+    <t>Alchemist</t>
+  </si>
+  <si>
+    <t>Mystic</t>
+  </si>
+  <si>
+    <t>Magician</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Lvl10 (old)</t>
+  </si>
+  <si>
+    <t>Lvl10 (new)</t>
+  </si>
+  <si>
+    <t>Lvl25 (old)</t>
+  </si>
+  <si>
+    <t>Lvl25 (new)</t>
+  </si>
+  <si>
+    <t>Lvl50 (old)</t>
+  </si>
+  <si>
+    <t>Lvl50 (new)</t>
+  </si>
+  <si>
+    <t>Start (new)</t>
+  </si>
+  <si>
+    <t>Startlvl (old)</t>
+  </si>
+  <si>
+    <t>StartExp (old)</t>
+  </si>
+  <si>
+    <t>StartExp (new)</t>
+  </si>
+  <si>
+    <t>Tar</t>
+  </si>
+  <si>
+    <t>Selena</t>
+  </si>
+  <si>
+    <t>ClassFactor (old)</t>
+  </si>
+  <si>
+    <t>ClassFactor (new)</t>
+  </si>
+  <si>
+    <t>Nelvin</t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1685,12 +1775,270 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1736,6 +2084,37 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -3434,27 +3813,40 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" s="25" t="s">
+        <v>487</v>
+      </c>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -3462,103 +3854,463 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4" s="42" t="s">
+        <v>490</v>
+      </c>
+      <c r="F4" s="40" t="s">
+        <v>488</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>501</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>502</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>503</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="M4" s="31" t="s">
+        <v>505</v>
+      </c>
+      <c r="N4" s="46" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
       <c r="B5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E5" s="43" t="s">
+        <v>491</v>
+      </c>
+      <c r="F5" s="30">
+        <v>75</v>
+      </c>
+      <c r="G5" s="34">
+        <v>75</v>
+      </c>
+      <c r="I5" s="33">
+        <f>50*F5</f>
+        <v>3750</v>
+      </c>
+      <c r="J5" s="34">
+        <f>50*G5</f>
+        <v>3750</v>
+      </c>
+      <c r="K5" s="33">
+        <f>325*F5</f>
+        <v>24375</v>
+      </c>
+      <c r="L5" s="34">
+        <f>325*G5</f>
+        <v>24375</v>
+      </c>
+      <c r="M5" s="33">
+        <f>1250*F5</f>
+        <v>93750</v>
+      </c>
+      <c r="N5" s="47">
+        <f>1250*G5</f>
+        <v>93750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E6" s="43" t="s">
+        <v>492</v>
+      </c>
+      <c r="F6" s="30">
+        <v>150</v>
+      </c>
+      <c r="G6" s="38">
+        <v>110</v>
+      </c>
+      <c r="I6" s="33">
+        <f t="shared" ref="I6:I14" si="0">50*F6</f>
+        <v>7500</v>
+      </c>
+      <c r="J6" s="34">
+        <f t="shared" ref="J6:J14" si="1">50*G6</f>
+        <v>5500</v>
+      </c>
+      <c r="K6" s="33">
+        <f t="shared" ref="K6:K14" si="2">325*F6</f>
+        <v>48750</v>
+      </c>
+      <c r="L6" s="34">
+        <f t="shared" ref="L6:L14" si="3">325*G6</f>
+        <v>35750</v>
+      </c>
+      <c r="M6" s="33">
+        <f t="shared" ref="M6:M14" si="4">1250*F6</f>
+        <v>187500</v>
+      </c>
+      <c r="N6" s="47">
+        <f t="shared" ref="N6:N14" si="5">1250*G6</f>
+        <v>137500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E7" s="43" t="s">
+        <v>493</v>
+      </c>
+      <c r="F7" s="30">
+        <v>180</v>
+      </c>
+      <c r="G7" s="38">
+        <v>155</v>
+      </c>
+      <c r="I7" s="33">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+      <c r="J7" s="34">
+        <f t="shared" si="1"/>
+        <v>7750</v>
+      </c>
+      <c r="K7" s="33">
+        <f t="shared" si="2"/>
+        <v>58500</v>
+      </c>
+      <c r="L7" s="34">
+        <f t="shared" si="3"/>
+        <v>50375</v>
+      </c>
+      <c r="M7" s="33">
+        <f t="shared" si="4"/>
+        <v>225000</v>
+      </c>
+      <c r="N7" s="47">
+        <f t="shared" si="5"/>
+        <v>193750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>119</v>
       </c>
       <c r="B8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E8" s="44" t="s">
+        <v>494</v>
+      </c>
+      <c r="F8" s="30">
+        <v>100</v>
+      </c>
+      <c r="G8" s="38">
+        <v>85</v>
+      </c>
+      <c r="I8" s="33">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="J8" s="34">
+        <f t="shared" si="1"/>
+        <v>4250</v>
+      </c>
+      <c r="K8" s="33">
+        <f t="shared" si="2"/>
+        <v>32500</v>
+      </c>
+      <c r="L8" s="34">
+        <f t="shared" si="3"/>
+        <v>27625</v>
+      </c>
+      <c r="M8" s="33">
+        <f t="shared" si="4"/>
+        <v>125000</v>
+      </c>
+      <c r="N8" s="47">
+        <f t="shared" si="5"/>
+        <v>106250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E9" s="44" t="s">
+        <v>495</v>
+      </c>
+      <c r="F9" s="30">
+        <v>125</v>
+      </c>
+      <c r="G9" s="34">
+        <v>125</v>
+      </c>
+      <c r="I9" s="33">
+        <f t="shared" si="0"/>
+        <v>6250</v>
+      </c>
+      <c r="J9" s="34">
+        <f t="shared" si="1"/>
+        <v>6250</v>
+      </c>
+      <c r="K9" s="33">
+        <f t="shared" si="2"/>
+        <v>40625</v>
+      </c>
+      <c r="L9" s="34">
+        <f t="shared" si="3"/>
+        <v>40625</v>
+      </c>
+      <c r="M9" s="33">
+        <f t="shared" si="4"/>
+        <v>156250</v>
+      </c>
+      <c r="N9" s="47">
+        <f t="shared" si="5"/>
+        <v>156250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>119</v>
       </c>
       <c r="B10" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E10" s="44" t="s">
+        <v>496</v>
+      </c>
+      <c r="F10" s="30">
+        <v>90</v>
+      </c>
+      <c r="G10" s="34">
+        <v>90</v>
+      </c>
+      <c r="I10" s="33">
+        <f t="shared" si="0"/>
+        <v>4500</v>
+      </c>
+      <c r="J10" s="34">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+      <c r="K10" s="33">
+        <f t="shared" si="2"/>
+        <v>29250</v>
+      </c>
+      <c r="L10" s="34">
+        <f t="shared" si="3"/>
+        <v>29250</v>
+      </c>
+      <c r="M10" s="33">
+        <f t="shared" si="4"/>
+        <v>112500</v>
+      </c>
+      <c r="N10" s="47">
+        <f t="shared" si="5"/>
+        <v>112500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>123</v>
       </c>
       <c r="B11" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E11" s="44" t="s">
+        <v>497</v>
+      </c>
+      <c r="F11" s="30">
+        <v>90</v>
+      </c>
+      <c r="G11" s="38">
+        <v>85</v>
+      </c>
+      <c r="I11" s="33">
+        <f t="shared" si="0"/>
+        <v>4500</v>
+      </c>
+      <c r="J11" s="34">
+        <f t="shared" si="1"/>
+        <v>4250</v>
+      </c>
+      <c r="K11" s="33">
+        <f t="shared" si="2"/>
+        <v>29250</v>
+      </c>
+      <c r="L11" s="34">
+        <f t="shared" si="3"/>
+        <v>27625</v>
+      </c>
+      <c r="M11" s="33">
+        <f t="shared" si="4"/>
+        <v>112500</v>
+      </c>
+      <c r="N11" s="47">
+        <f t="shared" si="5"/>
+        <v>106250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>123</v>
       </c>
       <c r="B12" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E12" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="F12" s="30">
+        <v>90</v>
+      </c>
+      <c r="G12" s="38">
+        <v>80</v>
+      </c>
+      <c r="I12" s="33">
+        <f t="shared" si="0"/>
+        <v>4500</v>
+      </c>
+      <c r="J12" s="34">
+        <f t="shared" si="1"/>
+        <v>4000</v>
+      </c>
+      <c r="K12" s="33">
+        <f t="shared" si="2"/>
+        <v>29250</v>
+      </c>
+      <c r="L12" s="34">
+        <f t="shared" si="3"/>
+        <v>26000</v>
+      </c>
+      <c r="M12" s="33">
+        <f t="shared" si="4"/>
+        <v>112500</v>
+      </c>
+      <c r="N12" s="47">
+        <f t="shared" si="5"/>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>123</v>
       </c>
       <c r="B13" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E13" s="44" t="s">
+        <v>499</v>
+      </c>
+      <c r="F13" s="30">
+        <v>95</v>
+      </c>
+      <c r="G13" s="34">
+        <v>95</v>
+      </c>
+      <c r="I13" s="33">
+        <f t="shared" si="0"/>
+        <v>4750</v>
+      </c>
+      <c r="J13" s="34">
+        <f t="shared" si="1"/>
+        <v>4750</v>
+      </c>
+      <c r="K13" s="33">
+        <f t="shared" si="2"/>
+        <v>30875</v>
+      </c>
+      <c r="L13" s="34">
+        <f t="shared" si="3"/>
+        <v>30875</v>
+      </c>
+      <c r="M13" s="33">
+        <f t="shared" si="4"/>
+        <v>118750</v>
+      </c>
+      <c r="N13" s="47">
+        <f t="shared" si="5"/>
+        <v>118750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>126</v>
       </c>
       <c r="B14" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E14" s="45" t="s">
+        <v>500</v>
+      </c>
+      <c r="F14" s="41">
+        <v>32767</v>
+      </c>
+      <c r="G14" s="36">
+        <v>32767</v>
+      </c>
+      <c r="I14" s="35">
+        <f t="shared" si="0"/>
+        <v>1638350</v>
+      </c>
+      <c r="J14" s="36">
+        <f t="shared" si="1"/>
+        <v>1638350</v>
+      </c>
+      <c r="K14" s="35">
+        <f t="shared" si="2"/>
+        <v>10649275</v>
+      </c>
+      <c r="L14" s="36">
+        <f t="shared" si="3"/>
+        <v>10649275</v>
+      </c>
+      <c r="M14" s="35">
+        <f t="shared" si="4"/>
+        <v>40958750</v>
+      </c>
+      <c r="N14" s="48">
+        <f t="shared" si="5"/>
+        <v>40958750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>126</v>
       </c>
@@ -3566,7 +4318,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>484</v>
       </c>
@@ -3574,7 +4326,303 @@
         <v>485</v>
       </c>
     </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E17" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>509</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>510</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>508</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>507</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>513</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E18" s="33" t="s">
+        <v>489</v>
+      </c>
+      <c r="F18" s="28">
+        <v>75</v>
+      </c>
+      <c r="G18" s="28">
+        <v>75</v>
+      </c>
+      <c r="H18" s="28">
+        <f t="shared" ref="H18:H20" si="6">IF(MOD(ROUNDDOWN(SQRT(2*F18/J18),0),2)=0,ROUNDDOWN(SQRT(2*F18/J18),0),ROUNDDOWN(-0.5+SQRT(0.25+2*F18/J18),0))</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="28">
+        <f t="shared" ref="I18:I20" si="7">IF(MOD(ROUNDDOWN(SQRT(2*G18/K18),0),2)=0,ROUNDDOWN(SQRT(2*G18/K18),0),ROUNDDOWN(-0.5+SQRT(0.25+2*G18/K18),0))</f>
+        <v>1</v>
+      </c>
+      <c r="J18" s="28">
+        <f>F5</f>
+        <v>75</v>
+      </c>
+      <c r="K18" s="34">
+        <f>G5</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="33" t="s">
+        <v>511</v>
+      </c>
+      <c r="F19" s="28">
+        <v>59850</v>
+      </c>
+      <c r="G19" s="28">
+        <v>59850</v>
+      </c>
+      <c r="H19" s="28">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="I19" s="28">
+        <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="J19" s="28">
+        <f>F13</f>
+        <v>95</v>
+      </c>
+      <c r="K19" s="34">
+        <f>G13</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E20" s="33" t="s">
+        <v>484</v>
+      </c>
+      <c r="F20" s="28">
+        <v>150</v>
+      </c>
+      <c r="G20" s="29">
+        <v>110</v>
+      </c>
+      <c r="H20" s="28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="28">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="28">
+        <f>F6</f>
+        <v>150</v>
+      </c>
+      <c r="K20" s="34">
+        <f>G6</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E21" s="33" t="s">
+        <v>512</v>
+      </c>
+      <c r="F21" s="28">
+        <v>600</v>
+      </c>
+      <c r="G21" s="29">
+        <v>550</v>
+      </c>
+      <c r="H21" s="28">
+        <f>IF(MOD(ROUNDDOWN(SQRT(2*F21/J21),0),2)=0,ROUNDDOWN(SQRT(2*F21/J21),0),ROUNDDOWN(-0.5+SQRT(0.25+2*F21/J21),0))</f>
+        <v>3</v>
+      </c>
+      <c r="I21" s="28">
+        <f>IF(MOD(ROUNDDOWN(SQRT(2*G21/K21),0),2)=0,ROUNDDOWN(SQRT(2*G21/K21),0),ROUNDDOWN(-0.5+SQRT(0.25+2*G21/K21),0))</f>
+        <v>3</v>
+      </c>
+      <c r="J21" s="28">
+        <f>F8</f>
+        <v>100</v>
+      </c>
+      <c r="K21" s="34">
+        <f>G8</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="33" t="s">
+        <v>515</v>
+      </c>
+      <c r="F22" s="28">
+        <v>950</v>
+      </c>
+      <c r="G22" s="28">
+        <v>950</v>
+      </c>
+      <c r="H22" s="28">
+        <f t="shared" ref="H19:H27" si="8">ROUNDDOWN(-0.5+SQRT(0.25+2*F22/J22),0)</f>
+        <v>4</v>
+      </c>
+      <c r="I22" s="28">
+        <f t="shared" ref="I19:I27" si="9">ROUNDDOWN(-0.5+SQRT(0.25+2*G22/K22),0)</f>
+        <v>4</v>
+      </c>
+      <c r="J22" s="28">
+        <f>F13</f>
+        <v>95</v>
+      </c>
+      <c r="K22" s="34">
+        <f>G13</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="28">
+        <v>1890</v>
+      </c>
+      <c r="G23" s="28">
+        <v>1890</v>
+      </c>
+      <c r="H23" s="28">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="I23" s="28">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="J23" s="28">
+        <f>F10</f>
+        <v>90</v>
+      </c>
+      <c r="K23" s="34">
+        <f>G10</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="F24" s="28">
+        <v>4500</v>
+      </c>
+      <c r="G24" s="28">
+        <v>4500</v>
+      </c>
+      <c r="H24" s="28">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="I24" s="28">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="J24" s="28">
+        <f>F9</f>
+        <v>125</v>
+      </c>
+      <c r="K24" s="34">
+        <f>G9</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="28">
+        <v>12240</v>
+      </c>
+      <c r="G25" s="29">
+        <v>11500</v>
+      </c>
+      <c r="H25" s="28">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="I25" s="28">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="J25" s="28">
+        <f>F12</f>
+        <v>90</v>
+      </c>
+      <c r="K25" s="34">
+        <f>G12</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E26" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="28">
+        <v>29250</v>
+      </c>
+      <c r="G26" s="29">
+        <v>28750</v>
+      </c>
+      <c r="H26" s="28">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="I26" s="28">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="J26" s="28">
+        <f>F11</f>
+        <v>90</v>
+      </c>
+      <c r="K26" s="34">
+        <f>G11</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="39">
+        <v>113400</v>
+      </c>
+      <c r="G27" s="49">
+        <v>100000</v>
+      </c>
+      <c r="H27" s="39">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="I27" s="39">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="J27" s="39">
+        <f>F7</f>
+        <v>180</v>
+      </c>
+      <c r="K27" s="36">
+        <f>G7</f>
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added first parts of the new dungeon
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\C#\Projects\Ambermoon\Ambermoon-Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE40E04-619E-4758-A17E-80A90CF3037E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEB6945-14BC-4AD6-81FA-62714AFE18E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="16" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,8 @@
     <sheet name="Tiles" sheetId="15" r:id="rId20"/>
     <sheet name="SpellChanges" sheetId="17" r:id="rId21"/>
     <sheet name="Quest - Sea Creatures" sheetId="18" r:id="rId22"/>
+    <sheet name="SpellDamage" sheetId="27" r:id="rId23"/>
+    <sheet name="BlazingMountain" sheetId="29" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="708">
   <si>
     <t>In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
@@ -1610,12 +1612,591 @@
   <si>
     <t>Nelvin</t>
   </si>
+  <si>
+    <t>Fire Mountain 1 / Feuerberg 1</t>
+  </si>
+  <si>
+    <t>First level of the fire mountain dungeon</t>
+  </si>
+  <si>
+    <t>Max L-P to 65</t>
+  </si>
+  <si>
+    <t>Max F-T to 90</t>
+  </si>
+  <si>
+    <t>Max D-T to 90</t>
+  </si>
+  <si>
+    <t>Hero</t>
+  </si>
+  <si>
+    <t>TP/Lvl to 7</t>
+  </si>
+  <si>
+    <t>Each level increases the spell damage by 1% so at max level 50 you have +50% damage.</t>
+  </si>
+  <si>
+    <t>INT changes the damage by (INT-50)/5 in percent.</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Elements grant a damage bonus or malus as well now.</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Attacker \ Defender</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Spirit</t>
+  </si>
+  <si>
+    <t>Undead</t>
+  </si>
+  <si>
+    <t>Mental</t>
+  </si>
+  <si>
+    <t>Values are total damage percentage. A value of 0 means immunity against a spell of that element.</t>
+  </si>
+  <si>
+    <t>All above values are added together as a total percentage bonus or malus with the exception of element immunity where the spell is aborted with a message instead.</t>
+  </si>
+  <si>
+    <t>If a target has multiple elements, any immunity will immediately abort the spell. If no immunity exists, the elemental factor is always 100% regardless of the elements.</t>
+  </si>
+  <si>
+    <t>LP Stealer</t>
+  </si>
+  <si>
+    <t>SP Stealer</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Dispell Undead</t>
+  </si>
+  <si>
+    <t>Destroy Undead</t>
+  </si>
+  <si>
+    <t>Holy Word</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>This is only controlled by the undead monster flag</t>
+  </si>
+  <si>
+    <t>Ghost Weapon</t>
+  </si>
+  <si>
+    <t>The following damaging spells exist</t>
+  </si>
+  <si>
+    <t>This one is special. It has it's own formula.</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Does 150% damage against physical and undead enemies, otherwise 100%.</t>
+  </si>
+  <si>
+    <t>Magic Projectile</t>
+  </si>
+  <si>
+    <t>Magic Arrows</t>
+  </si>
+  <si>
+    <t>Earth spells</t>
+  </si>
+  <si>
+    <t>Wind spells</t>
+  </si>
+  <si>
+    <t>Fire spells</t>
+  </si>
+  <si>
+    <t>Water spells</t>
+  </si>
+  <si>
+    <t>150% against water, 50% against wind, 75% against undead.</t>
+  </si>
+  <si>
+    <t>150% against earth, 50% against fire, 75% against undead.</t>
+  </si>
+  <si>
+    <t>150% against wind, 50% against water, 75% against spirit, 125% against undead.</t>
+  </si>
+  <si>
+    <t>150% against fire, 50% against earth, 75% against undead.</t>
+  </si>
+  <si>
+    <t>In original it steals the character level as damage but at max the remaining LP of the target.</t>
+  </si>
+  <si>
+    <t>Now it will steal the character level plus INT/4.</t>
+  </si>
+  <si>
+    <t>Same as LP stealer.</t>
+  </si>
+  <si>
+    <t>Code changes (example is AM2_CPU german).</t>
+  </si>
+  <si>
+    <t>At 0023f192 there is the function to calculate the spell damage for the main 4 elemental types.</t>
+  </si>
+  <si>
+    <t>The spell damage values are located at 0026d390. One word for min and one word for max damage.</t>
+  </si>
+  <si>
+    <t>At 0023f1c0 a random word is multiplied by the damage range (max value - min value) and then swapped.</t>
+  </si>
+  <si>
+    <t>This essentially is a modulo so that the random value is inside the given range.</t>
+  </si>
+  <si>
+    <t>And then the min damage is added to that value.</t>
+  </si>
+  <si>
+    <t>These operations take 6 bytes which is the same amount we need for a JMP instruction. So we replace them.</t>
+  </si>
+  <si>
+    <t>Those instructions must be preserved so we have to copy them over to the new function: c0 c1 48 40 d0 52.</t>
+  </si>
+  <si>
+    <t>In asm this is:</t>
+  </si>
+  <si>
+    <t>mulu.w D1w,D0</t>
+  </si>
+  <si>
+    <t>swap D0</t>
+  </si>
+  <si>
+    <t>add.w (A2),D0w</t>
+  </si>
+  <si>
+    <t>The new function should look like this:</t>
+  </si>
+  <si>
+    <t>D0w now has the total base damage.</t>
+  </si>
+  <si>
+    <t>We add a table with damage factors from above as byte values.</t>
+  </si>
+  <si>
+    <t>moveq 0,D2</t>
+  </si>
+  <si>
+    <t>jsr FUN_00243b4e.l</t>
+  </si>
+  <si>
+    <t>Get pointer to current caster</t>
+  </si>
+  <si>
+    <t>(INT-50)/5</t>
+  </si>
+  <si>
+    <t>move.w (0x32,A1),D2w</t>
+  </si>
+  <si>
+    <t>add.w (0x36,A1),D2w</t>
+  </si>
+  <si>
+    <t>Move caster's total INT to D2</t>
+  </si>
+  <si>
+    <t>subi.w 50,D2w</t>
+  </si>
+  <si>
+    <t>ext.l D2</t>
+  </si>
+  <si>
+    <t>divs.w 5,D2w</t>
+  </si>
+  <si>
+    <t>move.b (0x5,A1),D1b</t>
+  </si>
+  <si>
+    <t>Move caster level to D1</t>
+  </si>
+  <si>
+    <t>moveq 0,D1</t>
+  </si>
+  <si>
+    <t>add.w D1w,D2w</t>
+  </si>
+  <si>
+    <t>Add level and INT factor together</t>
+  </si>
+  <si>
+    <t>lea (DAT_0026be70).l,A1</t>
+  </si>
+  <si>
+    <t>mulu.w #0x1e,D1</t>
+  </si>
+  <si>
+    <t>add.w (DAT_0027b75c).l,D1w</t>
+  </si>
+  <si>
+    <t>subq.w #0x1,D1w</t>
+  </si>
+  <si>
+    <t>mulu.w #0x5,D1</t>
+  </si>
+  <si>
+    <t>adda.w D1w,A1</t>
+  </si>
+  <si>
+    <t>Pointer to spell info</t>
+  </si>
+  <si>
+    <t>move.b (0x4,A1),D1b</t>
+  </si>
+  <si>
+    <t>Element is now in D1b</t>
+  </si>
+  <si>
+    <t>If no element, don't change the damage value (as it is 100%)</t>
+  </si>
+  <si>
+    <t>END:</t>
+  </si>
+  <si>
+    <t>rts</t>
+  </si>
+  <si>
+    <t>movem.l { A1, D2, D1 },-(SP)</t>
+  </si>
+  <si>
+    <t>movem.l (SP)+, { A1, D2, D1 }</t>
+  </si>
+  <si>
+    <t>andi.b #0x1,D1b</t>
+  </si>
+  <si>
+    <t>NEXT:</t>
+  </si>
+  <si>
+    <t>beq.b END</t>
+  </si>
+  <si>
+    <t>movem.l { D7, D1 },-(SP)</t>
+  </si>
+  <si>
+    <t>movem.l (SP)+, { D7, D1 }</t>
+  </si>
+  <si>
+    <t>moveq 0, D7</t>
+  </si>
+  <si>
+    <t>bne.b DONE</t>
+  </si>
+  <si>
+    <t>addi.b 1,D7b</t>
+  </si>
+  <si>
+    <t>bra.b NEXT</t>
+  </si>
+  <si>
+    <t>DONE:</t>
+  </si>
+  <si>
+    <t>D7 now holds the 0-based index of the first set element bit (starting from bit 0). This is the row in the element table.</t>
+  </si>
+  <si>
+    <t>We don't need to check for the index as the 8 bits always contain at least one set bit, otherwise the function would not have been called at all.</t>
+  </si>
+  <si>
+    <t>Multiply by 8 to get the row offset.</t>
+  </si>
+  <si>
+    <t>jsr FUN_00243b8c.l</t>
+  </si>
+  <si>
+    <t>movea.l D0,A1</t>
+  </si>
+  <si>
+    <t>move.w (SP)+,D0w</t>
+  </si>
+  <si>
+    <t>move.w D0w,-(SP)</t>
+  </si>
+  <si>
+    <t>jsr CALCELEMDMG</t>
+  </si>
+  <si>
+    <t>// CALCELEMDMG</t>
+  </si>
+  <si>
+    <t>Otherwise set the damage to 1.</t>
+  </si>
+  <si>
+    <t>EXIT:</t>
+  </si>
+  <si>
+    <t>and.l #0xffff,D0</t>
+  </si>
+  <si>
+    <t>Ensure the upper word is 0.</t>
+  </si>
+  <si>
+    <t>Base damage * Damage percentage</t>
+  </si>
+  <si>
+    <t>Result / 100 to get the real value</t>
+  </si>
+  <si>
+    <t>movem.l { D7, D1, D0 },-(SP)</t>
+  </si>
+  <si>
+    <t>movem.l (SP)+, { D7, D1, D0 }</t>
+  </si>
+  <si>
+    <t>move.b D1b,D0b</t>
+  </si>
+  <si>
+    <t>move.b (0x5,A0),D0b</t>
+  </si>
+  <si>
+    <t>Get pointer to target</t>
+  </si>
+  <si>
+    <t>move.b DAT_0027b4de,D0b</t>
+  </si>
+  <si>
+    <t>Release pointer</t>
+  </si>
+  <si>
+    <t>move.b (0x13,A1),D0b</t>
+  </si>
+  <si>
+    <t>// GETELEMINDEX (D0=Elem)</t>
+  </si>
+  <si>
+    <t>move.b D0b,D1b</t>
+  </si>
+  <si>
+    <t>lsr.b #0x1,D0b</t>
+  </si>
+  <si>
+    <t>move.l D7,D0</t>
+  </si>
+  <si>
+    <t>Input is D1=Element, Output is D2=Factor</t>
+  </si>
+  <si>
+    <t>jsr.l GETELEMINDEX</t>
+  </si>
+  <si>
+    <t>lsl.w 3,D0w</t>
+  </si>
+  <si>
+    <t>Store our index for later</t>
+  </si>
+  <si>
+    <t>move.w D0b,D1b</t>
+  </si>
+  <si>
+    <t>Store target element in D0b</t>
+  </si>
+  <si>
+    <t>D0b now stores the element index</t>
+  </si>
+  <si>
+    <t>add.b D1b,D0b</t>
+  </si>
+  <si>
+    <t>Add the row offset to get the total index</t>
+  </si>
+  <si>
+    <t>and.b 0x3f,D0b</t>
+  </si>
+  <si>
+    <t>Ensure index is inside range for safety</t>
+  </si>
+  <si>
+    <t>lea (DAT_Elems),A1</t>
+  </si>
+  <si>
+    <t>Load element table into A1</t>
+  </si>
+  <si>
+    <t>move.b (0x0,A1,D0b*0x1),D0b</t>
+  </si>
+  <si>
+    <t>Store element bonus percentage value to D0b</t>
+  </si>
+  <si>
+    <t>ext.w D0w</t>
+  </si>
+  <si>
+    <t>add.w D0w,D2w</t>
+  </si>
+  <si>
+    <t>Add element bonus to D2 (which was the bonus before)</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>48 e7 60 40</t>
+  </si>
+  <si>
+    <t>c0 c1</t>
+  </si>
+  <si>
+    <t>48 40</t>
+  </si>
+  <si>
+    <t>d0 52</t>
+  </si>
+  <si>
+    <t>3f 00</t>
+  </si>
+  <si>
+    <t>10 39 XX XX XX XX</t>
+  </si>
+  <si>
+    <t>4e b9 XX XX XX XX</t>
+  </si>
+  <si>
+    <t>22 40</t>
+  </si>
+  <si>
+    <t>30 1f</t>
+  </si>
+  <si>
+    <t>74 00</t>
+  </si>
+  <si>
+    <t>34 29 00 32</t>
+  </si>
+  <si>
+    <t>d4 69 00 36</t>
+  </si>
+  <si>
+    <t>04 42 00 32</t>
+  </si>
+  <si>
+    <t>48 c2</t>
+  </si>
+  <si>
+    <t>85 fc 00 05</t>
+  </si>
+  <si>
+    <t>72 00</t>
+  </si>
+  <si>
+    <t>12 29 00 05</t>
+  </si>
+  <si>
+    <t>d4 41</t>
+  </si>
+  <si>
+    <t>43 f9 XX XX XX XX</t>
+  </si>
+  <si>
+    <t>c2 fc 00 1e</t>
+  </si>
+  <si>
+    <t>c2 7c XX XX XX XX</t>
+  </si>
+  <si>
+    <t>53 41</t>
+  </si>
+  <si>
+    <t>c2 fc 00 05</t>
+  </si>
+  <si>
+    <t>d2 c1</t>
+  </si>
+  <si>
+    <t>12 29 00 04</t>
+  </si>
+  <si>
+    <t>67 06</t>
+  </si>
+  <si>
+    <t>c1 c2</t>
+  </si>
+  <si>
+    <t>muls.w D2,D0</t>
+  </si>
+  <si>
+    <t>divs.w 100,D0</t>
+  </si>
+  <si>
+    <t>If the resulting dmg &gt; 0, then go to exit, damage in D0w.</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>81 fc 00 64</t>
+  </si>
+  <si>
+    <t>bgt.s EXIT</t>
+  </si>
+  <si>
+    <t>6e 02</t>
+  </si>
+  <si>
+    <t>moveq.l 1,D0</t>
+  </si>
+  <si>
+    <t>70 01</t>
+  </si>
+  <si>
+    <t>New Maps</t>
+  </si>
+  <si>
+    <t>Tileset/Labdata</t>
+  </si>
+  <si>
+    <t>36 (new)</t>
+  </si>
+  <si>
+    <t>Feuerberg - 2 / Blazing Mountain - 2</t>
+  </si>
+  <si>
+    <t>Feuerberg - 1 / Blazing Mountain - 1</t>
+  </si>
+  <si>
+    <t>Palette</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="\+0&quot;%&quot;;\-0&quot;%&quot;;&quot;No change&quot;"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1640,6 +2221,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1670,7 +2258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -2033,12 +2621,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2093,6 +2705,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -2115,6 +2729,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -2416,10 +3069,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD8B38F-295E-46BA-A316-56C9E4745E5F}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,16 +3083,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="28" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2651,6 +3304,20 @@
       </c>
       <c r="D16" t="s">
         <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>464</v>
+      </c>
+      <c r="B17" t="s">
+        <v>516</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -2877,8 +3544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D8139E-327A-4885-8257-94E3A09DB943}">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3815,8 +4482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC23CFDD-BBD1-493E-8BC8-E0E0F16426DA}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3872,31 +4539,31 @@
       <c r="B4" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="44" t="s">
         <v>490</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="42" t="s">
         <v>488</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="33" t="s">
         <v>501</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="34" t="s">
         <v>502</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="33" t="s">
         <v>503</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="34" t="s">
         <v>504</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="33" t="s">
         <v>505</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="N4" s="48" t="s">
         <v>506</v>
       </c>
     </row>
@@ -3907,36 +4574,36 @@
       <c r="B5" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="45" t="s">
         <v>491</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="32">
         <v>75</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="36">
         <v>75</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="35">
         <f>50*F5</f>
         <v>3750</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="36">
         <f>50*G5</f>
         <v>3750</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="35">
         <f>325*F5</f>
         <v>24375</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="36">
         <f>325*G5</f>
         <v>24375</v>
       </c>
-      <c r="M5" s="33">
+      <c r="M5" s="35">
         <f>1250*F5</f>
         <v>93750</v>
       </c>
-      <c r="N5" s="47">
+      <c r="N5" s="49">
         <f>1250*G5</f>
         <v>93750</v>
       </c>
@@ -3948,36 +4615,36 @@
       <c r="B6" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="45" t="s">
         <v>492</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="32">
         <v>150</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="40">
         <v>110</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="35">
         <f t="shared" ref="I6:I14" si="0">50*F6</f>
         <v>7500</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="36">
         <f t="shared" ref="J6:J14" si="1">50*G6</f>
         <v>5500</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="35">
         <f t="shared" ref="K6:K14" si="2">325*F6</f>
         <v>48750</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6" s="36">
         <f t="shared" ref="L6:L14" si="3">325*G6</f>
         <v>35750</v>
       </c>
-      <c r="M6" s="33">
+      <c r="M6" s="35">
         <f t="shared" ref="M6:M14" si="4">1250*F6</f>
         <v>187500</v>
       </c>
-      <c r="N6" s="47">
+      <c r="N6" s="49">
         <f t="shared" ref="N6:N14" si="5">1250*G6</f>
         <v>137500</v>
       </c>
@@ -3989,36 +4656,36 @@
       <c r="B7" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="45" t="s">
         <v>493</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="32">
         <v>180</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="40">
         <v>155</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="35">
         <f t="shared" si="0"/>
         <v>9000</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="36">
         <f t="shared" si="1"/>
         <v>7750</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="35">
         <f t="shared" si="2"/>
         <v>58500</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L7" s="36">
         <f t="shared" si="3"/>
         <v>50375</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="35">
         <f t="shared" si="4"/>
         <v>225000</v>
       </c>
-      <c r="N7" s="47">
+      <c r="N7" s="49">
         <f t="shared" si="5"/>
         <v>193750</v>
       </c>
@@ -4030,36 +4697,36 @@
       <c r="B8" t="s">
         <v>120</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="46" t="s">
         <v>494</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="32">
         <v>100</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="40">
         <v>85</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="35">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="36">
         <f t="shared" si="1"/>
         <v>4250</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="35">
         <f t="shared" si="2"/>
         <v>32500</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L8" s="36">
         <f t="shared" si="3"/>
         <v>27625</v>
       </c>
-      <c r="M8" s="33">
+      <c r="M8" s="35">
         <f t="shared" si="4"/>
         <v>125000</v>
       </c>
-      <c r="N8" s="47">
+      <c r="N8" s="49">
         <f t="shared" si="5"/>
         <v>106250</v>
       </c>
@@ -4071,36 +4738,36 @@
       <c r="B9" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="46" t="s">
         <v>495</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="32">
         <v>125</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="36">
         <v>125</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="35">
         <f t="shared" si="0"/>
         <v>6250</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="36">
         <f t="shared" si="1"/>
         <v>6250</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K9" s="35">
         <f t="shared" si="2"/>
         <v>40625</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="36">
         <f t="shared" si="3"/>
         <v>40625</v>
       </c>
-      <c r="M9" s="33">
+      <c r="M9" s="35">
         <f t="shared" si="4"/>
         <v>156250</v>
       </c>
-      <c r="N9" s="47">
+      <c r="N9" s="49">
         <f t="shared" si="5"/>
         <v>156250</v>
       </c>
@@ -4112,36 +4779,36 @@
       <c r="B10" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="46" t="s">
         <v>496</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="32">
         <v>90</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="36">
         <v>90</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="35">
         <f t="shared" si="0"/>
         <v>4500</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="36">
         <f t="shared" si="1"/>
         <v>4500</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="35">
         <f t="shared" si="2"/>
         <v>29250</v>
       </c>
-      <c r="L10" s="34">
+      <c r="L10" s="36">
         <f t="shared" si="3"/>
         <v>29250</v>
       </c>
-      <c r="M10" s="33">
+      <c r="M10" s="35">
         <f t="shared" si="4"/>
         <v>112500</v>
       </c>
-      <c r="N10" s="47">
+      <c r="N10" s="49">
         <f t="shared" si="5"/>
         <v>112500</v>
       </c>
@@ -4153,36 +4820,36 @@
       <c r="B11" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="46" t="s">
         <v>497</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="32">
         <v>90</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="40">
         <v>85</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="35">
         <f t="shared" si="0"/>
         <v>4500</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="36">
         <f t="shared" si="1"/>
         <v>4250</v>
       </c>
-      <c r="K11" s="33">
+      <c r="K11" s="35">
         <f t="shared" si="2"/>
         <v>29250</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="36">
         <f t="shared" si="3"/>
         <v>27625</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="35">
         <f t="shared" si="4"/>
         <v>112500</v>
       </c>
-      <c r="N11" s="47">
+      <c r="N11" s="49">
         <f t="shared" si="5"/>
         <v>106250</v>
       </c>
@@ -4194,36 +4861,36 @@
       <c r="B12" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="46" t="s">
         <v>498</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="32">
         <v>90</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="40">
         <v>80</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="35">
         <f t="shared" si="0"/>
         <v>4500</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="36">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="K12" s="33">
+      <c r="K12" s="35">
         <f t="shared" si="2"/>
         <v>29250</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L12" s="36">
         <f t="shared" si="3"/>
         <v>26000</v>
       </c>
-      <c r="M12" s="33">
+      <c r="M12" s="35">
         <f t="shared" si="4"/>
         <v>112500</v>
       </c>
-      <c r="N12" s="47">
+      <c r="N12" s="49">
         <f t="shared" si="5"/>
         <v>100000</v>
       </c>
@@ -4235,36 +4902,36 @@
       <c r="B13" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="46" t="s">
         <v>499</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="32">
         <v>95</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="36">
         <v>95</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="35">
         <f t="shared" si="0"/>
         <v>4750</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="36">
         <f t="shared" si="1"/>
         <v>4750</v>
       </c>
-      <c r="K13" s="33">
+      <c r="K13" s="35">
         <f t="shared" si="2"/>
         <v>30875</v>
       </c>
-      <c r="L13" s="34">
+      <c r="L13" s="36">
         <f t="shared" si="3"/>
         <v>30875</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="35">
         <f t="shared" si="4"/>
         <v>118750</v>
       </c>
-      <c r="N13" s="47">
+      <c r="N13" s="49">
         <f t="shared" si="5"/>
         <v>118750</v>
       </c>
@@ -4276,36 +4943,36 @@
       <c r="B14" t="s">
         <v>127</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="47" t="s">
         <v>500</v>
       </c>
-      <c r="F14" s="41">
+      <c r="F14" s="43">
         <v>32767</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="38">
         <v>32767</v>
       </c>
-      <c r="I14" s="35">
+      <c r="I14" s="37">
         <f t="shared" si="0"/>
         <v>1638350</v>
       </c>
-      <c r="J14" s="36">
+      <c r="J14" s="38">
         <f t="shared" si="1"/>
         <v>1638350</v>
       </c>
-      <c r="K14" s="35">
+      <c r="K14" s="37">
         <f t="shared" si="2"/>
         <v>10649275</v>
       </c>
-      <c r="L14" s="36">
+      <c r="L14" s="38">
         <f t="shared" si="3"/>
         <v>10649275</v>
       </c>
-      <c r="M14" s="35">
+      <c r="M14" s="37">
         <f t="shared" si="4"/>
         <v>40958750</v>
       </c>
-      <c r="N14" s="48">
+      <c r="N14" s="50">
         <f t="shared" si="5"/>
         <v>40958750</v>
       </c>
@@ -4326,295 +4993,319 @@
         <v>485</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E17" s="31" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>512</v>
+      </c>
+      <c r="B17" t="s">
+        <v>518</v>
+      </c>
+      <c r="E17" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="39" t="s">
         <v>509</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="39" t="s">
         <v>510</v>
       </c>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="39" t="s">
         <v>508</v>
       </c>
-      <c r="I17" s="37" t="s">
+      <c r="I17" s="39" t="s">
         <v>507</v>
       </c>
-      <c r="J17" s="37" t="s">
+      <c r="J17" s="39" t="s">
         <v>513</v>
       </c>
-      <c r="K17" s="32" t="s">
+      <c r="K17" s="34" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E18" s="33" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>512</v>
+      </c>
+      <c r="B18" t="s">
+        <v>519</v>
+      </c>
+      <c r="E18" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="30">
         <v>75</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="30">
         <v>75</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="30">
         <f t="shared" ref="H18:H20" si="6">IF(MOD(ROUNDDOWN(SQRT(2*F18/J18),0),2)=0,ROUNDDOWN(SQRT(2*F18/J18),0),ROUNDDOWN(-0.5+SQRT(0.25+2*F18/J18),0))</f>
         <v>1</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="30">
         <f t="shared" ref="I18:I20" si="7">IF(MOD(ROUNDDOWN(SQRT(2*G18/K18),0),2)=0,ROUNDDOWN(SQRT(2*G18/K18),0),ROUNDDOWN(-0.5+SQRT(0.25+2*G18/K18),0))</f>
         <v>1</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="30">
         <f>F5</f>
         <v>75</v>
       </c>
-      <c r="K18" s="34">
+      <c r="K18" s="36">
         <f>G5</f>
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="33" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>512</v>
+      </c>
+      <c r="B19" t="s">
+        <v>520</v>
+      </c>
+      <c r="E19" s="35" t="s">
         <v>511</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="30">
         <v>59850</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="30">
         <v>59850</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="30">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="30">
         <f t="shared" si="7"/>
         <v>35</v>
       </c>
-      <c r="J19" s="28">
+      <c r="J19" s="30">
         <f>F13</f>
         <v>95</v>
       </c>
-      <c r="K19" s="34">
+      <c r="K19" s="36">
         <f>G13</f>
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="33" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>521</v>
+      </c>
+      <c r="B20" t="s">
+        <v>522</v>
+      </c>
+      <c r="E20" s="35" t="s">
         <v>484</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="30">
         <v>150</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="31">
         <v>110</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H20" s="30">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="30">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J20" s="30">
         <f>F6</f>
         <v>150</v>
       </c>
-      <c r="K20" s="34">
+      <c r="K20" s="36">
         <f>G6</f>
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="33" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E21" s="35" t="s">
         <v>512</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="30">
         <v>600</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="31">
         <v>550</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="30">
         <f>IF(MOD(ROUNDDOWN(SQRT(2*F21/J21),0),2)=0,ROUNDDOWN(SQRT(2*F21/J21),0),ROUNDDOWN(-0.5+SQRT(0.25+2*F21/J21),0))</f>
         <v>3</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="30">
         <f>IF(MOD(ROUNDDOWN(SQRT(2*G21/K21),0),2)=0,ROUNDDOWN(SQRT(2*G21/K21),0),ROUNDDOWN(-0.5+SQRT(0.25+2*G21/K21),0))</f>
         <v>3</v>
       </c>
-      <c r="J21" s="28">
+      <c r="J21" s="30">
         <f>F8</f>
         <v>100</v>
       </c>
-      <c r="K21" s="34">
+      <c r="K21" s="36">
         <f>G8</f>
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="33" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="30">
         <v>950</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="30">
         <v>950</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H22" s="30">
         <f t="shared" ref="H19:H27" si="8">ROUNDDOWN(-0.5+SQRT(0.25+2*F22/J22),0)</f>
         <v>4</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="30">
         <f t="shared" ref="I19:I27" si="9">ROUNDDOWN(-0.5+SQRT(0.25+2*G22/K22),0)</f>
         <v>4</v>
       </c>
-      <c r="J22" s="28">
+      <c r="J22" s="30">
         <f>F13</f>
         <v>95</v>
       </c>
-      <c r="K22" s="34">
+      <c r="K22" s="36">
         <f>G13</f>
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="33" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="30">
         <v>1890</v>
       </c>
-      <c r="G23" s="28">
+      <c r="G23" s="30">
         <v>1890</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="30">
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="30">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="J23" s="28">
+      <c r="J23" s="30">
         <f>F10</f>
         <v>90</v>
       </c>
-      <c r="K23" s="34">
+      <c r="K23" s="36">
         <f>G10</f>
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="33" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="30">
         <v>4500</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="30">
         <v>4500</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="30">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="30">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="30">
         <f>F9</f>
         <v>125</v>
       </c>
-      <c r="K24" s="34">
+      <c r="K24" s="36">
         <f>G9</f>
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="33" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="30">
         <v>12240</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="31">
         <v>11500</v>
       </c>
-      <c r="H25" s="28">
+      <c r="H25" s="30">
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="I25" s="28">
+      <c r="I25" s="30">
         <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="J25" s="28">
+      <c r="J25" s="30">
         <f>F12</f>
         <v>90</v>
       </c>
-      <c r="K25" s="34">
+      <c r="K25" s="36">
         <f>G12</f>
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="33" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E26" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="30">
         <v>29250</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="31">
         <v>28750</v>
       </c>
-      <c r="H26" s="28">
+      <c r="H26" s="30">
         <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="I26" s="28">
+      <c r="I26" s="30">
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="J26" s="28">
+      <c r="J26" s="30">
         <f>F11</f>
         <v>90</v>
       </c>
-      <c r="K26" s="34">
+      <c r="K26" s="36">
         <f>G11</f>
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="35" t="s">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="39">
+      <c r="F27" s="41">
         <v>113400</v>
       </c>
-      <c r="G27" s="49">
+      <c r="G27" s="51">
         <v>100000</v>
       </c>
-      <c r="H27" s="39">
+      <c r="H27" s="41">
         <f t="shared" si="8"/>
         <v>35</v>
       </c>
-      <c r="I27" s="39">
+      <c r="I27" s="41">
         <f t="shared" si="9"/>
         <v>35</v>
       </c>
-      <c r="J27" s="39">
+      <c r="J27" s="41">
         <f>F7</f>
         <v>180</v>
       </c>
-      <c r="K27" s="36">
+      <c r="K27" s="38">
         <f>G7</f>
         <v>155</v>
       </c>
@@ -5478,6 +6169,1428 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E14A00-C10C-40A3-8CD1-A30440ECE4D7}">
+  <dimension ref="A1:K150"/>
+  <sheetViews>
+    <sheetView topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H108" sqref="H108"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>525</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
+        <v>0</v>
+      </c>
+      <c r="B5" s="54">
+        <f>ROUNDDOWN((A5-50)/5,0)</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
+        <v>25</v>
+      </c>
+      <c r="B6" s="54">
+        <f t="shared" ref="B6:B11" si="0">ROUNDDOWN((A6-50)/5,0)</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>50</v>
+      </c>
+      <c r="B7" s="54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>75</v>
+      </c>
+      <c r="B8" s="54">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
+        <v>100</v>
+      </c>
+      <c r="B9" s="54">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
+        <v>125</v>
+      </c>
+      <c r="B10" s="54">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="37">
+        <v>150</v>
+      </c>
+      <c r="B11" s="55">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>529</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>536</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>534</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>535</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>530</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>531</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>532</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>536</v>
+      </c>
+      <c r="B16" s="30">
+        <v>0</v>
+      </c>
+      <c r="C16" s="30">
+        <v>100</v>
+      </c>
+      <c r="D16" s="30">
+        <v>100</v>
+      </c>
+      <c r="E16" s="30">
+        <v>100</v>
+      </c>
+      <c r="F16" s="30">
+        <v>100</v>
+      </c>
+      <c r="G16" s="30">
+        <v>100</v>
+      </c>
+      <c r="H16" s="30">
+        <v>100</v>
+      </c>
+      <c r="I16" s="36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>534</v>
+      </c>
+      <c r="B17" s="30">
+        <v>100</v>
+      </c>
+      <c r="C17" s="30">
+        <v>0</v>
+      </c>
+      <c r="D17" s="30">
+        <v>150</v>
+      </c>
+      <c r="E17" s="30">
+        <v>150</v>
+      </c>
+      <c r="F17" s="30">
+        <v>100</v>
+      </c>
+      <c r="G17" s="30">
+        <v>100</v>
+      </c>
+      <c r="H17" s="30">
+        <v>100</v>
+      </c>
+      <c r="I17" s="36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>528</v>
+      </c>
+      <c r="B18" s="30">
+        <v>100</v>
+      </c>
+      <c r="C18" s="30">
+        <v>100</v>
+      </c>
+      <c r="D18" s="30">
+        <v>0</v>
+      </c>
+      <c r="E18" s="30">
+        <v>100</v>
+      </c>
+      <c r="F18" s="30">
+        <v>100</v>
+      </c>
+      <c r="G18" s="30">
+        <v>100</v>
+      </c>
+      <c r="H18" s="30">
+        <v>100</v>
+      </c>
+      <c r="I18" s="36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>535</v>
+      </c>
+      <c r="B19" s="30">
+        <v>100</v>
+      </c>
+      <c r="C19" s="30">
+        <v>100</v>
+      </c>
+      <c r="D19" s="30">
+        <v>100</v>
+      </c>
+      <c r="E19" s="30">
+        <v>0</v>
+      </c>
+      <c r="F19" s="30">
+        <v>100</v>
+      </c>
+      <c r="G19" s="30">
+        <v>100</v>
+      </c>
+      <c r="H19" s="30">
+        <v>100</v>
+      </c>
+      <c r="I19" s="36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>530</v>
+      </c>
+      <c r="B20" s="30">
+        <v>100</v>
+      </c>
+      <c r="C20" s="30">
+        <v>100</v>
+      </c>
+      <c r="D20" s="30">
+        <v>100</v>
+      </c>
+      <c r="E20" s="30">
+        <v>75</v>
+      </c>
+      <c r="F20" s="30">
+        <v>0</v>
+      </c>
+      <c r="G20" s="30">
+        <v>50</v>
+      </c>
+      <c r="H20" s="30">
+        <v>100</v>
+      </c>
+      <c r="I20" s="36">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>531</v>
+      </c>
+      <c r="B21" s="30">
+        <v>100</v>
+      </c>
+      <c r="C21" s="30">
+        <v>100</v>
+      </c>
+      <c r="D21" s="30">
+        <v>100</v>
+      </c>
+      <c r="E21" s="30">
+        <v>75</v>
+      </c>
+      <c r="F21" s="30">
+        <v>150</v>
+      </c>
+      <c r="G21" s="30">
+        <v>0</v>
+      </c>
+      <c r="H21" s="30">
+        <v>50</v>
+      </c>
+      <c r="I21" s="36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>532</v>
+      </c>
+      <c r="B22" s="30">
+        <v>100</v>
+      </c>
+      <c r="C22" s="30">
+        <v>75</v>
+      </c>
+      <c r="D22" s="30">
+        <v>100</v>
+      </c>
+      <c r="E22" s="30">
+        <v>125</v>
+      </c>
+      <c r="F22" s="30">
+        <v>100</v>
+      </c>
+      <c r="G22" s="30">
+        <v>150</v>
+      </c>
+      <c r="H22" s="30">
+        <v>0</v>
+      </c>
+      <c r="I22" s="36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="57" t="s">
+        <v>533</v>
+      </c>
+      <c r="B23" s="41">
+        <v>100</v>
+      </c>
+      <c r="C23" s="41">
+        <v>100</v>
+      </c>
+      <c r="D23" s="41">
+        <v>100</v>
+      </c>
+      <c r="E23" s="41">
+        <v>75</v>
+      </c>
+      <c r="F23" s="41">
+        <v>50</v>
+      </c>
+      <c r="G23" s="41">
+        <v>100</v>
+      </c>
+      <c r="H23" s="41">
+        <v>150</v>
+      </c>
+      <c r="I23" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>542</v>
+      </c>
+      <c r="C32" s="58" t="s">
+        <v>551</v>
+      </c>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>546</v>
+      </c>
+      <c r="C33" s="60" t="s">
+        <v>547</v>
+      </c>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="62"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>544</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>546</v>
+      </c>
+      <c r="C34" s="60" t="s">
+        <v>547</v>
+      </c>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="62"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>545</v>
+      </c>
+      <c r="B35" s="49" t="s">
+        <v>546</v>
+      </c>
+      <c r="C35" s="60" t="s">
+        <v>547</v>
+      </c>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="62"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>548</v>
+      </c>
+      <c r="B36" s="49" t="s">
+        <v>534</v>
+      </c>
+      <c r="C36" s="64" t="s">
+        <v>552</v>
+      </c>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>540</v>
+      </c>
+      <c r="B37" s="49" t="s">
+        <v>535</v>
+      </c>
+      <c r="C37" s="63" t="s">
+        <v>550</v>
+      </c>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>541</v>
+      </c>
+      <c r="B38" s="49" t="s">
+        <v>534</v>
+      </c>
+      <c r="C38" s="63" t="s">
+        <v>550</v>
+      </c>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>553</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>534</v>
+      </c>
+      <c r="C39" s="64" t="s">
+        <v>552</v>
+      </c>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>554</v>
+      </c>
+      <c r="B40" s="49" t="s">
+        <v>534</v>
+      </c>
+      <c r="C40" s="64" t="s">
+        <v>552</v>
+      </c>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>555</v>
+      </c>
+      <c r="B41" s="49" t="s">
+        <v>530</v>
+      </c>
+      <c r="C41" s="64" t="s">
+        <v>559</v>
+      </c>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>556</v>
+      </c>
+      <c r="B42" s="49" t="s">
+        <v>531</v>
+      </c>
+      <c r="C42" s="64" t="s">
+        <v>560</v>
+      </c>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>557</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>532</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>561</v>
+      </c>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
+        <v>558</v>
+      </c>
+      <c r="B44" s="49" t="s">
+        <v>533</v>
+      </c>
+      <c r="C44" s="64" t="s">
+        <v>562</v>
+      </c>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="59"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="59"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="59"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="59"/>
+      <c r="H47" s="59"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="65" t="s">
+        <v>540</v>
+      </c>
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="65"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="59" t="s">
+        <v>563</v>
+      </c>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="59"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="65" t="s">
+        <v>541</v>
+      </c>
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65"/>
+      <c r="G52" s="65"/>
+      <c r="H52" s="65"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="65" t="s">
+        <v>566</v>
+      </c>
+      <c r="B57" s="65"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="65"/>
+      <c r="F57" s="65"/>
+      <c r="G57" s="65"/>
+      <c r="H57" s="65"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="66" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="66" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="66" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H73" s="65" t="s">
+        <v>665</v>
+      </c>
+      <c r="I73" s="65"/>
+      <c r="J73" s="65"/>
+      <c r="K73" s="65"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="66" t="s">
+        <v>608</v>
+      </c>
+      <c r="H74" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="66" t="s">
+        <v>575</v>
+      </c>
+      <c r="H75" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="66" t="s">
+        <v>576</v>
+      </c>
+      <c r="H76" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="66" t="s">
+        <v>577</v>
+      </c>
+      <c r="C77" t="s">
+        <v>579</v>
+      </c>
+      <c r="H77" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="66" t="s">
+        <v>626</v>
+      </c>
+      <c r="H78" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="66" t="s">
+        <v>640</v>
+      </c>
+      <c r="H79" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="66" t="s">
+        <v>582</v>
+      </c>
+      <c r="H80" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="66" t="s">
+        <v>624</v>
+      </c>
+      <c r="C81" t="s">
+        <v>583</v>
+      </c>
+      <c r="H81" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="66" t="s">
+        <v>640</v>
+      </c>
+      <c r="H82" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="66" t="s">
+        <v>623</v>
+      </c>
+      <c r="H83" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="66" t="s">
+        <v>625</v>
+      </c>
+      <c r="H84" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="66" t="s">
+        <v>581</v>
+      </c>
+      <c r="H85" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="66" t="s">
+        <v>585</v>
+      </c>
+      <c r="H86" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="66" t="s">
+        <v>586</v>
+      </c>
+      <c r="C87" t="s">
+        <v>587</v>
+      </c>
+      <c r="H87" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="66" t="s">
+        <v>588</v>
+      </c>
+      <c r="H88" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="66" t="s">
+        <v>589</v>
+      </c>
+      <c r="H89" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="66" t="s">
+        <v>590</v>
+      </c>
+      <c r="C90" t="s">
+        <v>584</v>
+      </c>
+      <c r="H90" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="66" t="s">
+        <v>593</v>
+      </c>
+      <c r="H91" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="66" t="s">
+        <v>591</v>
+      </c>
+      <c r="C92" t="s">
+        <v>592</v>
+      </c>
+      <c r="H92" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="66" t="s">
+        <v>594</v>
+      </c>
+      <c r="C93" t="s">
+        <v>595</v>
+      </c>
+      <c r="H93" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="66" t="s">
+        <v>596</v>
+      </c>
+      <c r="H94" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="66" t="s">
+        <v>597</v>
+      </c>
+      <c r="H95" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="66" t="s">
+        <v>598</v>
+      </c>
+      <c r="H96" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="66" t="s">
+        <v>599</v>
+      </c>
+      <c r="H97" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="66" t="s">
+        <v>600</v>
+      </c>
+      <c r="H98" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="66" t="s">
+        <v>601</v>
+      </c>
+      <c r="C99" t="s">
+        <v>602</v>
+      </c>
+      <c r="H99" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="66" t="s">
+        <v>603</v>
+      </c>
+      <c r="C100" t="s">
+        <v>604</v>
+      </c>
+      <c r="H100" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="66" t="s">
+        <v>612</v>
+      </c>
+      <c r="C101" t="s">
+        <v>605</v>
+      </c>
+      <c r="H101" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="66" t="s">
+        <v>627</v>
+      </c>
+      <c r="C102" t="s">
+        <v>647</v>
+      </c>
+      <c r="H102" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="66" t="s">
+        <v>606</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="66" t="s">
+        <v>693</v>
+      </c>
+      <c r="C104" t="s">
+        <v>633</v>
+      </c>
+      <c r="H104" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="66" t="s">
+        <v>694</v>
+      </c>
+      <c r="C105" t="s">
+        <v>634</v>
+      </c>
+      <c r="H105" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="66" t="s">
+        <v>698</v>
+      </c>
+      <c r="C106" t="s">
+        <v>695</v>
+      </c>
+      <c r="H106" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="66" t="s">
+        <v>700</v>
+      </c>
+      <c r="C107" t="s">
+        <v>629</v>
+      </c>
+      <c r="H107" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="66" t="s">
+        <v>630</v>
+      </c>
+      <c r="H108" s="13" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="66" t="s">
+        <v>631</v>
+      </c>
+      <c r="C109" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="66" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="66" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="66" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="66" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="66" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="66" t="s">
+        <v>648</v>
+      </c>
+      <c r="C117" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="66" t="s">
+        <v>649</v>
+      </c>
+      <c r="C118" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="66" t="s">
+        <v>651</v>
+      </c>
+      <c r="C119" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="66" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="66" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="66" t="s">
+        <v>624</v>
+      </c>
+      <c r="C122" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="66" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="66" t="s">
+        <v>623</v>
+      </c>
+      <c r="C124" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="66" t="s">
+        <v>642</v>
+      </c>
+      <c r="C125" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="66" t="s">
+        <v>648</v>
+      </c>
+      <c r="C126" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="66" t="s">
+        <v>654</v>
+      </c>
+      <c r="C127" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="66" t="s">
+        <v>656</v>
+      </c>
+      <c r="C128" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="66" t="s">
+        <v>658</v>
+      </c>
+      <c r="C129" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="66" t="s">
+        <v>660</v>
+      </c>
+      <c r="C130" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="66" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="66" t="s">
+        <v>663</v>
+      </c>
+      <c r="C132" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="66" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="66" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="66"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="66"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="66" t="s">
+        <v>613</v>
+      </c>
+      <c r="C138" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="66" t="s">
+        <v>615</v>
+      </c>
+      <c r="C139" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="66" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="66" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="66" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="66" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="66" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="66" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="66" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="66" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="66" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="66" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="66" t="s">
+        <v>607</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A52:H52"/>
+    <mergeCell ref="A57:H57"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C37:H37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409CD694-F799-4E97-A2FE-008BA8288F2C}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>702</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>703</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="30">
+        <v>464</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>706</v>
+      </c>
+      <c r="D3" s="30">
+        <v>7</v>
+      </c>
+      <c r="E3" s="30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>465</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>705</v>
+      </c>
+      <c r="D4" s="67" t="s">
+        <v>704</v>
+      </c>
+      <c r="E4" s="30">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fixed lead class condition code, multi cursor condition code, extended lab data for next paladin guild level
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="856">
   <si>
     <t xml:space="preserve">Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Exp well</t>
   </si>
   <si>
-    <t xml:space="preserve">Crashes on game exit</t>
+    <t xml:space="preserve">Crashes on game exit (1.14 english does too!)</t>
   </si>
   <si>
     <t xml:space="preserve">More events, rewards, actions, conditions</t>
@@ -1689,6 +1689,15 @@
   </si>
   <si>
     <t xml:space="preserve">2Overlay3D.amb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paladin guild left door pillar overlay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paladin guild 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paladin guild right door pillar overlay</t>
   </si>
   <si>
     <t xml:space="preserve">Tileset Graphics (Icon Gfx)</t>
@@ -3270,10 +3279,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A14 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3299,10 +3308,10 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="A14 D26"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -3680,10 +3689,10 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="1" sqref="A14 E42"/>
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -3773,10 +3782,10 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="A14 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -3995,10 +4004,10 @@
   <dimension ref="A1:A43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="1" sqref="A14 G18"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4199,10 +4208,10 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M31" activeCellId="1" sqref="A14 M31"/>
+      <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -4409,10 +4418,10 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D46" activeCellId="1" sqref="A14 D46"/>
+      <selection pane="topLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83"/>
@@ -5032,10 +5041,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="A14 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -5099,10 +5108,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A14 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
@@ -5150,10 +5159,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A14 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5179,10 +5188,10 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="A14 B21"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -6027,11 +6036,11 @@
   </sheetPr>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6207,10 +6216,10 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T39" activeCellId="1" sqref="A14 T39"/>
+      <selection pane="topLeft" activeCell="T39" activeCellId="0" sqref="T39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -6337,11 +6346,11 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="A14 C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -6418,8 +6427,33 @@
         <v>544</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>544</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6440,10 +6474,10 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="1" sqref="A14 K8"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -6451,19 +6485,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>132</v>
@@ -6472,7 +6506,7 @@
         <v>128</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>132</v>
@@ -6489,7 +6523,7 @@
         <v>1193</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>4</v>
@@ -6498,7 +6532,7 @@
         <v>1167</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6509,7 +6543,7 @@
         <v>1194</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>4</v>
@@ -6518,7 +6552,7 @@
         <v>1168</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6529,7 +6563,7 @@
         <v>1195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>4</v>
@@ -6538,7 +6572,7 @@
         <v>1169</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6549,7 +6583,7 @@
         <v>1196</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>4</v>
@@ -6558,7 +6592,7 @@
         <v>1170</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6569,7 +6603,7 @@
         <v>1197</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>4</v>
@@ -6578,7 +6612,7 @@
         <v>1171</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6589,7 +6623,7 @@
         <v>1198</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>4</v>
@@ -6598,7 +6632,7 @@
         <v>1172</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6609,7 +6643,7 @@
         <v>1199</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -6618,7 +6652,7 @@
         <v>1173</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6629,7 +6663,7 @@
         <v>1200</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>4</v>
@@ -6638,7 +6672,7 @@
         <v>1174</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -6664,10 +6698,10 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A14 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -6676,426 +6710,426 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D2" s="43"/>
       <c r="E2" s="44"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="E3" s="45"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -7120,42 +7154,42 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A14 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>
@@ -7177,10 +7211,10 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="1" sqref="A14 A57"/>
+      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -7188,21 +7222,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="46" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7270,42 +7304,42 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="50" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="B16" s="34" t="n">
         <v>0</v>
@@ -7334,7 +7368,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="50" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="B17" s="34" t="n">
         <v>100</v>
@@ -7363,7 +7397,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="50" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="B18" s="34" t="n">
         <v>100</v>
@@ -7392,7 +7426,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="50" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="B19" s="34" t="n">
         <v>100</v>
@@ -7421,7 +7455,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="50" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B20" s="34" t="n">
         <v>100</v>
@@ -7450,7 +7484,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="50" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="B21" s="34" t="n">
         <v>100</v>
@@ -7479,7 +7513,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="50" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="B22" s="34" t="n">
         <v>100</v>
@@ -7508,7 +7542,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B23" s="36" t="n">
         <v>100</v>
@@ -7537,22 +7571,22 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7560,10 +7594,10 @@
         <v>133</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="D32" s="53"/>
       <c r="E32" s="53"/>
@@ -7573,13 +7607,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="34" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
@@ -7589,13 +7623,13 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="34" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="D34" s="54"/>
       <c r="E34" s="54"/>
@@ -7605,13 +7639,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="34" t="s">
+        <v>673</v>
+      </c>
+      <c r="B35" s="26" t="s">
         <v>670</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>667</v>
-      </c>
       <c r="C35" s="54" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="D35" s="54"/>
       <c r="E35" s="54"/>
@@ -7621,13 +7655,13 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="34" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="C36" s="55" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="D36" s="55"/>
       <c r="E36" s="55"/>
@@ -7637,13 +7671,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="34" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="D37" s="54"/>
       <c r="E37" s="54"/>
@@ -7653,13 +7687,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="34" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="D38" s="54"/>
       <c r="E38" s="54"/>
@@ -7669,13 +7703,13 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="34" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="D39" s="55"/>
       <c r="E39" s="55"/>
@@ -7685,13 +7719,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="34" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="D40" s="55"/>
       <c r="E40" s="55"/>
@@ -7701,13 +7735,13 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="34" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="D41" s="55"/>
       <c r="E41" s="55"/>
@@ -7717,13 +7751,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="34" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="D42" s="55"/>
       <c r="E42" s="55"/>
@@ -7733,13 +7767,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="34" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="C43" s="55" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
@@ -7749,13 +7783,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="34" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="C44" s="55" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="D44" s="55"/>
       <c r="E44" s="55"/>
@@ -7795,7 +7829,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="57" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="B48" s="57"/>
       <c r="C48" s="57"/>
@@ -7807,7 +7841,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="56" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="B49" s="56"/>
       <c r="C49" s="56"/>
@@ -7819,12 +7853,12 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="57" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="B52" s="57"/>
       <c r="C52" s="57"/>
@@ -7836,12 +7870,12 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="57" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="B57" s="57"/>
       <c r="C57" s="57"/>
@@ -7853,72 +7887,72 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="58" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="58" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="58" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H73" s="57" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="I73" s="57"/>
       <c r="J73" s="57"/>
@@ -7926,483 +7960,483 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="58" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="58" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="58" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="58" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="58" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="58" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="58" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="58" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="58" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="58" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="58" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="58" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="58" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="58" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="58" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="58" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="58" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="58" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="58" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="58" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="58" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="58" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="58" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="58" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="58" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="58" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="58" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="58" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="58" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="58" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="58" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="58" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="58" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="58" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="58" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="58" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="58" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="58" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="58" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="58" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="58" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="58" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="58" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="58" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="58" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="58" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="58" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="58" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="58" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="58" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="58" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="58" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="58" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="58" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="58" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="58" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="58" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="58" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="58" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8413,78 +8447,78 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="58" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="58" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="58" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="58" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="58" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="58" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="58" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="58" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="58" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="58" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="58" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="58" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="58" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>
@@ -8525,10 +8559,10 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="1" sqref="A14 I16"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -8536,7 +8570,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -8554,10 +8588,10 @@
         <v>133</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>826</v>
+        <v>829</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8568,7 +8602,7 @@
         <v>248</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c r="D3" s="34" t="n">
         <v>7</v>
@@ -8585,10 +8619,10 @@
         <v>255</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="E4" s="34" t="n">
         <v>6</v>
@@ -8602,10 +8636,10 @@
         <v>255</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="E5" s="61" t="n">
         <v>6</v>
@@ -8619,10 +8653,10 @@
         <v>248</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="E6" s="61" t="n">
         <v>1</v>
@@ -8650,34 +8684,34 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="A14 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
     </row>
   </sheetData>
@@ -8699,26 +8733,26 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="1" sqref="A14 I9"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="65" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
       <c r="D1" s="65"/>
       <c r="E1" s="65" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="F1" s="65"/>
       <c r="G1" s="65"/>
       <c r="H1" s="65"/>
       <c r="I1" s="65" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="J1" s="65"/>
       <c r="K1" s="65"/>
@@ -8734,10 +8768,10 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8745,10 +8779,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8756,10 +8790,10 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8767,25 +8801,25 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="1" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I7" s="0" t="s">
-        <v>851</v>
+      <c r="I7" s="1" t="s">
+        <v>854</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I8" s="0" t="s">
-        <v>852</v>
+      <c r="I8" s="1" t="s">
+        <v>855</v>
       </c>
     </row>
   </sheetData>
@@ -8812,10 +8846,10 @@
   <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="1" sqref="A14 A43"/>
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -9045,10 +9079,10 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="A14 A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -9153,10 +9187,10 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="A14 A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -9256,10 +9290,10 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="1" sqref="A14 E26"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -9410,10 +9444,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="A14 C16"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -9481,10 +9515,10 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="1" sqref="A14 F22"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -10022,10 +10056,10 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="1" sqref="A14 L15"/>
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Added paladin guild level 2
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -6036,8 +6036,8 @@
   </sheetPr>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6346,8 +6346,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added entrance to wine cellar on world map and some details
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="857">
   <si>
     <t xml:space="preserve">Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">Disable spells on map 465. Jumps should not be possible.</t>
   </si>
   <si>
-    <t xml:space="preserve">Disallow scrolls when magic is disabled.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chests</t>
   </si>
   <si>
@@ -127,24 +124,15 @@
     <t xml:space="preserve">Add more details to wine cellar</t>
   </si>
   <si>
-    <t xml:space="preserve">Fix teleports in wine cellar</t>
-  </si>
-  <si>
     <t xml:space="preserve">Add monsters to wine cellar</t>
   </si>
   <si>
-    <t xml:space="preserve">Automap for secondary paladin guild 1 map should have explored parts of the dark map (inner circle)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Add monsters to paladin guild</t>
   </si>
   <si>
     <t xml:space="preserve">Add event for altair in paladin guild</t>
   </si>
   <si>
-    <t xml:space="preserve">Fix teleport to paladin guild 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
   <si>
@@ -268,6 +256,12 @@
     <t xml:space="preserve">259: Ignited all candles in paladin guild</t>
   </si>
   <si>
+    <t xml:space="preserve">260: Opened entrance to Crystal wine cellar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">261: Opened exit from paladin guild to world map</t>
+  </si>
+  <si>
     <t xml:space="preserve">In Original all keywords from 0 to 114 are used.</t>
   </si>
   <si>
@@ -671,6 +665,12 @@
   </si>
   <si>
     <t xml:space="preserve">Can be sold (Quest maybe?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gildenschlüssel / Guild Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key for the paladin guild door</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1445,7 +1445,10 @@
     <t xml:space="preserve">Second gate keeper door</t>
   </si>
   <si>
-    <t xml:space="preserve">Manyeyes' upper boos door</t>
+    <t xml:space="preserve">Manyeyes' upper boss door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paladin guild locked door</t>
   </si>
   <si>
     <t xml:space="preserve">Text</t>
@@ -3282,7 +3285,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3308,10 +3311,10 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -3320,16 +3323,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3692,7 +3695,7 @@
       <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -3785,7 +3788,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -3793,13 +3796,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4007,7 +4010,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4211,7 +4214,7 @@
       <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -4219,16 +4222,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>360</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4421,7 +4424,7 @@
       <selection pane="topLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83"/>
@@ -4431,7 +4434,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>360</v>
@@ -4455,13 +4458,13 @@
         <v>393</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>360</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4687,7 +4690,7 @@
         <v>423</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>424</v>
@@ -5038,13 +5041,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -5054,7 +5057,7 @@
         <v>459</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5087,6 +5090,14 @@
       </c>
       <c r="B5" s="1" t="s">
         <v>463</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -5111,33 +5122,33 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -5162,11 +5173,11 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -5191,7 +5202,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -5207,80 +5218,80 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="F5" s="23" t="n">
         <v>75</v>
@@ -5315,13 +5326,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F6" s="23" t="n">
         <v>150</v>
@@ -5356,13 +5367,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F7" s="23" t="n">
         <v>180</v>
@@ -5397,13 +5408,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F8" s="23" t="n">
         <v>100</v>
@@ -5438,13 +5449,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F9" s="23" t="n">
         <v>125</v>
@@ -5479,13 +5490,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F10" s="23" t="n">
         <v>90</v>
@@ -5520,13 +5531,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F11" s="23" t="n">
         <v>90</v>
@@ -5561,13 +5572,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F12" s="23" t="n">
         <v>90</v>
@@ -5602,13 +5613,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F13" s="23" t="n">
         <v>95</v>
@@ -5643,13 +5654,13 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F14" s="29" t="n">
         <v>32767</v>
@@ -5684,58 +5695,58 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G17" s="33" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="I17" s="33" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="F18" s="34" t="n">
         <v>75</v>
@@ -5762,13 +5773,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="F19" s="34" t="n">
         <v>59850</v>
@@ -5795,13 +5806,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F20" s="34" t="n">
         <v>150</v>
@@ -5828,7 +5839,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="25" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F21" s="34" t="n">
         <v>600</v>
@@ -5855,7 +5866,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="25" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="F22" s="34" t="n">
         <v>950</v>
@@ -5882,7 +5893,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="25" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F23" s="34" t="n">
         <v>1890</v>
@@ -5909,7 +5920,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="25" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F24" s="34" t="n">
         <v>4500</v>
@@ -5936,7 +5947,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="25" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F25" s="34" t="n">
         <v>12240</v>
@@ -5963,7 +5974,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="25" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F26" s="34" t="n">
         <v>29250</v>
@@ -5990,7 +6001,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="31" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F27" s="36" t="n">
         <v>113400</v>
@@ -6036,11 +6047,11 @@
   </sheetPr>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6068,134 +6079,122 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6219,7 +6218,7 @@
       <selection pane="topLeft" activeCell="T39" activeCellId="0" sqref="T39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -6228,19 +6227,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C1" s="39" t="s">
         <v>294</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6248,16 +6247,16 @@
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6265,16 +6264,16 @@
         <v>153</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6282,16 +6281,16 @@
         <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6299,16 +6298,16 @@
         <v>154</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6316,16 +6315,16 @@
         <v>374</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -6350,7 +6349,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -6359,16 +6358,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>294</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6376,13 +6375,13 @@
         <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>297</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6390,13 +6389,13 @@
         <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>297</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,13 +6403,13 @@
         <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>297</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6418,13 +6417,13 @@
         <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6432,13 +6431,13 @@
         <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6446,13 +6445,13 @@
         <v>97</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>546</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -6477,7 +6476,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -6485,34 +6484,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6523,7 +6522,7 @@
         <v>1193</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>4</v>
@@ -6532,7 +6531,7 @@
         <v>1167</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6543,7 +6542,7 @@
         <v>1194</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>4</v>
@@ -6552,7 +6551,7 @@
         <v>1168</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6563,7 +6562,7 @@
         <v>1195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>4</v>
@@ -6572,7 +6571,7 @@
         <v>1169</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6583,7 +6582,7 @@
         <v>1196</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>4</v>
@@ -6592,7 +6591,7 @@
         <v>1170</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6603,7 +6602,7 @@
         <v>1197</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>4</v>
@@ -6612,7 +6611,7 @@
         <v>1171</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6623,7 +6622,7 @@
         <v>1198</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>4</v>
@@ -6632,7 +6631,7 @@
         <v>1172</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6643,7 +6642,7 @@
         <v>1199</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -6652,7 +6651,7 @@
         <v>1173</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6663,7 +6662,7 @@
         <v>1200</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>4</v>
@@ -6672,7 +6671,7 @@
         <v>1174</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -6701,7 +6700,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -6710,426 +6709,426 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D2" s="43"/>
       <c r="E2" s="44"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E3" s="45"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -7157,39 +7156,39 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -7214,7 +7213,7 @@
       <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -7222,21 +7221,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="46" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7304,42 +7303,42 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="50" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B16" s="34" t="n">
         <v>0</v>
@@ -7368,7 +7367,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="50" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B17" s="34" t="n">
         <v>100</v>
@@ -7397,7 +7396,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="50" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B18" s="34" t="n">
         <v>100</v>
@@ -7426,7 +7425,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="50" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B19" s="34" t="n">
         <v>100</v>
@@ -7455,7 +7454,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="50" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B20" s="34" t="n">
         <v>100</v>
@@ -7484,7 +7483,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="50" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B21" s="34" t="n">
         <v>100</v>
@@ -7513,7 +7512,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="50" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B22" s="34" t="n">
         <v>100</v>
@@ -7542,7 +7541,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B23" s="36" t="n">
         <v>100</v>
@@ -7571,33 +7570,33 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D32" s="53"/>
       <c r="E32" s="53"/>
@@ -7607,13 +7606,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="34" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
@@ -7623,13 +7622,13 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="34" t="s">
+        <v>673</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>671</v>
+      </c>
+      <c r="C34" s="54" t="s">
         <v>672</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>670</v>
-      </c>
-      <c r="C34" s="54" t="s">
-        <v>671</v>
       </c>
       <c r="D34" s="54"/>
       <c r="E34" s="54"/>
@@ -7639,13 +7638,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="34" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D35" s="54"/>
       <c r="E35" s="54"/>
@@ -7655,13 +7654,13 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="34" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C36" s="55" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D36" s="55"/>
       <c r="E36" s="55"/>
@@ -7671,13 +7670,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="34" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D37" s="54"/>
       <c r="E37" s="54"/>
@@ -7687,13 +7686,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="34" t="s">
+        <v>679</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>657</v>
+      </c>
+      <c r="C38" s="54" t="s">
         <v>678</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>656</v>
-      </c>
-      <c r="C38" s="54" t="s">
-        <v>677</v>
       </c>
       <c r="D38" s="54"/>
       <c r="E38" s="54"/>
@@ -7703,13 +7702,13 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="34" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D39" s="55"/>
       <c r="E39" s="55"/>
@@ -7719,13 +7718,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="34" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D40" s="55"/>
       <c r="E40" s="55"/>
@@ -7735,13 +7734,13 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="34" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="D41" s="55"/>
       <c r="E41" s="55"/>
@@ -7751,13 +7750,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="34" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D42" s="55"/>
       <c r="E42" s="55"/>
@@ -7767,13 +7766,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="34" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C43" s="55" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
@@ -7783,13 +7782,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="34" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C44" s="55" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D44" s="55"/>
       <c r="E44" s="55"/>
@@ -7829,7 +7828,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="57" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B48" s="57"/>
       <c r="C48" s="57"/>
@@ -7841,7 +7840,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="56" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B49" s="56"/>
       <c r="C49" s="56"/>
@@ -7853,12 +7852,12 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="57" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B52" s="57"/>
       <c r="C52" s="57"/>
@@ -7870,12 +7869,12 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="57" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B57" s="57"/>
       <c r="C57" s="57"/>
@@ -7887,72 +7886,72 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="58" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="58" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="58" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H73" s="57" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="I73" s="57"/>
       <c r="J73" s="57"/>
@@ -7960,483 +7959,483 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="58" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="58" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="58" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="58" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="58" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="58" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="58" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="58" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="58" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="58" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="58" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="58" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="58" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="58" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="58" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="58" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="58" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="58" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="58" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="58" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="58" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="58" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="58" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="58" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="58" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="58" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="58" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="58" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="58" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="58" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="58" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="58" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="58" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="58" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="58" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="58" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="58" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="58" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="58" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="58" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="58" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="58" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="58" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="58" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="58" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="58" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="58" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="58" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="58" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="58" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="58" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="58" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="58" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="58" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="58" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="58" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="58" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="58" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="58" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8447,78 +8446,78 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="58" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="58" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="58" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="58" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="58" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="58" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="58" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="58" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="58" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="58" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="58" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="58" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="58" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
   </sheetData>
@@ -8562,7 +8561,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -8570,7 +8569,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -8582,16 +8581,16 @@
         <v>208</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8602,7 +8601,7 @@
         <v>248</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D3" s="34" t="n">
         <v>7</v>
@@ -8619,10 +8618,10 @@
         <v>255</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="E4" s="34" t="n">
         <v>6</v>
@@ -8636,10 +8635,10 @@
         <v>255</v>
       </c>
       <c r="C5" s="63" t="s">
+        <v>835</v>
+      </c>
+      <c r="D5" s="60" t="s">
         <v>834</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>833</v>
       </c>
       <c r="E5" s="61" t="n">
         <v>6</v>
@@ -8653,10 +8652,10 @@
         <v>248</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="E6" s="61" t="n">
         <v>1</v>
@@ -8687,31 +8686,31 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
   </sheetData>
@@ -8736,23 +8735,23 @@
       <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="65" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
       <c r="D1" s="65"/>
       <c r="E1" s="65" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="F1" s="65"/>
       <c r="G1" s="65"/>
       <c r="H1" s="65"/>
       <c r="I1" s="65" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J1" s="65"/>
       <c r="K1" s="65"/>
@@ -8768,10 +8767,10 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8779,10 +8778,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8790,10 +8789,10 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8801,25 +8800,25 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="1" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I7" s="1" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I8" s="1" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
   </sheetData>
@@ -8843,221 +8842,231 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A42"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -9082,90 +9091,90 @@
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -9190,85 +9199,85 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -9293,7 +9302,7 @@
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -9301,13 +9310,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9315,10 +9324,10 @@
         <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9326,10 +9335,10 @@
         <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9337,10 +9346,10 @@
         <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9348,10 +9357,10 @@
         <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9359,10 +9368,10 @@
         <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9370,10 +9379,10 @@
         <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9381,10 +9390,10 @@
         <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9392,15 +9401,15 @@
         <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9408,10 +9417,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9419,10 +9428,10 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -9447,20 +9456,20 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9471,7 +9480,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9482,7 +9491,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9493,7 +9502,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -9512,13 +9521,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -9528,19 +9537,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -9550,22 +9559,22 @@
         <v>403</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9573,22 +9582,22 @@
         <v>404</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>249</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9596,22 +9605,22 @@
         <v>405</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>251</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9619,13 +9628,13 @@
         <v>406</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9633,13 +9642,13 @@
         <v>407</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9647,13 +9656,13 @@
         <v>408</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9661,13 +9670,13 @@
         <v>409</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9675,13 +9684,13 @@
         <v>410</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9689,13 +9698,13 @@
         <v>411</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9703,13 +9712,13 @@
         <v>412</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9717,13 +9726,13 @@
         <v>413</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9731,13 +9740,13 @@
         <v>414</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9745,13 +9754,13 @@
         <v>415</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9759,16 +9768,16 @@
         <v>416</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -9778,19 +9787,19 @@
         <v>417</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9798,19 +9807,19 @@
         <v>418</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>188</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9818,19 +9827,19 @@
         <v>419</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>189</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9838,19 +9847,19 @@
         <v>420</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>190</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9858,16 +9867,16 @@
         <v>421</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>191</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9875,16 +9884,16 @@
         <v>422</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>192</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9892,10 +9901,10 @@
         <v>423</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9903,10 +9912,10 @@
         <v>424</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9914,10 +9923,10 @@
         <v>425</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9925,10 +9934,10 @@
         <v>426</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9936,10 +9945,10 @@
         <v>427</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9947,10 +9956,10 @@
         <v>428</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9958,10 +9967,10 @@
         <v>429</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9969,10 +9978,10 @@
         <v>430</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9980,10 +9989,10 @@
         <v>431</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9991,10 +10000,10 @@
         <v>432</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10002,10 +10011,10 @@
         <v>433</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10013,10 +10022,10 @@
         <v>434</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10024,12 +10033,26 @@
         <v>435</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>436</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>207</v>
       </c>
     </row>
@@ -10059,7 +10082,7 @@
       <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>
@@ -10074,19 +10097,19 @@
         <v>208</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>209</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>210</v>
@@ -10117,10 +10140,10 @@
         <v>208</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added new party member prototype
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="858">
   <si>
     <t xml:space="preserve">Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -2583,6 +2583,9 @@
   </si>
   <si>
     <t xml:space="preserve">Add new merchants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add new party member</t>
   </si>
   <si>
     <t xml:space="preserve">New Events</t>
@@ -4211,7 +4214,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6047,7 +6050,7 @@
   </sheetPr>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -8680,10 +8683,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8711,6 +8714,11 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>842</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -8739,19 +8747,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="65" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
       <c r="D1" s="65"/>
       <c r="E1" s="65" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="F1" s="65"/>
       <c r="G1" s="65"/>
       <c r="H1" s="65"/>
       <c r="I1" s="65" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="J1" s="65"/>
       <c r="K1" s="65"/>
@@ -8767,10 +8775,10 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8778,10 +8786,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8789,10 +8797,10 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8800,25 +8808,25 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="1" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I7" s="1" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I8" s="1" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -8845,7 +8853,7 @@
   <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Reworked firestaff, added paladin master event
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Finish lava stream map</t>
   </si>
   <si>
-    <t xml:space="preserve">Make map music dependent on world surface flag and not travel type flag! Check if this is possible.</t>
+    <t xml:space="preserve">?Make map music dependent on world surface flag and not travel type flag! Check if this is possible.</t>
   </si>
   <si>
     <t xml:space="preserve">Teleporters must be larger</t>
@@ -6287,8 +6287,8 @@
   </sheetPr>
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9850,7 +9850,7 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added monsters to wine cellar
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -118,9 +118,6 @@
     <t xml:space="preserve">Add more details to wine cellar</t>
   </si>
   <si>
-    <t xml:space="preserve">Add monsters to wine cellar</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remove animal class for most items</t>
   </si>
   <si>
@@ -971,6 +968,9 @@
   </si>
   <si>
     <t xml:space="preserve">4x Untoter Paladin (v2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x Höhlenspinne, 2x Gr. Giftspinne</t>
   </si>
   <si>
     <t xml:space="preserve">Architektenbüro / Architect's Office</t>
@@ -3527,7 +3527,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3539,16 +3539,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4012,13 +4012,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4438,16 +4438,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>409</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4636,7 +4636,7 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -4650,7 +4650,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>409</v>
@@ -4674,13 +4674,13 @@
         <v>442</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>409</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4906,7 +4906,7 @@
         <v>472</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>473</v>
@@ -5328,7 +5328,7 @@
         <v>514</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6318,8 +6318,8 @@
   </sheetPr>
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6444,9 +6444,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
@@ -6458,48 +6456,48 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6541,7 +6539,7 @@
         <v>582</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1" s="39" t="s">
         <v>343</v>
@@ -6672,7 +6670,7 @@
         <v>582</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>343</v>
@@ -6810,19 +6808,19 @@
         <v>606</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>606</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7901,7 +7899,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B32" s="52" t="s">
         <v>723</v>
@@ -8889,13 +8887,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D2" s="59" t="s">
         <v>885</v>
@@ -9182,258 +9180,258 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -9465,83 +9463,83 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -9573,78 +9571,78 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -9677,13 +9675,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9691,10 +9689,10 @@
         <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9702,10 +9700,10 @@
         <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9713,10 +9711,10 @@
         <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9724,10 +9722,10 @@
         <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9735,10 +9733,10 @@
         <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9746,10 +9744,10 @@
         <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9757,10 +9755,10 @@
         <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9768,15 +9766,15 @@
         <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9784,10 +9782,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9795,10 +9793,10 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -9830,13 +9828,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9847,7 +9845,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9858,7 +9856,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9869,7 +9867,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -9891,7 +9889,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9904,19 +9902,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -9926,22 +9924,22 @@
         <v>403</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9949,22 +9947,22 @@
         <v>404</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>249</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9972,22 +9970,22 @@
         <v>405</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>251</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9995,13 +9993,13 @@
         <v>406</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10009,13 +10007,13 @@
         <v>407</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10023,13 +10021,13 @@
         <v>408</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10037,13 +10035,13 @@
         <v>409</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10051,13 +10049,13 @@
         <v>410</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10065,13 +10063,13 @@
         <v>411</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10079,13 +10077,13 @@
         <v>412</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10093,13 +10091,13 @@
         <v>413</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10107,13 +10105,13 @@
         <v>414</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10121,13 +10119,13 @@
         <v>415</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10135,16 +10133,16 @@
         <v>416</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -10154,19 +10152,19 @@
         <v>417</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10174,19 +10172,19 @@
         <v>418</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>188</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10194,19 +10192,19 @@
         <v>419</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>189</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10214,19 +10212,19 @@
         <v>420</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>190</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10234,16 +10232,16 @@
         <v>421</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>191</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10251,16 +10249,16 @@
         <v>422</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>192</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10268,16 +10266,16 @@
         <v>423</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>193</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10285,16 +10283,16 @@
         <v>424</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>194</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10302,16 +10300,16 @@
         <v>425</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>195</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10319,16 +10317,16 @@
         <v>426</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F25" s="1" t="n">
         <v>196</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10336,16 +10334,16 @@
         <v>427</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>197</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10353,16 +10351,16 @@
         <v>428</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>198</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10370,16 +10368,16 @@
         <v>429</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>199</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10387,16 +10385,16 @@
         <v>430</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>200</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10404,10 +10402,10 @@
         <v>431</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10415,10 +10413,10 @@
         <v>432</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10426,10 +10424,10 @@
         <v>433</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10437,10 +10435,10 @@
         <v>434</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10448,13 +10446,13 @@
         <v>435</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10462,13 +10460,13 @@
         <v>436</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10476,13 +10474,13 @@
         <v>437</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10490,10 +10488,10 @@
         <v>438</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10501,10 +10499,10 @@
         <v>439</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10512,10 +10510,10 @@
         <v>440</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10523,10 +10521,10 @@
         <v>441</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10534,10 +10532,10 @@
         <v>442</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10545,10 +10543,10 @@
         <v>443</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10556,13 +10554,13 @@
         <v>444</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10570,13 +10568,13 @@
         <v>445</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10584,13 +10582,13 @@
         <v>446</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10598,13 +10596,13 @@
         <v>447</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10612,13 +10610,13 @@
         <v>448</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10626,13 +10624,13 @@
         <v>449</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -10655,10 +10653,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10674,25 +10672,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -10702,28 +10700,28 @@
         <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>87</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10731,25 +10729,25 @@
         <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>88</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N3" s="1" t="n">
         <v>19</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10757,25 +10755,25 @@
         <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>89</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>21</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10783,16 +10781,16 @@
         <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>90</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10800,16 +10798,16 @@
         <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>91</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10817,16 +10815,16 @@
         <v>62</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>92</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10834,16 +10832,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>93</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10851,16 +10849,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>94</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10868,16 +10866,16 @@
         <v>65</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>95</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10885,16 +10883,16 @@
         <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>96</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10902,16 +10900,16 @@
         <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>97</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10919,16 +10917,16 @@
         <v>68</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>98</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10936,16 +10934,16 @@
         <v>69</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>99</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10953,16 +10951,16 @@
         <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>114</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10970,16 +10968,16 @@
         <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>115</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10987,16 +10985,16 @@
         <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>116</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11004,7 +11002,7 @@
         <v>117</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11012,7 +11010,7 @@
         <v>118</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11020,7 +11018,7 @@
         <v>119</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11028,7 +11026,7 @@
         <v>120</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11036,6 +11034,14 @@
         <v>121</v>
       </c>
       <c r="I22" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H23" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>295</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extended tileset for lavastream map
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="911">
   <si>
     <t xml:space="preserve">Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -1073,6 +1073,12 @@
   </si>
   <si>
     <t xml:space="preserve">Paladin Guild 2 / Paladingilde 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beneath the sands / Unter  dem Sand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desert temple underground</t>
   </si>
   <si>
     <t xml:space="preserve">New labdata</t>
@@ -3516,10 +3522,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3879,6 +3885,20 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>292</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>473</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -3914,19 +3934,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3934,16 +3954,16 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3951,16 +3971,16 @@
         <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3971,7 +3991,7 @@
         <v>303</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -4018,10 +4038,10 @@
         <v>157</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4029,10 +4049,10 @@
         <v>198</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4040,10 +4060,10 @@
         <v>257</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4051,10 +4071,10 @@
         <v>258</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4062,10 +4082,10 @@
         <v>259</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4073,10 +4093,10 @@
         <v>262</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4084,10 +4104,10 @@
         <v>263</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4095,10 +4115,10 @@
         <v>273</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4106,10 +4126,10 @@
         <v>421</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4117,10 +4137,10 @@
         <v>77</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4128,10 +4148,10 @@
         <v>112</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4139,10 +4159,10 @@
         <v>135</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4150,10 +4170,10 @@
         <v>139</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4161,10 +4181,10 @@
         <v>244</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4172,10 +4192,10 @@
         <v>163</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4222,182 +4242,182 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -4436,7 +4456,7 @@
         <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>123</v>
@@ -4447,13 +4467,13 @@
         <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4461,13 +4481,13 @@
         <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4475,10 +4495,10 @@
         <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4486,10 +4506,10 @@
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4497,13 +4517,13 @@
         <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4511,13 +4531,13 @@
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4525,13 +4545,13 @@
         <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4539,13 +4559,13 @@
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4553,13 +4573,13 @@
         <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>417</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4567,19 +4587,19 @@
         <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L20" s="13" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
@@ -4590,10 +4610,10 @@
         <v>11</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4601,10 +4621,10 @@
         <v>19</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -4645,13 +4665,13 @@
         <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="F1" s="4"/>
     </row>
@@ -4660,16 +4680,16 @@
         <v>132</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>133</v>
@@ -4680,19 +4700,19 @@
         <v>133</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4700,19 +4720,19 @@
         <v>134</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4720,19 +4740,19 @@
         <v>135</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>124</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4740,19 +4760,19 @@
         <v>136</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>84</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4760,19 +4780,19 @@
         <v>137</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4780,19 +4800,19 @@
         <v>138</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>104</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4800,10 +4820,10 @@
         <v>139</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4811,10 +4831,10 @@
         <v>140</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4822,10 +4842,10 @@
         <v>141</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4833,10 +4853,10 @@
         <v>142</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4844,10 +4864,10 @@
         <v>143</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4855,10 +4875,10 @@
         <v>144</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4866,10 +4886,10 @@
         <v>145</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4877,13 +4897,13 @@
         <v>146</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="F16" s="4"/>
     </row>
@@ -4892,22 +4912,22 @@
         <v>147</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>127</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4915,10 +4935,10 @@
         <v>148</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4926,10 +4946,10 @@
         <v>149</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4937,10 +4957,10 @@
         <v>150</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4948,10 +4968,10 @@
         <v>151</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4959,10 +4979,10 @@
         <v>152</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4970,10 +4990,10 @@
         <v>153</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4981,10 +5001,10 @@
         <v>154</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4992,10 +5012,10 @@
         <v>155</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5003,10 +5023,10 @@
         <v>156</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5014,10 +5034,10 @@
         <v>157</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5025,10 +5045,10 @@
         <v>158</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5036,10 +5056,10 @@
         <v>159</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5047,10 +5067,10 @@
         <v>160</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,10 +5078,10 @@
         <v>161</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5069,10 +5089,10 @@
         <v>162</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5080,10 +5100,10 @@
         <v>163</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5091,10 +5111,10 @@
         <v>164</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5102,10 +5122,10 @@
         <v>165</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5113,10 +5133,10 @@
         <v>166</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5124,10 +5144,10 @@
         <v>167</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5135,10 +5155,10 @@
         <v>168</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5146,10 +5166,10 @@
         <v>169</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5157,10 +5177,10 @@
         <v>170</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5168,10 +5188,10 @@
         <v>171</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,10 +5199,10 @@
         <v>172</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5190,10 +5210,10 @@
         <v>173</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5201,10 +5221,10 @@
         <v>174</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5212,10 +5232,10 @@
         <v>175</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5223,10 +5243,10 @@
         <v>176</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,10 +5254,10 @@
         <v>177</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,10 +5265,10 @@
         <v>178</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5256,10 +5276,10 @@
         <v>179</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,10 +5287,10 @@
         <v>180</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5278,10 +5298,10 @@
         <v>181</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,10 +5309,10 @@
         <v>182</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -5328,7 +5348,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>123</v>
@@ -5339,7 +5359,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5347,7 +5367,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5355,7 +5375,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5363,7 +5383,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5371,7 +5391,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5379,7 +5399,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5387,7 +5407,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5395,7 +5415,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5403,7 +5423,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -5435,26 +5455,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -5483,7 +5503,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -5524,80 +5544,80 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>525</v>
-      </c>
       <c r="E5" s="23" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="F5" s="24" t="n">
         <v>75</v>
@@ -5632,13 +5652,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="F6" s="24" t="n">
         <v>150</v>
@@ -5673,13 +5693,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="F7" s="24" t="n">
         <v>180</v>
@@ -5714,13 +5734,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="F8" s="24" t="n">
         <v>100</v>
@@ -5755,13 +5775,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="F9" s="24" t="n">
         <v>125</v>
@@ -5796,13 +5816,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="F10" s="24" t="n">
         <v>90</v>
@@ -5837,13 +5857,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="F11" s="24" t="n">
         <v>90</v>
@@ -5878,13 +5898,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="F12" s="24" t="n">
         <v>90</v>
@@ -5919,13 +5939,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="F13" s="24" t="n">
         <v>95</v>
@@ -5960,13 +5980,13 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="F14" s="30" t="n">
         <v>32767</v>
@@ -6001,58 +6021,58 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F18" s="35" t="n">
         <v>75</v>
@@ -6079,13 +6099,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F19" s="35" t="n">
         <v>59850</v>
@@ -6112,13 +6132,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="F20" s="35" t="n">
         <v>150</v>
@@ -6145,7 +6165,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="26" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="F21" s="35" t="n">
         <v>600</v>
@@ -6172,7 +6192,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="26" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="F22" s="35" t="n">
         <v>950</v>
@@ -6199,7 +6219,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="26" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="F23" s="35" t="n">
         <v>1890</v>
@@ -6226,7 +6246,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="26" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="F24" s="35" t="n">
         <v>4500</v>
@@ -6253,7 +6273,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="26" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="F25" s="35" t="n">
         <v>12240</v>
@@ -6280,7 +6300,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="26" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F26" s="35" t="n">
         <v>29250</v>
@@ -6307,7 +6327,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="32" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="F27" s="37" t="n">
         <v>113400</v>
@@ -6353,7 +6373,7 @@
   </sheetPr>
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -6517,19 +6537,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="39" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>123</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6537,16 +6557,16 @@
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>299</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6554,16 +6574,16 @@
         <v>153</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>299</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6571,16 +6591,16 @@
         <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>299</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6588,16 +6608,16 @@
         <v>154</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>299</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6605,16 +6625,16 @@
         <v>374</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -6648,16 +6668,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>123</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6665,13 +6685,13 @@
         <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6679,13 +6699,13 @@
         <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6693,13 +6713,13 @@
         <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>591</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6707,13 +6727,13 @@
         <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6721,13 +6741,13 @@
         <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6735,13 +6755,13 @@
         <v>97</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -6774,19 +6794,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>127</v>
@@ -6795,7 +6815,7 @@
         <v>123</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>127</v>
@@ -6812,7 +6832,7 @@
         <v>1193</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>4</v>
@@ -6821,7 +6841,7 @@
         <v>1167</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6832,7 +6852,7 @@
         <v>1194</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>4</v>
@@ -6841,7 +6861,7 @@
         <v>1168</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6852,7 +6872,7 @@
         <v>1195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>4</v>
@@ -6861,7 +6881,7 @@
         <v>1169</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6872,7 +6892,7 @@
         <v>1196</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>4</v>
@@ -6881,7 +6901,7 @@
         <v>1170</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6892,7 +6912,7 @@
         <v>1197</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>4</v>
@@ -6901,7 +6921,7 @@
         <v>1171</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6912,7 +6932,7 @@
         <v>1198</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>4</v>
@@ -6921,7 +6941,7 @@
         <v>1172</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6932,7 +6952,7 @@
         <v>1199</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -6941,7 +6961,7 @@
         <v>1173</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6952,7 +6972,7 @@
         <v>1200</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>4</v>
@@ -6961,7 +6981,7 @@
         <v>1174</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
   </sheetData>
@@ -6999,426 +7019,426 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="42" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="D2" s="44"/>
       <c r="E2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="E3" s="46"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -7453,32 +7473,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -7511,21 +7531,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="47" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7593,42 +7613,42 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="B16" s="35" t="n">
         <v>0</v>
@@ -7657,7 +7677,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B17" s="35" t="n">
         <v>100</v>
@@ -7686,7 +7706,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B18" s="35" t="n">
         <v>100</v>
@@ -7715,7 +7735,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B19" s="35" t="n">
         <v>100</v>
@@ -7744,7 +7764,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B20" s="35" t="n">
         <v>100</v>
@@ -7773,7 +7793,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="51" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B21" s="35" t="n">
         <v>100</v>
@@ -7802,7 +7822,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B22" s="35" t="n">
         <v>100</v>
@@ -7831,7 +7851,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B23" s="37" t="n">
         <v>100</v>
@@ -7860,22 +7880,22 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7883,10 +7903,10 @@
         <v>128</v>
       </c>
       <c r="B32" s="53" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
@@ -7896,13 +7916,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="35" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C33" s="55" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="D33" s="55"/>
       <c r="E33" s="55"/>
@@ -7912,13 +7932,13 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="35" t="s">
+        <v>724</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>722</v>
       </c>
-      <c r="B34" s="27" t="s">
-        <v>720</v>
-      </c>
       <c r="C34" s="55" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="D34" s="55"/>
       <c r="E34" s="55"/>
@@ -7928,13 +7948,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="35" t="s">
+        <v>725</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>722</v>
+      </c>
+      <c r="C35" s="55" t="s">
         <v>723</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>720</v>
-      </c>
-      <c r="C35" s="55" t="s">
-        <v>721</v>
       </c>
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
@@ -7944,13 +7964,13 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="35" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C36" s="56" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="D36" s="56"/>
       <c r="E36" s="56"/>
@@ -7960,13 +7980,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="35" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
@@ -7976,13 +7996,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="35" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="D38" s="55"/>
       <c r="E38" s="55"/>
@@ -7992,13 +8012,13 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="35" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C39" s="56" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="D39" s="56"/>
       <c r="E39" s="56"/>
@@ -8008,13 +8028,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="35" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C40" s="56" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
@@ -8024,13 +8044,13 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="35" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="C41" s="56" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="D41" s="56"/>
       <c r="E41" s="56"/>
@@ -8040,13 +8060,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="35" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C42" s="56" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="D42" s="56"/>
       <c r="E42" s="56"/>
@@ -8056,13 +8076,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="35" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="C43" s="56" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="D43" s="56"/>
       <c r="E43" s="56"/>
@@ -8072,13 +8092,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="35" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C44" s="56" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
@@ -8118,7 +8138,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="58" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B48" s="58"/>
       <c r="C48" s="58"/>
@@ -8130,7 +8150,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="57" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B49" s="57"/>
       <c r="C49" s="57"/>
@@ -8142,12 +8162,12 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="58" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B52" s="58"/>
       <c r="C52" s="58"/>
@@ -8159,12 +8179,12 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="58" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B57" s="58"/>
       <c r="C57" s="58"/>
@@ -8176,72 +8196,72 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="59" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="59" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="59" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H73" s="58" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="I73" s="58"/>
       <c r="J73" s="58"/>
@@ -8249,483 +8269,483 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="59" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="59" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="59" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="59" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="59" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="59" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="59" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="59" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="59" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="59" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="59" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="59" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="59" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="59" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="59" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="59" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="59" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="59" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="59" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="59" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="59" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="59" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="59" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="59" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="59" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="59" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="59" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="59" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="59" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="59" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="59" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="59" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="59" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="59" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="59" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="59" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="59" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="59" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="59" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="59" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="59" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="59" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="59" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="59" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="59" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="59" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="59" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="59" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="59" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="59" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="59" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="59" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="59" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="59" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="59" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="59" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="59" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="59" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="59" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8736,78 +8756,78 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="59" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="59" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="59" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="59" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="59" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="59" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="59" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="59" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="59" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="59" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="59" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="59" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="59" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
   </sheetData>
@@ -8859,7 +8879,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="58" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -8877,10 +8897,10 @@
         <v>128</v>
       </c>
       <c r="D2" s="60" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="E2" s="60" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8891,7 +8911,7 @@
         <v>285</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="D3" s="35" t="n">
         <v>7</v>
@@ -8908,10 +8928,10 @@
         <v>292</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="E4" s="35" t="n">
         <v>6</v>
@@ -8925,10 +8945,10 @@
         <v>292</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="E5" s="62" t="n">
         <v>6</v>
@@ -8942,10 +8962,10 @@
         <v>285</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="E6" s="62" t="n">
         <v>1</v>
@@ -8980,37 +9000,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -9039,19 +9059,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="66" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
       <c r="D1" s="66"/>
       <c r="E1" s="66" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="F1" s="66"/>
       <c r="G1" s="66"/>
       <c r="H1" s="66"/>
       <c r="I1" s="66" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="J1" s="66"/>
       <c r="K1" s="66"/>
@@ -9067,16 +9087,16 @@
         <v>24</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9084,10 +9104,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9095,10 +9115,10 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9106,25 +9126,25 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="1" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I7" s="1" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I8" s="1" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increased version info box, added new self-healing spell, made pet food granting that spell
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -58,9 +58,6 @@
     <t xml:space="preserve">Version string „Ambermoon Advanced …“ is too long in original.</t>
   </si>
   <si>
-    <t xml:space="preserve">You can avoid some spinners (at least in remake) at the end when moving along the pillars</t>
-  </si>
-  <si>
     <t xml:space="preserve">You can avoid the lava in first 3D section by passing by the pillar</t>
   </si>
   <si>
@@ -109,7 +106,10 @@
     <t xml:space="preserve">- Fix non-blocking walls in 3 maps</t>
   </si>
   <si>
-    <t xml:space="preserve">Add secondary functionality of the two levers in desert temple</t>
+    <t xml:space="preserve">Add spell name for self healing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Savegame, add charge for all pet food (inventory, merchant, chest)</t>
   </si>
   <si>
     <t xml:space="preserve">In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
@@ -3567,10 +3567,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A38 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3596,10 +3596,10 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="1" sqref="A38 B35"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -3991,10 +3991,10 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="1" sqref="A38 E42"/>
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -4084,10 +4084,10 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="A38 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -4306,10 +4306,10 @@
   <dimension ref="A1:A43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="1" sqref="A38 G18"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4510,10 +4510,10 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A38 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -4720,10 +4720,10 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="1" sqref="A38 C38"/>
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83"/>
@@ -5409,10 +5409,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="A38 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -5516,10 +5516,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A38 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
@@ -5567,10 +5567,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A38 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5596,10 +5596,10 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="A38 B21"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -6445,10 +6445,10 @@
   <dimension ref="A1:A46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6464,13 +6464,11 @@
       <c r="A3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6484,17 +6482,17 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6505,7 +6503,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6517,7 +6515,7 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6525,12 +6523,12 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6539,58 +6537,60 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
@@ -6623,10 +6623,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="A38 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -6788,10 +6788,10 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A38 B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -6915,10 +6915,10 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="1" sqref="A38 K8"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -7139,10 +7139,10 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A38 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -7595,10 +7595,10 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A38 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
@@ -7652,10 +7652,10 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="1" sqref="A38 A57"/>
+      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -9000,10 +9000,10 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="1" sqref="A38 I16"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -9125,10 +9125,10 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A38 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -9184,10 +9184,10 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A38 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="67" t="s">
@@ -9303,10 +9303,10 @@
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G52" activeCellId="1" sqref="A38 G52"/>
+      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -9674,10 +9674,10 @@
   <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="A38 A17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -9807,10 +9807,10 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="A38 A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -9910,10 +9910,10 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A38 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -10064,10 +10064,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="A38 C16"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -10135,10 +10135,10 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="A38 A28"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -10905,10 +10905,10 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L33" activeCellId="1" sqref="A38 L33"/>
+      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Code improvements regarding animal party members, documenting code
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Add item which grant lock picking for Selena and maybe someone else.</t>
   </si>
   <si>
-    <t xml:space="preserve">Version string „Ambermoon Advanced …“ is too long in original.</t>
+    <t xml:space="preserve">Larger version box is not cleared after returning to game (drawn left and right outside the map screen)</t>
   </si>
   <si>
     <t xml:space="preserve">You can avoid the lava in first 3D section by passing by the pillar</t>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">Ensure distributing gold/food is not possible in Amiga version for animals</t>
   </si>
   <si>
+    <t xml:space="preserve">Can’t access animal inventory, can’t use items, etc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Texte verfeinern (besonders die Bücher)</t>
   </si>
   <si>
@@ -106,10 +109,7 @@
     <t xml:space="preserve">- Fix non-blocking walls in 3 maps</t>
   </si>
   <si>
-    <t xml:space="preserve">Add spell name for self healing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Savegame, add charge for all pet food (inventory, merchant, chest)</t>
+    <t xml:space="preserve">Old savegames: add charge for all pet food (inventory, merchant, chest)</t>
   </si>
   <si>
     <t xml:space="preserve">In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
@@ -3570,7 +3570,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3599,7 +3599,7 @@
       <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -3994,7 +3994,7 @@
       <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -4087,7 +4087,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -4309,7 +4309,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4513,7 +4513,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -4723,7 +4723,7 @@
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83"/>
@@ -5412,7 +5412,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -5519,7 +5519,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
@@ -5570,7 +5570,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5599,7 +5599,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -6445,10 +6445,10 @@
   <dimension ref="A1:A46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6456,12 +6456,12 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
@@ -6532,57 +6532,57 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
@@ -6626,7 +6626,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -6791,7 +6791,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -6918,7 +6918,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -7142,7 +7142,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -7598,7 +7598,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
@@ -7655,7 +7655,7 @@
       <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -9003,7 +9003,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -9128,7 +9128,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -9187,7 +9187,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="67" t="s">
@@ -9306,7 +9306,7 @@
       <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -9677,7 +9677,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -9810,7 +9810,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -9913,7 +9913,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -10067,7 +10067,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -10138,7 +10138,7 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -10908,7 +10908,7 @@
       <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Added map flag to disallow eagle/broom and used it on lava stream
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
   <si>
-    <t xml:space="preserve">Add item which grant lock picking for Selena and maybe someone else.</t>
+    <t xml:space="preserve">Add item which grant lock picking for Selena and maybe someone else. There is the Silverhand but you only get it when killing Nagier.</t>
   </si>
   <si>
     <t xml:space="preserve">Larger version box is not cleared after returning to game (drawn left and right outside the map screen)</t>
@@ -3582,7 +3582,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3611,7 +3611,7 @@
       <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -4006,7 +4006,7 @@
       <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -4099,7 +4099,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -4321,7 +4321,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4525,7 +4525,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -4735,7 +4735,7 @@
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83"/>
@@ -5424,7 +5424,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -5531,7 +5531,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
@@ -5582,7 +5582,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5611,7 +5611,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -6457,10 +6457,10 @@
   <dimension ref="A1:A48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6582,7 +6582,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -6600,25 +6600,25 @@
       <c r="A35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6650,7 +6650,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -6815,7 +6815,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -6942,7 +6942,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -7166,7 +7166,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -7622,7 +7622,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
@@ -7679,7 +7679,7 @@
       <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -9027,7 +9027,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -9152,7 +9152,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -9211,7 +9211,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="67" t="s">
@@ -9330,7 +9330,7 @@
       <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -9701,7 +9701,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -9834,7 +9834,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -9937,7 +9937,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -10091,7 +10091,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -10162,7 +10162,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -10932,7 +10932,7 @@
       <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Adjusted SP cost for empowered spells (party members only)
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -2124,49 +2124,49 @@
     <t xml:space="preserve">- Ghost Weapon: 5 -&gt; 30</t>
   </si>
   <si>
-    <t xml:space="preserve">Firebeam | 20-30 | 40-60</t>
+    <t xml:space="preserve">Firebeam | 20-30 | 35-55</t>
   </si>
   <si>
     <t xml:space="preserve">- Create Food: 10 -&gt; 15</t>
   </si>
   <si>
-    <t xml:space="preserve">Fireball | 40-85 | 70-120</t>
+    <t xml:space="preserve">Fireball | 40-85 | 70-105</t>
   </si>
   <si>
     <t xml:space="preserve">- Blink: 5 -&gt; 15</t>
   </si>
   <si>
-    <t xml:space="preserve">Firestorm | 35-65 | 65-110</t>
+    <t xml:space="preserve">Firestorm | 35-65 | 65-95</t>
   </si>
   <si>
     <t xml:space="preserve">- Jump: 10 -&gt; 50</t>
   </si>
   <si>
-    <t xml:space="preserve">Firepillar | 40-70 | 60-100</t>
+    <t xml:space="preserve">Firepillar | 40-70 | 55-85</t>
   </si>
   <si>
     <t xml:space="preserve">- Word Of Marking: 20 -&gt; 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Waterfall | 32-60 | 55-75</t>
+    <t xml:space="preserve">Waterfall | 32-60 | 60-75</t>
   </si>
   <si>
     <t xml:space="preserve">- Word Of Returning: 20 -&gt; 80</t>
   </si>
   <si>
-    <t xml:space="preserve">Iceball | 90-180 | 150-200</t>
+    <t xml:space="preserve">Iceball | 90-180 | 110-150</t>
   </si>
   <si>
     <t xml:space="preserve">- Magic Shield: 10 -&gt; 25</t>
   </si>
   <si>
-    <t xml:space="preserve">Icestorm | 64-128 | 125-175</t>
+    <t xml:space="preserve">Icestorm | 64-128 | 100-135</t>
   </si>
   <si>
     <t xml:space="preserve">- Magic Wall: 15 -&gt; 35</t>
   </si>
   <si>
-    <t xml:space="preserve">Iceshower | 128-256 | 110-170</t>
+    <t xml:space="preserve">Iceshower | 128-256 | 90-120</t>
   </si>
   <si>
     <t xml:space="preserve">- Magic Barrier: 20 -&gt; 45</t>
@@ -6729,7 +6729,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -7394,8 +7394,8 @@
   </sheetPr>
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added restless ghost and finalized the associated quest
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">Change water of life to only grant „Wake the dead“</t>
   </si>
   <si>
-    <t xml:space="preserve">Finish Isdir quests</t>
+    <t xml:space="preserve">Finish Isdir quests, including the end reward (essence)</t>
   </si>
   <si>
     <t xml:space="preserve">Add restless spirit/ghost, add the item drop</t>
@@ -3720,7 +3720,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3749,7 +3749,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -3939,16 +3939,16 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>377</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>380</v>
       </c>
     </row>
@@ -4158,7 +4158,7 @@
       <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -4251,7 +4251,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -4469,11 +4469,11 @@
   </sheetPr>
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4677,7 +4677,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -4901,7 +4901,7 @@
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83"/>
@@ -5590,7 +5590,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -5697,7 +5697,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
@@ -5748,7 +5748,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5777,7 +5777,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -6622,11 +6622,11 @@
   </sheetPr>
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6801,17 +6801,17 @@
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -6837,7 +6837,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -7053,10 +7053,10 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7137,7 +7137,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -7278,7 +7278,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -7502,7 +7502,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -7958,7 +7958,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
@@ -8015,7 +8015,7 @@
       <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -9363,7 +9363,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -9488,7 +9488,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -9547,7 +9547,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="66" t="s">
@@ -9666,7 +9666,7 @@
       <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -10079,7 +10079,7 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -10227,7 +10227,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -10330,7 +10330,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -10484,7 +10484,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -10555,7 +10555,7 @@
       <selection pane="topLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -10664,13 +10664,13 @@
       <c r="D5" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>254</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>191</v>
       </c>
     </row>
@@ -11346,7 +11346,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>452</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -11360,7 +11360,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="1" t="n">
         <v>453</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -11374,7 +11374,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="1" t="n">
         <v>454</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -11388,7 +11388,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="A54" s="1" t="n">
         <v>455</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -11427,7 +11427,7 @@
       <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>
@@ -11890,7 +11890,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <v>128</v>
       </c>
       <c r="I29" s="1" t="s">

</xml_diff>

<commit_message>
Did most for the eyrie
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="1043">
   <si>
     <t xml:space="preserve">Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -107,15 +107,6 @@
     <t xml:space="preserve">After the essences are used, you should get the cores back</t>
   </si>
   <si>
-    <t xml:space="preserve">Add new loader options to remake and packer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add new lob mode to remake and packer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compress everything as good as possible</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remove cheat protection events on Morag and add no-use flags instead. Also remove the texts. Should free some mem.</t>
   </si>
   <si>
@@ -125,6 +116,12 @@
     <t xml:space="preserve">Replace greeting text in grandpa’s house to state that this is no longer episode 1!</t>
   </si>
   <si>
+    <t xml:space="preserve">Fix eyrie teleport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add new items to Thalion Office (essences etc)</t>
+  </si>
+  <si>
     <t xml:space="preserve">In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t xml:space="preserve">302: Talked about the paladin guild with Baron Karsten </t>
+  </si>
+  <si>
+    <t xml:space="preserve">303: Touched eagle in eyrie once</t>
   </si>
   <si>
     <t xml:space="preserve">In Original all keywords from 0 to 114 are used.</t>
@@ -1912,6 +1912,12 @@
   </si>
   <si>
     <t xml:space="preserve">1x Magma Key, 1x Flamberge, 3000 Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eyrie (468)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x Lugthir’s Essence</t>
   </si>
   <si>
     <t xml:space="preserve">DoorIndex</t>
@@ -3843,7 +3849,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3872,7 +3878,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -4281,7 +4287,7 @@
       <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -4374,7 +4380,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -4596,7 +4602,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4800,7 +4806,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -5018,13 +5024,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83"/>
@@ -5729,6 +5735,17 @@
       </c>
       <c r="C56" s="1" t="s">
         <v>618</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -5757,14 +5774,14 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>175</v>
@@ -5775,7 +5792,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5783,7 +5800,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5791,7 +5808,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5799,7 +5816,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5807,7 +5824,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5815,7 +5832,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5823,7 +5840,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5831,7 +5848,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5839,7 +5856,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -5864,33 +5881,33 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -5915,11 +5932,11 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -5944,7 +5961,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -5960,80 +5977,80 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>640</v>
-      </c>
       <c r="E5" s="23" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="F5" s="24" t="n">
         <v>75</v>
@@ -6068,13 +6085,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="F6" s="24" t="n">
         <v>150</v>
@@ -6109,13 +6126,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="F7" s="24" t="n">
         <v>180</v>
@@ -6150,13 +6167,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="F8" s="24" t="n">
         <v>100</v>
@@ -6191,13 +6208,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="F9" s="24" t="n">
         <v>125</v>
@@ -6232,13 +6249,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="F10" s="24" t="n">
         <v>90</v>
@@ -6273,13 +6290,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="F11" s="24" t="n">
         <v>90</v>
@@ -6314,13 +6331,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="F12" s="24" t="n">
         <v>90</v>
@@ -6355,13 +6372,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="F13" s="24" t="n">
         <v>95</v>
@@ -6396,13 +6413,13 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="F14" s="30" t="n">
         <v>32767</v>
@@ -6437,58 +6454,58 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="F18" s="35" t="n">
         <v>75</v>
@@ -6515,13 +6532,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="F19" s="35" t="n">
         <v>59850</v>
@@ -6548,13 +6565,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="F20" s="35" t="n">
         <v>150</v>
@@ -6581,7 +6598,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="26" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="F21" s="35" t="n">
         <v>600</v>
@@ -6608,7 +6625,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="26" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="F22" s="35" t="n">
         <v>950</v>
@@ -6635,7 +6652,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="26" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="F23" s="35" t="n">
         <v>1890</v>
@@ -6662,7 +6679,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="26" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="F24" s="35" t="n">
         <v>4500</v>
@@ -6689,7 +6706,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="26" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="F25" s="35" t="n">
         <v>12240</v>
@@ -6716,7 +6733,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="26" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="F26" s="35" t="n">
         <v>29250</v>
@@ -6743,7 +6760,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="32" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="F27" s="37" t="n">
         <v>113400</v>
@@ -6787,13 +6804,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:A54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6931,49 +6948,42 @@
       <c r="A37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A38" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A45" s="0" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -6996,7 +7006,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -7005,7 +7015,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="39" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>175</v>
@@ -7014,10 +7024,10 @@
         <v>435</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7025,16 +7035,16 @@
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>399</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7042,16 +7052,16 @@
         <v>153</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>399</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7059,16 +7069,16 @@
         <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>399</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7076,16 +7086,16 @@
         <v>154</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>399</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7093,16 +7103,16 @@
         <v>374</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7110,16 +7120,16 @@
         <v>375</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>399</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7127,16 +7137,16 @@
         <v>376</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>705</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>702</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7144,16 +7154,16 @@
         <v>377</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7161,16 +7171,16 @@
         <v>378</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7178,16 +7188,16 @@
         <v>379</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>707</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>
@@ -7212,7 +7222,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.6"/>
@@ -7220,7 +7230,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>175</v>
@@ -7229,7 +7239,7 @@
         <v>435</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7237,13 +7247,13 @@
         <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7251,13 +7261,13 @@
         <v>174</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7265,13 +7275,13 @@
         <v>175</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -7296,7 +7306,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -7305,7 +7315,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>175</v>
@@ -7314,7 +7324,7 @@
         <v>435</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7322,13 +7332,13 @@
         <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>438</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7336,13 +7346,13 @@
         <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>438</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7350,13 +7360,13 @@
         <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>438</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7364,13 +7374,13 @@
         <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7378,13 +7388,13 @@
         <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>724</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7392,13 +7402,13 @@
         <v>97</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>724</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7406,13 +7416,13 @@
         <v>98</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
   </sheetData>
@@ -7437,7 +7447,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -7445,19 +7455,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="G1" s="5" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>179</v>
@@ -7466,7 +7476,7 @@
         <v>175</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>179</v>
@@ -7483,7 +7493,7 @@
         <v>1193</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>4</v>
@@ -7492,7 +7502,7 @@
         <v>1167</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7503,7 +7513,7 @@
         <v>1194</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>4</v>
@@ -7512,7 +7522,7 @@
         <v>1168</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7523,7 +7533,7 @@
         <v>1195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>4</v>
@@ -7532,7 +7542,7 @@
         <v>1169</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7543,7 +7553,7 @@
         <v>1196</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>4</v>
@@ -7552,7 +7562,7 @@
         <v>1170</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7563,7 +7573,7 @@
         <v>1197</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>4</v>
@@ -7572,7 +7582,7 @@
         <v>1171</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7583,7 +7593,7 @@
         <v>1198</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>4</v>
@@ -7592,7 +7602,7 @@
         <v>1172</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7603,7 +7613,7 @@
         <v>1199</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -7612,7 +7622,7 @@
         <v>1173</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7623,7 +7633,7 @@
         <v>1200</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>4</v>
@@ -7632,7 +7642,7 @@
         <v>1174</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -7661,7 +7671,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -7670,426 +7680,426 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="42" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="D2" s="44"/>
       <c r="E2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="E3" s="46"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
     </row>
   </sheetData>
@@ -8117,39 +8127,39 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -8174,7 +8184,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -8182,21 +8192,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="47" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8264,42 +8274,42 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B16" s="35" t="n">
         <v>0</v>
@@ -8328,7 +8338,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="B17" s="35" t="n">
         <v>100</v>
@@ -8357,7 +8367,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B18" s="35" t="n">
         <v>100</v>
@@ -8386,7 +8396,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B19" s="35" t="n">
         <v>100</v>
@@ -8415,7 +8425,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B20" s="35" t="n">
         <v>100</v>
@@ -8444,7 +8454,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="51" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B21" s="35" t="n">
         <v>100</v>
@@ -8473,7 +8483,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="B22" s="35" t="n">
         <v>100</v>
@@ -8502,7 +8512,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="B23" s="37" t="n">
         <v>100</v>
@@ -8531,22 +8541,22 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8554,10 +8564,10 @@
         <v>180</v>
       </c>
       <c r="B32" s="53" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
@@ -8567,13 +8577,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="35" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="C33" s="55" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="D33" s="55"/>
       <c r="E33" s="55"/>
@@ -8583,13 +8593,13 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="35" t="s">
+        <v>853</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>851</v>
       </c>
-      <c r="B34" s="27" t="s">
-        <v>849</v>
-      </c>
       <c r="C34" s="55" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="D34" s="55"/>
       <c r="E34" s="55"/>
@@ -8599,13 +8609,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="35" t="s">
+        <v>854</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>851</v>
+      </c>
+      <c r="C35" s="55" t="s">
         <v>852</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>849</v>
-      </c>
-      <c r="C35" s="55" t="s">
-        <v>850</v>
       </c>
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
@@ -8615,13 +8625,13 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="35" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C36" s="56" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="D36" s="56"/>
       <c r="E36" s="56"/>
@@ -8631,13 +8641,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="35" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
@@ -8647,13 +8657,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="35" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="D38" s="55"/>
       <c r="E38" s="55"/>
@@ -8663,13 +8673,13 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="35" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C39" s="56" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="D39" s="56"/>
       <c r="E39" s="56"/>
@@ -8679,13 +8689,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="35" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C40" s="56" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
@@ -8695,13 +8705,13 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="35" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="C41" s="56" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="D41" s="56"/>
       <c r="E41" s="56"/>
@@ -8711,13 +8721,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="35" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="C42" s="56" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="D42" s="56"/>
       <c r="E42" s="56"/>
@@ -8727,13 +8737,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="35" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C43" s="56" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="D43" s="56"/>
       <c r="E43" s="56"/>
@@ -8743,13 +8753,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="35" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="C44" s="56" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
@@ -8789,7 +8799,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="58" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B48" s="58"/>
       <c r="C48" s="58"/>
@@ -8801,7 +8811,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="57" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="B49" s="57"/>
       <c r="C49" s="57"/>
@@ -8813,12 +8823,12 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="58" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="B52" s="58"/>
       <c r="C52" s="58"/>
@@ -8830,12 +8840,12 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="58" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="B57" s="58"/>
       <c r="C57" s="58"/>
@@ -8847,72 +8857,72 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="59" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="59" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="59" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H73" s="58" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="I73" s="58"/>
       <c r="J73" s="58"/>
@@ -8920,483 +8930,483 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="59" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="59" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="59" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="59" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="59" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="59" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="59" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="59" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="59" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="59" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="59" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="59" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="59" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="59" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="59" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="59" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="59" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="59" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="59" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="59" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="59" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="59" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="59" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="59" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="59" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="59" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="59" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="59" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="59" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="59" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="59" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="59" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="59" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="59" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="59" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="59" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="59" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="59" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="59" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="59" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="59" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="59" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="59" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="59" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="59" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="59" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="59" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="59" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="59" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="59" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="59" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="59" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="59" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="59" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="59" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="59" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="59" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="59" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="59" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9407,78 +9417,78 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="59" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="59" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="59" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="59" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="59" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="59" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="59" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="59" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="59" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="59" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="59" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="59" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="59" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
     </row>
   </sheetData>
@@ -9522,7 +9532,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -9530,7 +9540,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="58" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -9548,10 +9558,10 @@
         <v>180</v>
       </c>
       <c r="D2" s="60" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="E2" s="60" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9562,7 +9572,7 @@
         <v>385</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D3" s="35" t="n">
         <v>7</v>
@@ -9579,10 +9589,10 @@
         <v>392</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E4" s="35" t="n">
         <v>6</v>
@@ -9596,10 +9606,10 @@
         <v>392</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E5" s="62" t="n">
         <v>6</v>
@@ -9613,10 +9623,10 @@
         <v>385</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="E6" s="62" t="n">
         <v>1</v>
@@ -9647,46 +9657,46 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
     </row>
   </sheetData>
@@ -9711,23 +9721,23 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="66" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
       <c r="D1" s="66"/>
       <c r="E1" s="66" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="F1" s="66"/>
       <c r="G1" s="66"/>
       <c r="H1" s="66"/>
       <c r="I1" s="66" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="J1" s="66"/>
       <c r="K1" s="66"/>
@@ -9743,16 +9753,16 @@
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9760,10 +9770,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9771,10 +9781,10 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9782,35 +9792,35 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="1" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I7" s="1" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I8" s="1" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I9" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I10" s="1" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
     </row>
   </sheetData>
@@ -9834,435 +9844,440 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A85"/>
+  <dimension ref="A1:A86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
+      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
         <v>108</v>
       </c>
     </row>
@@ -10288,7 +10303,7 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -10451,7 +10466,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -10554,7 +10569,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -10708,7 +10723,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -10776,10 +10791,10 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -11783,7 +11798,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Finalized fire temple enter quest (Baron Karsten)
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -107,9 +107,6 @@
     <t xml:space="preserve">After the essences are used, you should get the cores back</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove cheat protection events on Morag and add no-use flags instead. Also remove the texts. Should free some mem.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Check if any map graphics (tiles, walls, objects, overlays) are unused and remove them. Adjust refs of course!</t>
   </si>
   <si>
@@ -462,6 +459,9 @@
   </si>
   <si>
     <t xml:space="preserve">139: CRYSTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">140: SCHWARZBERGE / BLACK MOUNTAINS</t>
   </si>
   <si>
     <t xml:space="preserve">In Original all goto points till 78 (including) are used except for 2 and 17.</t>
@@ -3893,7 +3893,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6836,7 +6836,7 @@
   <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6977,14 +6977,12 @@
       <c r="A37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6995,7 +6993,7 @@
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7005,25 +7003,25 @@
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -9888,8 +9886,8 @@
   </sheetPr>
   <dimension ref="A1:A86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9899,428 +9897,428 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -10339,10 +10337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10352,137 +10350,142 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>137</v>
       </c>
     </row>
@@ -10833,7 +10836,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added more details to wine cellar, added text for locked item and locked cat life item in savegame
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -99,6 +99,9 @@
     <t xml:space="preserve">Maybe sell a few real copies for hardcore fans</t>
   </si>
   <si>
+    <t xml:space="preserve">Avoid moving the animal revive in Amiga code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Skip possibility and welcome text for Inns if the animal is the only alive party member (search for TODO)</t>
   </si>
   <si>
@@ -118,9 +121,6 @@
   </si>
   <si>
     <t xml:space="preserve">Check glob var 193, is set when looting shandra’s grave, but not connected in original data of map 428</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add new text and use it („Can’t exchange exp with animals“)</t>
   </si>
   <si>
     <t xml:space="preserve">Clearly state how the exp exchange works in the book! Transfer stone, use it, user and target will exchange, not cast on self, not cast on animals, etc. The stone will be consumed in any case!</t>
@@ -7298,7 +7298,7 @@
   <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7411,15 +7411,19 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7427,13 +7431,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7448,30 +7452,26 @@
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">

</xml_diff>

<commit_message>
Added Kasimir portraits and finalized Sandra events
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,6 +39,7 @@
     <sheet name="CodeChanges" sheetId="29" state="visible" r:id="rId30"/>
     <sheet name="Exp Table" sheetId="30" state="visible" r:id="rId31"/>
     <sheet name="Bosses" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="Portraits" sheetId="32" state="visible" r:id="rId33"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="1117">
   <si>
     <t xml:space="preserve">Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -88,7 +89,25 @@
     <t xml:space="preserve">Skip possibility and welcome text for Inns if the animal is the only alive party member (search for TODO)</t>
   </si>
   <si>
-    <t xml:space="preserve">After the essences are used, you should get the cores back</t>
+    <t xml:space="preserve">Check desert temple sand hole hints, maybe make it clearer or add another orb with „Shovel and Pickaxe“</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clearly state how the exp exchange works in the book! Transfer stone, use it, user and target will exchange, not cast on self, not cast on animals, etc. The stone will be consumed in any case!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide more stones of knowledge (currently there are 3 I guess)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write and print an awesome game manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe sell a few real copies for hardcore fans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torch in ice cave gfx issue on amiga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t show „next level at exp …“ when leveling up Kasimir!</t>
   </si>
   <si>
     <t xml:space="preserve">Test recharge limit of spell ChargeItem</t>
@@ -106,27 +125,6 @@
     <t xml:space="preserve">Test extended chests on Amiga (works, test chest 256)</t>
   </si>
   <si>
-    <t xml:space="preserve">Check desert temple sand hole hints, maybe make it clearer or add another orb with „Shovel and Pickaxe“</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clearly state how the exp exchange works in the book! Transfer stone, use it, user and target will exchange, not cast on self, not cast on animals, etc. The stone will be consumed in any case!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hide more stones of knowledge (currently there are 3 I guess)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Write and print an awesome game manual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maybe sell a few real copies for hardcore fans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torch in ice cave gfx issue on amiga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don’t show „next level at exp …“ when leveling up Kasimir!</t>
-  </si>
-  <si>
     <t xml:space="preserve">In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
   </si>
   <si>
@@ -389,6 +387,9 @@
   </si>
   <si>
     <t xml:space="preserve">306: Transfer Stone available on Altar of Knowledge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">307: Transferred any essence</t>
   </si>
   <si>
     <t xml:space="preserve">In Original all keywords from 0 to 114 are used.</t>
@@ -3402,6 +3403,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empowered Kasimir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full power Kasimir</t>
   </si>
 </sst>
 </file>
@@ -7412,8 +7419,8 @@
   </sheetPr>
   <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7489,42 +7496,42 @@
       <c r="A18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A19" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
+      <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
+      <c r="A26" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7532,46 +7539,38 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>18</v>
+      <c r="A36" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>19</v>
+      <c r="A37" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10451,10 +10450,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A89"/>
+  <dimension ref="A1:A90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10464,442 +10463,447 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
         <v>112</v>
       </c>
     </row>
@@ -11805,6 +11809,46 @@
       </c>
       <c r="B6" s="0" t="s">
         <v>1114</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>1116</v>
       </c>
     </row>
   </sheetData>
@@ -12337,7 +12381,7 @@
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed portrait loading issue
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="31"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -86,9 +86,6 @@
     <t xml:space="preserve">Old savegames: add charge for all pet food (inventory, merchant, chest)</t>
   </si>
   <si>
-    <t xml:space="preserve">Skip possibility and welcome text for Inns if the animal is the only alive party member (search for TODO)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Check desert temple sand hole hints, maybe make it clearer or add another orb with „Shovel and Pickaxe“</t>
   </si>
   <si>
@@ -110,6 +107,12 @@
     <t xml:space="preserve">Don’t show „next level at exp …“ when leveling up Kasimir!</t>
   </si>
   <si>
+    <t xml:space="preserve">Test and implement changing portraits and Sandra events on Amiga!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age is very high for all chars (including NPCs) and also for new games. Maybe a display issue?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test recharge limit of spell ChargeItem</t>
   </si>
   <si>
@@ -387,9 +390,6 @@
   </si>
   <si>
     <t xml:space="preserve">306: Transfer Stone available on Altar of Knowledge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">307: Transferred any essence</t>
   </si>
   <si>
     <t xml:space="preserve">In Original all keywords from 0 to 114 are used.</t>
@@ -7419,8 +7419,8 @@
   </sheetPr>
   <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7488,80 +7488,86 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10450,10 +10456,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A90"/>
+  <dimension ref="A1:A89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10463,447 +10469,442 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
         <v>112</v>
       </c>
     </row>
@@ -11829,7 +11830,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added more items to the wine cellar chest and improved the map
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="1195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="1195">
   <si>
     <t xml:space="preserve">Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -61,6 +61,15 @@
     <t xml:space="preserve">Kasimir has all elemental spell damage bonusses from start but a penalty of 50%. This means if he uses the cores they all do the same base damage but 50% lower than the normal version a black mage can use. Around 50-60 dmg.</t>
   </si>
   <si>
+    <t xml:space="preserve">Findings:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monstergroup 24 ist gleich zu 48. Lebabs Golems und die in der Quelle des Lebens.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check glob var 193, is set when looting shandra’s grave, but not connected in original data of map 428</t>
+  </si>
+  <si>
     <t xml:space="preserve">Add item which grant lock picking for Selena and maybe someone else. There is the Silverhand but you only get it when killing Nagier.</t>
   </si>
   <si>
@@ -88,9 +97,6 @@
     <t xml:space="preserve">- Fix non-blocking walls in 3 maps</t>
   </si>
   <si>
-    <t xml:space="preserve">Old savegames: add charge for all pet food (inventory, merchant, chest)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clearly state how the exp exchange works in the book! Transfer stone, use it, user and target will exchange, not cast on self, not cast on animals, etc. The stone will be consumed in any case!</t>
   </si>
   <si>
@@ -100,7 +106,7 @@
     <t xml:space="preserve">Torch in ice cave gfx issue on amiga</t>
   </si>
   <si>
-    <t xml:space="preserve">Kasimir gets food when it is distributed</t>
+    <t xml:space="preserve">Maybe hint somehow that there is another room with the brooch. A sign?</t>
   </si>
   <si>
     <t xml:space="preserve">Some hints about the Sunny brooch might be good. Maybe if you show them someone he would react? Lebab, Gryban.</t>
@@ -109,100 +115,94 @@
     <t xml:space="preserve">Test recharge limit of spell ChargeItem</t>
   </si>
   <si>
+    <t xml:space="preserve">Test if saving works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if chest 256 still works with extended chests on Amiga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See sheet „Custom Translations“ here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elementanpassungen:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Fluchwespe: Keins -&gt; Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Gizzek: Keins -&gt; Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Gizzek Königin: Keins -&gt; Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Tornak: Keins -&gt; Erde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Tornakweibchen: Keins -&gt; Erde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Sandechse: Keins -&gt; Erde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Morag Drache: Keins -&gt; Feuer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Morag Echse: Keins -&gt; Erde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Magische Wache: Keins -&gt; Geist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Biest: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Nera: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Bandit: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Banditenhauptmann: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Höhlenmolch: Keins -&gt; Wasser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Zombiemeister: Untot -&gt; Keins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Meisterdieb: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Ork: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Ork Hauptmann: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Reg: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Krieger: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Minotaur: Keins -&gt; Physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Sansri: Keins -&gt; Mental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- alle Echsenlords: Keins -&gt; Mental</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if any map graphics (tiles, walls, objects, overlays) are unused and remove them. Adjust refs of course!</t>
   </si>
   <si>
-    <t xml:space="preserve">Check glob var 193, is set when looting shandra’s grave, but not connected in original data of map 428</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test if saving works</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test extended chests on Amiga (works, test chest 256)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Write and print an awesome game manual</t>
   </si>
   <si>
     <t xml:space="preserve">Maybe sell a few real copies for hardcore fans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See sheet „Custom Translations“ here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monstergroup 24 ist gleich zu 48. Lebabs Golems und die in der Quelle des Lebens.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elementanpassungen:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Fluchwespe: Keins -&gt; Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Gizzek: Keins -&gt; Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Gizzek Königin: Keins -&gt; Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Tornak: Keins -&gt; Erde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Tornakweibchen: Keins -&gt; Erde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Sandechse: Keins -&gt; Erde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Morag Drache: Keins -&gt; Feuer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Morag Echse: Keins -&gt; Erde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Magische Wache: Keins -&gt; Geist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Biest: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Nera: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Bandit: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Banditenhauptmann: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Höhlenmolch: Keins -&gt; Wasser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Zombiemeister: Untot -&gt; Keins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Meisterdieb: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Ork: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Ork Hauptmann: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Reg: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Krieger: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Minotaur: Keins -&gt; Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Sansri: Keins -&gt; Mental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- alle Echsenlords: Keins -&gt; Mental</t>
   </si>
   <si>
     <t xml:space="preserve">In Original all vars from 1 to 223 are used except for 0, 53 and 54.</t>
@@ -2048,7 +2048,25 @@
     <t xml:space="preserve">1x Pickaxe, 1x Shovel</t>
   </si>
   <si>
-    <t xml:space="preserve">1x Sunny’s Brooch</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1x Sunny’s Brooch, 1x Moon Amulet, 5x Old Wine, 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">x Wishing Coins, 2000 Gold</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">1x Giant Mallet</t>
@@ -3659,7 +3677,7 @@
     <numFmt numFmtId="168" formatCode="dd/\ mmm"/>
     <numFmt numFmtId="169" formatCode="\+0\%;\-0\%;&quot;No change&quot;"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3703,6 +3721,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4250,7 +4274,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4290,15 +4314,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4392,13 +4416,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4406,8 +4430,23 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4429,10 +4468,10 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -4841,7 +4880,7 @@
       <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -4934,7 +4973,7 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -5280,7 +5319,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5484,7 +5523,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -5704,11 +5743,11 @@
   </sheetPr>
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
@@ -6045,7 +6084,7 @@
       <c r="C22" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>637</v>
       </c>
     </row>
@@ -6059,7 +6098,7 @@
       <c r="C23" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>639</v>
       </c>
     </row>
@@ -6073,7 +6112,7 @@
       <c r="C24" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>641</v>
       </c>
     </row>
@@ -6087,7 +6126,7 @@
       <c r="C25" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>643</v>
       </c>
     </row>
@@ -6668,7 +6707,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -6754,7 +6793,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -6783,7 +6822,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
@@ -6834,7 +6873,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6863,7 +6902,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -7706,17 +7745,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A66"/>
+  <dimension ref="A1:A71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7724,7 +7763,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7732,256 +7771,245 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-    </row>
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>12</v>
+      <c r="A20" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>15</v>
+      <c r="A25" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A38" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A40" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>26</v>
+      <c r="A43" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>27</v>
+      <c r="A44" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>28</v>
+      <c r="A45" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>29</v>
+      <c r="A46" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>30</v>
+      <c r="A47" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>31</v>
+      <c r="A48" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>32</v>
+      <c r="A49" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>33</v>
+      <c r="A50" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>34</v>
+      <c r="A51" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>35</v>
+      <c r="A52" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>36</v>
+      <c r="A53" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>37</v>
+      <c r="A54" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
+      <c r="A55" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
+      <c r="A57" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>42</v>
+      <c r="A59" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>49</v>
       </c>
     </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8004,7 +8032,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -8220,7 +8248,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.6"/>
@@ -8304,7 +8332,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -8445,7 +8473,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -8669,7 +8697,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -9125,7 +9153,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
@@ -9182,7 +9210,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -10530,7 +10558,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -10655,7 +10683,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -10719,7 +10747,7 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="70" t="s">
@@ -10848,7 +10876,7 @@
       <selection pane="topLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -11326,9 +11354,9 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11355,307 +11383,307 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H2</f>
         <v>47250</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H2</f>
         <v>582675</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">(A3*A3+A3)/2</f>
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">B3</f>
         <v>3</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H3</f>
         <v>94500</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H3</f>
         <v>1165350</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <f aca="false">(A4*A4+A4)/2</f>
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">C3+B4</f>
         <v>9</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H4</f>
         <v>113400</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H4</f>
         <v>1398420</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <f aca="false">(A5*A5+A5)/2</f>
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <f aca="false">C4+B5</f>
         <v>19</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H5</f>
         <v>63000</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H5</f>
         <v>776900</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <f aca="false">(A6*A6+A6)/2</f>
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <f aca="false">C5+B6</f>
         <v>34</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H6</f>
         <v>78750</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H6</f>
         <v>971125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <f aca="false">(A7*A7+A7)/2</f>
         <v>21</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <f aca="false">C6+B7</f>
         <v>55</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H7</f>
         <v>56700</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H7</f>
         <v>699210</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <f aca="false">(A8*A8+A8)/2</f>
         <v>28</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <f aca="false">C7+B8</f>
         <v>83</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H8</f>
         <v>56700</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H8</f>
         <v>699210</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <f aca="false">(A9*A9+A9)/2</f>
         <v>36</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <f aca="false">C8+B9</f>
         <v>119</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H9</f>
         <v>56700</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H9</f>
         <v>699210</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <f aca="false">(A10*A10+A10)/2</f>
         <v>45</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <f aca="false">C9+B10</f>
         <v>164</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>1138</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$B$51,2,0)*H10</f>
         <v>59850</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="1" t="n">
         <f aca="false">VLOOKUP($H$15,$A$2:$C$51,3,0)*H10</f>
         <v>738055</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <f aca="false">(A11*A11+A11)/2</f>
         <v>55</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <f aca="false">C10+B11</f>
         <v>219</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <f aca="false">(A12*A12+A12)/2</f>
         <v>66</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <f aca="false">C11+B12</f>
         <v>285</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <f aca="false">(A13*A13+A13)/2</f>
         <v>78</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <f aca="false">C12+B13</f>
         <v>363</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <f aca="false">(A14*A14+A14)/2</f>
         <v>91</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <f aca="false">C13+B14</f>
         <v>454</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <f aca="false">(A15*A15+A15)/2</f>
         <v>105</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <f aca="false">C14+B15</f>
         <v>559</v>
       </c>
@@ -11667,470 +11695,470 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <f aca="false">(A16*A16+A16)/2</f>
         <v>120</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <f aca="false">C15+B16</f>
         <v>679</v>
       </c>
       <c r="H16" s="74"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <f aca="false">(A17*A17+A17)/2</f>
         <v>136</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <f aca="false">C16+B17</f>
         <v>815</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <f aca="false">(A18*A18+A18)/2</f>
         <v>153</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <f aca="false">C17+B18</f>
         <v>968</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <f aca="false">(A19*A19+A19)/2</f>
         <v>171</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <f aca="false">C18+B19</f>
         <v>1139</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <f aca="false">(A20*A20+A20)/2</f>
         <v>190</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <f aca="false">C19+B20</f>
         <v>1329</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <f aca="false">(A21*A21+A21)/2</f>
         <v>210</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <f aca="false">C20+B21</f>
         <v>1539</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <f aca="false">(A22*A22+A22)/2</f>
         <v>231</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <f aca="false">C21+B22</f>
         <v>1770</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <f aca="false">(A23*A23+A23)/2</f>
         <v>253</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <f aca="false">C22+B23</f>
         <v>2023</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <f aca="false">(A24*A24+A24)/2</f>
         <v>276</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <f aca="false">C23+B24</f>
         <v>2299</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <f aca="false">(A25*A25+A25)/2</f>
         <v>300</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <f aca="false">C24+B25</f>
         <v>2599</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <f aca="false">(A26*A26+A26)/2</f>
         <v>325</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <f aca="false">C25+B26</f>
         <v>2924</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <f aca="false">(A27*A27+A27)/2</f>
         <v>351</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <f aca="false">C26+B27</f>
         <v>3275</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <f aca="false">(A28*A28+A28)/2</f>
         <v>378</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <f aca="false">C27+B28</f>
         <v>3653</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <f aca="false">(A29*A29+A29)/2</f>
         <v>406</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <f aca="false">C28+B29</f>
         <v>4059</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <f aca="false">(A30*A30+A30)/2</f>
         <v>435</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <f aca="false">C29+B30</f>
         <v>4494</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <f aca="false">(A31*A31+A31)/2</f>
         <v>465</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <f aca="false">C30+B31</f>
         <v>4959</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <f aca="false">(A32*A32+A32)/2</f>
         <v>496</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="1" t="n">
         <f aca="false">C31+B32</f>
         <v>5455</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="1" t="n">
         <f aca="false">(A33*A33+A33)/2</f>
         <v>528</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="1" t="n">
         <f aca="false">C32+B33</f>
         <v>5983</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <f aca="false">(A34*A34+A34)/2</f>
         <v>561</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <f aca="false">C33+B34</f>
         <v>6544</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <f aca="false">(A35*A35+A35)/2</f>
         <v>595</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="1" t="n">
         <f aca="false">C34+B35</f>
         <v>7139</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <f aca="false">(A36*A36+A36)/2</f>
         <v>630</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <f aca="false">C35+B36</f>
         <v>7769</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <f aca="false">(A37*A37+A37)/2</f>
         <v>666</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="1" t="n">
         <f aca="false">C36+B37</f>
         <v>8435</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <f aca="false">(A38*A38+A38)/2</f>
         <v>703</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38" s="1" t="n">
         <f aca="false">C37+B38</f>
         <v>9138</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <f aca="false">(A39*A39+A39)/2</f>
         <v>741</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <f aca="false">C38+B39</f>
         <v>9879</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="1" t="n">
         <f aca="false">(A40*A40+A40)/2</f>
         <v>780</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40" s="1" t="n">
         <f aca="false">C39+B40</f>
         <v>10659</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="1" t="n">
         <f aca="false">(A41*A41+A41)/2</f>
         <v>820</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="1" t="n">
         <f aca="false">C40+B41</f>
         <v>11479</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <f aca="false">(A42*A42+A42)/2</f>
         <v>861</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="1" t="n">
         <f aca="false">C41+B42</f>
         <v>12340</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <f aca="false">(A43*A43+A43)/2</f>
         <v>903</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="1" t="n">
         <f aca="false">C42+B43</f>
         <v>13243</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <f aca="false">(A44*A44+A44)/2</f>
         <v>946</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44" s="1" t="n">
         <f aca="false">C43+B44</f>
         <v>14189</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <f aca="false">(A45*A45+A45)/2</f>
         <v>990</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="C45" s="1" t="n">
         <f aca="false">C44+B45</f>
         <v>15179</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <f aca="false">(A46*A46+A46)/2</f>
         <v>1035</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46" s="1" t="n">
         <f aca="false">C45+B46</f>
         <v>16214</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="1" t="n">
         <f aca="false">(A47*A47+A47)/2</f>
         <v>1081</v>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="C47" s="1" t="n">
         <f aca="false">C46+B47</f>
         <v>17295</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="1" t="n">
         <f aca="false">(A48*A48+A48)/2</f>
         <v>1128</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="1" t="n">
         <f aca="false">C47+B48</f>
         <v>18423</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B49" s="1" t="n">
         <f aca="false">(A49*A49+A49)/2</f>
         <v>1176</v>
       </c>
-      <c r="C49" s="0" t="n">
+      <c r="C49" s="1" t="n">
         <f aca="false">C48+B49</f>
         <v>19599</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+      <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="1" t="n">
         <f aca="false">(A50*A50+A50)/2</f>
         <v>1225</v>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="C50" s="1" t="n">
         <f aca="false">C49+B50</f>
         <v>20824</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="1" t="n">
         <f aca="false">(A51*A51+A51)/2</f>
         <v>1275</v>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="C51" s="1" t="n">
         <f aca="false">C50+B51</f>
         <v>22099</v>
       </c>
@@ -12158,53 +12186,53 @@
       <selection pane="topLeft" activeCell="K32" activeCellId="0" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>1141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>1142</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>1143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>1145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>1146</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>1147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>1148</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>1149</v>
       </c>
     </row>
@@ -12230,21 +12258,21 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>1151</v>
       </c>
     </row>
@@ -12264,114 +12292,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>1152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>1153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>1154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>1155</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>1156</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>1152</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>1158</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>1159</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>1160</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>470</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://github.com/Pyrdacor/Ambermoon/issues/43"/>
+    <hyperlink ref="C3" r:id="rId1" display="See https://github.com/Pyrdacor/Ambermoon/issues/43"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -12394,9 +12435,9 @@
       <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12436,13 +12477,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="68" t="s">
@@ -12459,13 +12500,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>1168</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E4" s="68"/>
@@ -12474,13 +12515,13 @@
       <c r="H4" s="68"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>1170</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E5" s="68"/>
@@ -12489,13 +12530,13 @@
       <c r="H5" s="68"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>1171</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E6" s="68"/>
@@ -12504,13 +12545,13 @@
       <c r="H6" s="68"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="68"/>
@@ -12519,13 +12560,13 @@
       <c r="H7" s="68"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>1167</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="78" t="s">
@@ -12545,35 +12586,35 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>1173</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>1174</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>25</v>
       </c>
       <c r="E11" s="78" t="s">
@@ -12584,13 +12625,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>1176</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>150</v>
       </c>
       <c r="E12" s="78" t="s">
@@ -12601,57 +12642,57 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>1178</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>1179</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>1180</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>1181</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>1182</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>85</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -12662,13 +12703,13 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>1184</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>25</v>
       </c>
       <c r="E18" s="77" t="s">
@@ -12685,13 +12726,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>1186</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>99</v>
       </c>
       <c r="E19" s="68" t="s">
@@ -12711,13 +12752,13 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>1187</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="68" t="s">
@@ -12735,18 +12776,18 @@
         <f aca="false">ROUNDDOWN(AVERAGE(F20:G20),0)</f>
         <v>300</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" s="1" t="s">
         <v>1188</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>1189</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>60</v>
       </c>
       <c r="E21" s="68" t="s">
@@ -12766,13 +12807,13 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E22" s="68" t="s">
@@ -12792,13 +12833,13 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E23" s="68" t="s">
@@ -12816,7 +12857,7 @@
         <f aca="false">ROUNDDOWN(AVERAGE(F23:G23),0)</f>
         <v>25</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" s="1" t="s">
         <v>1188</v>
       </c>
     </row>
@@ -12836,7 +12877,7 @@
         <f aca="false">ROUNDDOWN(AVERAGE(F24:G24),0)</f>
         <v>22</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" s="1" t="s">
         <v>1188</v>
       </c>
     </row>
@@ -12867,13 +12908,13 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E26" s="68" t="s">
@@ -12893,13 +12934,13 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>1178</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E27" s="68" t="s">
@@ -12919,13 +12960,13 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>1186</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E28" s="68" t="s">
@@ -12945,13 +12986,13 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>1168</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>22</v>
       </c>
       <c r="E29" s="68" t="s">
@@ -12971,13 +13012,13 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>1170</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E30" s="68" t="s">
@@ -13055,13 +13096,13 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E34" s="68" t="s">
@@ -13079,13 +13120,13 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>1181</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E35" s="68" t="s">
@@ -13104,13 +13145,13 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E36" s="68" t="s">
@@ -13129,13 +13170,13 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>1171</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E37" s="68" t="s">
@@ -13198,57 +13239,57 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>1167</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>1181</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>1173</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="C45" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -13264,46 +13305,46 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>1176</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B49" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C49" s="0" t="n">
+      <c r="C49" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>1171</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="C50" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>1181</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="C51" s="1" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13319,68 +13360,68 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B55" s="0" t="n">
+      <c r="B55" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="B56" s="0" t="n">
+      <c r="B56" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C56" s="0" t="n">
+      <c r="C56" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>1167</v>
       </c>
-      <c r="B57" s="0" t="n">
+      <c r="B57" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C57" s="0" t="n">
+      <c r="C57" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>1178</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="C58" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>1179</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C59" s="0" t="n">
+      <c r="C59" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C60" s="0" t="n">
+      <c r="C60" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -13396,57 +13437,57 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C63" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>1173</v>
       </c>
-      <c r="B64" s="0" t="n">
+      <c r="B64" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C64" s="0" t="n">
+      <c r="C64" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="B65" s="0" t="n">
+      <c r="B65" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C65" s="0" t="n">
+      <c r="C65" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>1168</v>
       </c>
-      <c r="B66" s="0" t="n">
+      <c r="B66" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C66" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C67" s="0" t="n">
+      <c r="C67" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -13462,35 +13503,35 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C70" s="0" t="n">
+      <c r="C70" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>1168</v>
       </c>
-      <c r="B71" s="0" t="n">
+      <c r="B71" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C71" s="0" t="n">
+      <c r="C71" s="1" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="B72" s="0" t="n">
+      <c r="B72" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C72" s="0" t="n">
+      <c r="C72" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -13506,90 +13547,90 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B77" s="0" t="n">
+      <c r="B77" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C77" s="0" t="n">
+      <c r="C77" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="B78" s="0" t="n">
+      <c r="B78" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C78" s="0" t="n">
+      <c r="C78" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>1174</v>
       </c>
-      <c r="B79" s="0" t="n">
+      <c r="B79" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>1179</v>
       </c>
-      <c r="B80" s="0" t="n">
+      <c r="B80" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C80" s="0" t="n">
+      <c r="C80" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>1170</v>
       </c>
-      <c r="B81" s="0" t="n">
+      <c r="B81" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C81" s="0" t="n">
+      <c r="C81" s="1" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>1194</v>
       </c>
-      <c r="B82" s="0" t="n">
+      <c r="B82" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C82" s="0" t="n">
+      <c r="C82" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="B83" s="0" t="n">
+      <c r="B83" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C83" s="0" t="n">
+      <c r="C83" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="B84" s="0" t="n">
+      <c r="B84" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C84" s="0" t="n">
+      <c r="C84" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -13620,7 +13661,7 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -13808,7 +13849,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -13911,7 +13952,7 @@
       <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -14044,7 +14085,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -14076,7 +14117,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -14147,7 +14188,7 @@
       <selection pane="topLeft" activeCell="D66" activeCellId="0" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -14853,7 +14894,7 @@
       <c r="C40" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="F40" s="1" t="n">
         <v>211</v>
       </c>
       <c r="G40" s="1" t="s">
@@ -14870,7 +14911,7 @@
       <c r="C41" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41" s="1" t="n">
         <v>212</v>
       </c>
       <c r="G41" s="1" t="s">
@@ -14887,7 +14928,7 @@
       <c r="C42" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42" s="1" t="n">
         <v>213</v>
       </c>
       <c r="G42" s="1" t="s">
@@ -15147,7 +15188,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="1" t="n">
         <v>462</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -15161,7 +15202,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+      <c r="A62" s="1" t="n">
         <v>463</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -15175,7 +15216,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="1" t="n">
         <v>464</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -15189,7 +15230,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="A64" s="1" t="n">
         <v>465</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -15203,7 +15244,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="1" t="n">
         <v>466</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -15242,7 +15283,7 @@
       <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Made Lich Lord a bit less OP, introduced spell dmg reduction
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -4439,7 +4439,7 @@
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4488,7 +4488,7 @@
       <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -4897,7 +4897,7 @@
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -5001,7 +5001,7 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -5347,7 +5347,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5551,7 +5551,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -5775,7 +5775,7 @@
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
@@ -6744,7 +6744,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -6859,7 +6859,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
@@ -6910,7 +6910,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6939,7 +6939,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -7785,10 +7785,10 @@
   <dimension ref="A1:A85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7893,7 +7893,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8057,7 +8057,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -8273,7 +8273,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.6"/>
@@ -8357,7 +8357,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -8498,7 +8498,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -8722,7 +8722,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -9178,7 +9178,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
@@ -9235,7 +9235,7 @@
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -10583,7 +10583,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -10708,7 +10708,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -10772,7 +10772,7 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="70" t="s">
@@ -10901,7 +10901,7 @@
       <selection pane="topLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -11379,7 +11379,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.1"/>
   </cols>
@@ -12211,7 +12211,7 @@
       <selection pane="topLeft" activeCell="K32" activeCellId="0" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -12283,7 +12283,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -12323,7 +12323,7 @@
       <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.92"/>
   </cols>
@@ -12434,7 +12434,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -12445,7 +12445,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -12455,9 +12455,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0"/>
-    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>554</v>
@@ -12483,26 +12481,26 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>460</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>456</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>457</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>1160</v>
       </c>
     </row>
@@ -12531,7 +12529,7 @@
       <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.35"/>
   </cols>
@@ -13757,7 +13755,7 @@
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -13950,7 +13948,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -14053,7 +14051,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -14218,7 +14216,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -14289,7 +14287,7 @@
       <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -15384,7 +15382,7 @@
       <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Fixed issue where you received dmg near alchemist tower
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -76,37 +76,37 @@
     <t xml:space="preserve">Tile issue at bottom rocks in lava stream (player is drawn above when moving from top to bottom but not after spawning there, in remake). Also on the lower middle lava island. Seems like a remake bug.</t>
   </si>
   <si>
+    <t xml:space="preserve">Fix original bugs:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Lava tile must block walk and horse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Fix stairs in Thalion office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Fix non-blocking walls in 3 maps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA Bugs:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torch in ice cave gfx issue on amiga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See sheet „Custom Translations“ here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texte verfeinern (besonders die Bücher)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe later:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Make many monsters „only move when see player“</t>
   </si>
   <si>
     <t xml:space="preserve">Done for: Paladin Guild, Fire temple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fix original bugs:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Lava tile must block walk and horse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Fix stairs in Thalion office</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Fix non-blocking walls in 3 maps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AA Bugs:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torch in ice cave gfx issue on amiga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See sheet „Custom Translations“ here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texte verfeinern (besonders die Bücher)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maybe later:</t>
   </si>
   <si>
     <t xml:space="preserve">Hide more stones of knowledge (currently there are 3 I guess)</t>
@@ -3812,16 +3812,16 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF468A1A"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF468A1A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -4181,7 +4181,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4213,15 +4213,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4265,7 +4265,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4297,7 +4297,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4305,19 +4305,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4377,7 +4377,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4417,7 +4417,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4541,7 +4541,7 @@
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4590,7 +4590,7 @@
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -4999,7 +4999,7 @@
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -5103,7 +5103,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -5449,7 +5449,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5653,7 +5653,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -5877,7 +5877,7 @@
       <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
@@ -6868,7 +6868,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -6983,16 +6983,16 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>744</v>
       </c>
     </row>
@@ -7034,7 +7034,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7063,7 +7063,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -7909,10 +7909,10 @@
   <dimension ref="A1:A85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7930,224 +7930,212 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
+      <c r="A10" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
+      <c r="A20" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>17</v>
+      <c r="A28" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
+      <c r="A34" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>24</v>
+      <c r="A36" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
+      <c r="A44" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>33</v>
+      <c r="A46" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -8197,7 +8185,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -8413,7 +8401,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.6"/>
@@ -8497,7 +8485,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -8638,7 +8626,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -8862,7 +8850,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -9318,7 +9306,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
@@ -9375,7 +9363,7 @@
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -10723,7 +10711,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -10848,7 +10836,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -10922,7 +10910,7 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="71" t="s">
@@ -11051,7 +11039,7 @@
       <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -11529,7 +11517,7 @@
       <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.1"/>
   </cols>
@@ -12036,9 +12024,9 @@
       <c r="G24" s="1" t="s">
         <v>1169</v>
       </c>
-      <c r="H24" s="1" t="n">
+      <c r="H24" s="1" t="e">
         <f aca="false">levelfromexp(H23,VLOOKUP(H22,G2:H10,2,0))</f>
-        <v>38</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12416,7 +12404,7 @@
       <selection pane="topLeft" activeCell="K32" activeCellId="0" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -12488,7 +12476,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -12528,7 +12516,7 @@
       <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.92"/>
   </cols>
@@ -12876,7 +12864,7 @@
       <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.35"/>
   </cols>
@@ -14102,7 +14090,7 @@
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -14295,7 +14283,7 @@
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -14403,7 +14391,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -14568,7 +14556,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -14639,7 +14627,7 @@
       <selection pane="topLeft" activeCell="D69" activeCellId="0" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -15860,7 +15848,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Some text adjustments and added english translations
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -781,7 +781,7 @@
     <t xml:space="preserve">Holy Sword</t>
   </si>
   <si>
-    <t xml:space="preserve">Blind-Branntwein / Blinding Booze</t>
+    <t xml:space="preserve">Blind-Branntwein / Blind Brandy</t>
   </si>
   <si>
     <t xml:space="preserve">Potion</t>
@@ -3656,10 +3656,10 @@
     <t xml:space="preserve"> einige</t>
   </si>
   <si>
-    <t xml:space="preserve">New goto point 90, and map text 0 (name)</t>
-  </si>
-  <si>
     <t xml:space="preserve">same as 233:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New goto point 90</t>
   </si>
   <si>
     <t xml:space="preserve">Objects</t>
@@ -3788,7 +3788,7 @@
     <numFmt numFmtId="168" formatCode="dd/\ mmm"/>
     <numFmt numFmtId="169" formatCode="\+0\%;\-0\%;&quot;No change&quot;"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3860,6 +3860,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -4132,7 +4138,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4441,6 +4447,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4541,7 +4551,7 @@
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4590,7 +4600,7 @@
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.15"/>
@@ -4999,7 +5009,7 @@
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.53"/>
@@ -5103,7 +5113,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61.58"/>
@@ -5449,7 +5459,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5653,7 +5663,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
@@ -5877,7 +5887,7 @@
       <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.44"/>
@@ -6868,7 +6878,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
   </cols>
@@ -6983,7 +6993,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
   </cols>
@@ -7034,7 +7044,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7063,7 +7073,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.29"/>
@@ -7908,11 +7918,11 @@
   </sheetPr>
   <dimension ref="A1:A85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8185,7 +8195,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -8401,7 +8411,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.6"/>
@@ -8485,7 +8495,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.88"/>
@@ -8626,7 +8636,7 @@
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.02"/>
@@ -8850,7 +8860,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
@@ -9306,7 +9316,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.57"/>
   </cols>
@@ -9363,7 +9373,7 @@
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
@@ -10711,7 +10721,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.69"/>
@@ -10836,7 +10846,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -10910,7 +10920,7 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="71" t="s">
@@ -11039,7 +11049,7 @@
       <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.42"/>
   </cols>
@@ -11517,7 +11527,7 @@
       <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.1"/>
   </cols>
@@ -12404,7 +12414,7 @@
       <selection pane="topLeft" activeCell="K32" activeCellId="0" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -12476,7 +12486,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -12512,11 +12522,11 @@
   </sheetPr>
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.92"/>
   </cols>
@@ -12736,8 +12746,8 @@
       <c r="A34" s="1" t="n">
         <v>474</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>1198</v>
+      <c r="B34" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12764,7 +12774,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12775,7 +12785,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>374</v>
+      </c>
+      <c r="C39" s="77" t="s">
+        <v>1199</v>
+      </c>
+    </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
@@ -12864,17 +12881,17 @@
       <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>1204</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
       <c r="E1" s="9" t="s">
         <v>1205</v>
       </c>
@@ -12883,25 +12900,25 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="79" t="s">
         <v>1206</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="79" t="s">
         <v>1208</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="80" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="80" t="s">
         <v>1209</v>
       </c>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="80" t="s">
         <v>1210</v>
       </c>
-      <c r="H2" s="79" t="s">
+      <c r="H2" s="80" t="s">
         <v>1211</v>
       </c>
     </row>
@@ -12998,18 +13015,18 @@
       <c r="C8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="81" t="s">
         <v>1215</v>
       </c>
-      <c r="F8" s="80" t="n">
+      <c r="F8" s="81" t="n">
         <f aca="false">SUM(F3:F7)</f>
         <v>5</v>
       </c>
-      <c r="G8" s="80" t="n">
+      <c r="G8" s="81" t="n">
         <f aca="false">SUM(G3:G7)</f>
         <v>5</v>
       </c>
-      <c r="H8" s="80" t="n">
+      <c r="H8" s="81" t="n">
         <f aca="false">SUM(H3:H7)</f>
         <v>10</v>
       </c>
@@ -13046,10 +13063,10 @@
       <c r="C11" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E11" s="80" t="s">
+      <c r="E11" s="81" t="s">
         <v>1218</v>
       </c>
-      <c r="F11" s="80" t="n">
+      <c r="F11" s="81" t="n">
         <v>10</v>
       </c>
     </row>
@@ -13063,10 +13080,10 @@
       <c r="C12" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="E12" s="80" t="s">
+      <c r="E12" s="81" t="s">
         <v>1220</v>
       </c>
-      <c r="F12" s="80" t="n">
+      <c r="F12" s="81" t="n">
         <v>7</v>
       </c>
     </row>
@@ -13141,16 +13158,16 @@
       <c r="C18" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E18" s="79" t="s">
+      <c r="E18" s="80" t="s">
         <v>1206</v>
       </c>
-      <c r="F18" s="79" t="s">
+      <c r="F18" s="80" t="s">
         <v>1207</v>
       </c>
-      <c r="G18" s="79" t="s">
+      <c r="G18" s="80" t="s">
         <v>1208</v>
       </c>
-      <c r="H18" s="79" t="s">
+      <c r="H18" s="80" t="s">
         <v>1228</v>
       </c>
     </row>
@@ -13171,7 +13188,7 @@
         <f aca="false">C3+C26+C34+C41+C48+C55+C63+C70+C77</f>
         <v>33</v>
       </c>
-      <c r="G19" s="80" t="n">
+      <c r="G19" s="81" t="n">
         <f aca="false">F19</f>
         <v>33</v>
       </c>
@@ -13197,7 +13214,7 @@
         <f aca="false">B4+B29+B66+B71+(F19-B3)*(F11/2)</f>
         <v>209</v>
       </c>
-      <c r="G20" s="80" t="n">
+      <c r="G20" s="81" t="n">
         <f aca="false">C4+C29+C66+C71+(G19-C3)*F11+H8</f>
         <v>391</v>
       </c>
@@ -13226,7 +13243,7 @@
         <f aca="false">B5+B30+B81+(F19-B3)*(F12/2)</f>
         <v>147</v>
       </c>
-      <c r="G21" s="80" t="n">
+      <c r="G21" s="81" t="n">
         <f aca="false">B5+B30+B81+(F19-B3)*F12</f>
         <v>259</v>
       </c>
@@ -13252,7 +13269,7 @@
         <f aca="false">B6+B37+B50</f>
         <v>5</v>
       </c>
-      <c r="G22" s="80" t="n">
+      <c r="G22" s="81" t="n">
         <f aca="false">F22</f>
         <v>5</v>
       </c>
@@ -13278,7 +13295,7 @@
         <f aca="false">B7+B36+B56+B65+ROUNDDOWN(F25/25,0)</f>
         <v>20</v>
       </c>
-      <c r="G23" s="80" t="n">
+      <c r="G23" s="81" t="n">
         <f aca="false">C7+C36+C56+C65+F8+ROUNDDOWN(G25/25,0)</f>
         <v>31</v>
       </c>
@@ -13298,7 +13315,7 @@
         <f aca="false">B8+B42+B57+ROUNDDOWN(F29/25,0)</f>
         <v>17</v>
       </c>
-      <c r="G24" s="80" t="n">
+      <c r="G24" s="81" t="n">
         <f aca="false">C8+C42+C57+G8+ROUNDDOWN(G29/25,0)</f>
         <v>27</v>
       </c>
@@ -13311,13 +13328,13 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="79" t="s">
         <v>1172</v>
       </c>
-      <c r="B25" s="78" t="s">
+      <c r="B25" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C25" s="78" t="s">
+      <c r="C25" s="79" t="s">
         <v>1208</v>
       </c>
       <c r="E25" s="69" t="s">
@@ -13327,7 +13344,7 @@
         <f aca="false">B9+B44+B64</f>
         <v>25</v>
       </c>
-      <c r="G25" s="80" t="n">
+      <c r="G25" s="81" t="n">
         <f aca="false">C9+C44+C64</f>
         <v>30</v>
       </c>
@@ -13353,7 +13370,7 @@
         <f aca="false">B10+B78</f>
         <v>15</v>
       </c>
-      <c r="G26" s="80" t="n">
+      <c r="G26" s="81" t="n">
         <f aca="false">C10+C78</f>
         <v>25</v>
       </c>
@@ -13379,7 +13396,7 @@
         <f aca="false">B11+B79</f>
         <v>30</v>
       </c>
-      <c r="G27" s="80" t="n">
+      <c r="G27" s="81" t="n">
         <f aca="false">C11+C79</f>
         <v>35</v>
       </c>
@@ -13405,7 +13422,7 @@
         <f aca="false">B12+B49</f>
         <v>145</v>
       </c>
-      <c r="G28" s="80" t="n">
+      <c r="G28" s="81" t="n">
         <f aca="false">C12+C49</f>
         <v>160</v>
       </c>
@@ -13431,7 +13448,7 @@
         <f aca="false">B13+B27+B58</f>
         <v>22</v>
       </c>
-      <c r="G29" s="80" t="n">
+      <c r="G29" s="81" t="n">
         <f aca="false">C13+C27+C58</f>
         <v>30</v>
       </c>
@@ -13457,7 +13474,7 @@
         <f aca="false">B14+B59+B80</f>
         <v>25</v>
       </c>
-      <c r="G30" s="80" t="n">
+      <c r="G30" s="81" t="n">
         <f aca="false">C14+C59+C80</f>
         <v>70</v>
       </c>
@@ -13474,7 +13491,7 @@
         <f aca="false">B15</f>
         <v>15</v>
       </c>
-      <c r="G31" s="80" t="n">
+      <c r="G31" s="81" t="n">
         <f aca="false">C15</f>
         <v>95</v>
       </c>
@@ -13491,7 +13508,7 @@
         <f aca="false">B16+B35+B43+B51</f>
         <v>15</v>
       </c>
-      <c r="G32" s="80" t="n">
+      <c r="G32" s="81" t="n">
         <f aca="false">C16+C35+C43+C51</f>
         <v>15</v>
       </c>
@@ -13501,13 +13518,13 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="78" t="s">
+      <c r="A33" s="79" t="s">
         <v>416</v>
       </c>
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C33" s="78" t="s">
+      <c r="C33" s="79" t="s">
         <v>1208</v>
       </c>
       <c r="E33" s="69" t="s">
@@ -13516,7 +13533,7 @@
       <c r="F33" s="69" t="n">
         <v>30</v>
       </c>
-      <c r="G33" s="80" t="n">
+      <c r="G33" s="81" t="n">
         <v>85</v>
       </c>
       <c r="H33" s="69" t="n">
@@ -13540,7 +13557,7 @@
       <c r="F34" s="69" t="n">
         <v>0</v>
       </c>
-      <c r="G34" s="80" t="n">
+      <c r="G34" s="81" t="n">
         <v>25</v>
       </c>
       <c r="H34" s="69" t="n">
@@ -13565,7 +13582,7 @@
         <f aca="false">B19+B28</f>
         <v>20</v>
       </c>
-      <c r="G35" s="80" t="n">
+      <c r="G35" s="81" t="n">
         <v>99</v>
       </c>
       <c r="H35" s="69" t="n">
@@ -13589,7 +13606,7 @@
       <c r="F36" s="69" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="80" t="n">
+      <c r="G36" s="81" t="n">
         <f aca="false">C20+C82</f>
         <v>5</v>
       </c>
@@ -13614,7 +13631,7 @@
       <c r="F37" s="69" t="n">
         <v>20</v>
       </c>
-      <c r="G37" s="80" t="n">
+      <c r="G37" s="81" t="n">
         <v>60</v>
       </c>
       <c r="H37" s="69" t="n">
@@ -13630,7 +13647,7 @@
         <f aca="false">B22+B45+B60+B84</f>
         <v>3</v>
       </c>
-      <c r="G38" s="80" t="n">
+      <c r="G38" s="81" t="n">
         <f aca="false">F38</f>
         <v>3</v>
       </c>
@@ -13647,7 +13664,7 @@
         <f aca="false">B23+B67+B72+B83</f>
         <v>3</v>
       </c>
-      <c r="G39" s="80" t="n">
+      <c r="G39" s="81" t="n">
         <f aca="false">F39</f>
         <v>3</v>
       </c>
@@ -13657,13 +13674,13 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="78" t="s">
+      <c r="A40" s="79" t="s">
         <v>432</v>
       </c>
-      <c r="B40" s="78" t="s">
+      <c r="B40" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C40" s="78" t="s">
+      <c r="C40" s="79" t="s">
         <v>1208</v>
       </c>
     </row>
@@ -13723,13 +13740,13 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="78" t="s">
+      <c r="A47" s="79" t="s">
         <v>1174</v>
       </c>
-      <c r="B47" s="78" t="s">
+      <c r="B47" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C47" s="78" t="s">
+      <c r="C47" s="79" t="s">
         <v>1208</v>
       </c>
     </row>
@@ -13778,13 +13795,13 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="78" t="s">
+      <c r="A54" s="79" t="s">
         <v>1176</v>
       </c>
-      <c r="B54" s="78" t="s">
+      <c r="B54" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C54" s="78" t="s">
+      <c r="C54" s="79" t="s">
         <v>1208</v>
       </c>
     </row>
@@ -13855,13 +13872,13 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="78" t="s">
+      <c r="A62" s="79" t="s">
         <v>1178</v>
       </c>
-      <c r="B62" s="78" t="s">
+      <c r="B62" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C62" s="78" t="s">
+      <c r="C62" s="79" t="s">
         <v>1208</v>
       </c>
     </row>
@@ -13921,13 +13938,13 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="78" t="s">
+      <c r="A69" s="79" t="s">
         <v>1235</v>
       </c>
-      <c r="B69" s="78" t="s">
+      <c r="B69" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C69" s="78" t="s">
+      <c r="C69" s="79" t="s">
         <v>1208</v>
       </c>
     </row>
@@ -13965,13 +13982,13 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="78" t="s">
+      <c r="A76" s="79" t="s">
         <v>1236</v>
       </c>
-      <c r="B76" s="78" t="s">
+      <c r="B76" s="79" t="s">
         <v>1207</v>
       </c>
-      <c r="C76" s="78" t="s">
+      <c r="C76" s="79" t="s">
         <v>1208</v>
       </c>
     </row>
@@ -14086,11 +14103,11 @@
   </sheetPr>
   <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49"/>
   </cols>
@@ -14283,7 +14300,7 @@
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.42"/>
   </cols>
@@ -14391,7 +14408,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="99.69"/>
@@ -14556,7 +14573,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
@@ -14623,11 +14640,11 @@
   </sheetPr>
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D69" activeCellId="0" sqref="D69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.14"/>
@@ -15848,7 +15865,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>

</xml_diff>

<commit_message>
Added new cocoon objects
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Ambermoon Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71DD908-303A-452A-A819-0F8B14AC3ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC819171-90CF-42BA-920A-C40E023338C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="828" firstSheet="8" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="828" firstSheet="8" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="1237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="1239">
   <si>
     <t>Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -3812,9 +3812,6 @@
     <t>Wesp</t>
   </si>
   <si>
-    <t>Wesp Cave</t>
-  </si>
-  <si>
     <t>From Monster Gfx</t>
   </si>
   <si>
@@ -3828,6 +3825,15 @@
   </si>
   <si>
     <t>Wasps' nest</t>
+  </si>
+  <si>
+    <t>Cocoon</t>
+  </si>
+  <si>
+    <t>Wasp Cave</t>
+  </si>
+  <si>
+    <t>Broken cocoon</t>
   </si>
 </sst>
 </file>
@@ -5107,13 +5113,13 @@
         <v>378</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>452</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -8361,10 +8367,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8569,13 +8575,47 @@
         <v>1230</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>1231</v>
+        <v>1237</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>801</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>1232</v>
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>381</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>801</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>382</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>801</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -8668,7 +8708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -8796,10 +8836,10 @@
         <v>99</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>1235</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>1236</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>823</v>

</xml_diff>

<commit_message>
Added new map prototype
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Ambermoon Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC528C7-0345-4A13-B293-FC3CE05516B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3BD43D-2DBD-43F3-98A3-3880A19EA0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="828" firstSheet="8" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="828" firstSheet="8" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -8331,7 +8331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -8670,7 +8670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added tile fixes from original
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Ambermoon Advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC03FC8-DF40-4852-9EA3-BECFE37EE02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB066DD-5A6C-4AE9-8DC3-83900E89633F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="828" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="1254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="1255">
   <si>
     <t>Note: Never add more than 530 entries to an archive otherwise the Amiga version will fail.</t>
   </si>
@@ -3879,6 +3879,9 @@
   </si>
   <si>
     <t>Wesps still have same data as curse wesps</t>
+  </si>
+  <si>
+    <t>Wesp object sprites seem messed up</t>
   </si>
 </sst>
 </file>
@@ -8206,7 +8209,7 @@
   <dimension ref="A1:A52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8297,6 +8300,11 @@
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1254</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Worked on the swamp dungeon
</commit_message>
<xml_diff>
--- a/AmbermoonAdvanced.xlsx
+++ b/AmbermoonAdvanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Neue Daten Ep3" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,18 +32,19 @@
     <sheet name="ObjectGfx" sheetId="22" state="visible" r:id="rId23"/>
     <sheet name="WallGfx" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="Overlays" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="Tiles" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="SpellChanges" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="Quest - Sea Creatures" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="SpellDamage" sheetId="28" state="visible" r:id="rId29"/>
-    <sheet name="Black Mountains" sheetId="29" state="visible" r:id="rId30"/>
-    <sheet name="SavegamePatching" sheetId="30" state="visible" r:id="rId31"/>
-    <sheet name="CodeChanges" sheetId="31" state="visible" r:id="rId32"/>
-    <sheet name="Exp Table" sheetId="32" state="visible" r:id="rId33"/>
-    <sheet name="Bosses" sheetId="33" state="visible" r:id="rId34"/>
-    <sheet name="Portraits" sheetId="34" state="visible" r:id="rId35"/>
-    <sheet name="Custom Translate" sheetId="35" state="visible" r:id="rId36"/>
-    <sheet name="Kasimir Stats" sheetId="36" state="visible" r:id="rId37"/>
+    <sheet name="Floors" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Tiles" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="SpellChanges" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="Quest - Sea Creatures" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="SpellDamage" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="Black Mountains" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="SavegamePatching" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="CodeChanges" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="Exp Table" sheetId="33" state="visible" r:id="rId34"/>
+    <sheet name="Bosses" sheetId="34" state="visible" r:id="rId35"/>
+    <sheet name="Portraits" sheetId="35" state="visible" r:id="rId36"/>
+    <sheet name="Custom Translate" sheetId="36" state="visible" r:id="rId37"/>
+    <sheet name="Kasimir Stats" sheetId="37" state="visible" r:id="rId38"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.0001"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="1347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1350">
   <si>
     <t xml:space="preserve">Map texts</t>
   </si>
@@ -3041,6 +3042,15 @@
   </si>
   <si>
     <t xml:space="preserve">Inactive wall overlay right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swamp dungeon lower wall border</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grail temple floor (swampy)</t>
   </si>
   <si>
     <t xml:space="preserve">Tileset Graphics (Icon Gfx)</t>
@@ -5020,7 +5030,7 @@
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -11052,10 +11062,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11219,6 +11229,20 @@
         <v>932</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>946</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>937</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -11231,6 +11255,43 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>948</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -11249,19 +11310,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="G1" s="12" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>267</v>
@@ -11270,7 +11331,7 @@
         <v>263</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>267</v>
@@ -11287,7 +11348,7 @@
         <v>1193</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="G3" s="6" t="n">
         <v>4</v>
@@ -11296,7 +11357,7 @@
         <v>1167</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11307,7 +11368,7 @@
         <v>1194</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="G4" s="6" t="n">
         <v>4</v>
@@ -11316,7 +11377,7 @@
         <v>1168</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11327,7 +11388,7 @@
         <v>1195</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="G5" s="6" t="n">
         <v>4</v>
@@ -11336,7 +11397,7 @@
         <v>1169</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11347,7 +11408,7 @@
         <v>1196</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>4</v>
@@ -11356,7 +11417,7 @@
         <v>1170</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11367,7 +11428,7 @@
         <v>1197</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="G7" s="6" t="n">
         <v>4</v>
@@ -11376,7 +11437,7 @@
         <v>1171</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11387,7 +11448,7 @@
         <v>1198</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="G8" s="6" t="n">
         <v>4</v>
@@ -11396,7 +11457,7 @@
         <v>1172</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11407,7 +11468,7 @@
         <v>1199</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="G9" s="6" t="n">
         <v>4</v>
@@ -11416,7 +11477,7 @@
         <v>1173</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11427,7 +11488,7 @@
         <v>1200</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="G10" s="6" t="n">
         <v>4</v>
@@ -11436,7 +11497,7 @@
         <v>1174</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
   </sheetData>
@@ -11454,7 +11515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -11476,15 +11537,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="G1" s="12" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
@@ -11492,10 +11553,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>954</v>
+        <v>957</v>
       </c>
       <c r="D2" s="53"/>
       <c r="E2" s="54"/>
@@ -11503,429 +11564,429 @@
         <v>268</v>
       </c>
       <c r="H2" s="52" t="s">
-        <v>955</v>
+        <v>958</v>
       </c>
       <c r="I2" s="52" t="s">
         <v>263</v>
       </c>
       <c r="J2" s="52" t="s">
-        <v>956</v>
+        <v>959</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>957</v>
+        <v>960</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>958</v>
+        <v>961</v>
       </c>
       <c r="E3" s="55"/>
       <c r="G3" s="1" t="s">
-        <v>959</v>
+        <v>962</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>961</v>
+        <v>964</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>962</v>
+        <v>965</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>963</v>
+        <v>966</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>965</v>
+        <v>968</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>967</v>
+        <v>970</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>970</v>
+        <v>973</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>972</v>
+        <v>975</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>973</v>
+        <v>976</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>974</v>
+        <v>977</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>975</v>
+        <v>978</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>976</v>
+        <v>979</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>977</v>
+        <v>980</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>978</v>
+        <v>981</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>979</v>
+        <v>982</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>981</v>
+        <v>984</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>984</v>
+        <v>987</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>985</v>
+        <v>988</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>986</v>
+        <v>989</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>987</v>
+        <v>990</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>988</v>
+        <v>991</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>989</v>
+        <v>992</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>990</v>
+        <v>993</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>995</v>
+        <v>998</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>996</v>
+        <v>999</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>997</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>1000</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>1004</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>1005</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>1007</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>1009</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>1010</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>1011</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>1012</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>1013</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>1014</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>1015</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>1016</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>1017</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>1018</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>1020</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>1023</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>1024</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>1025</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>1026</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>1027</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>1028</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>1029</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>1030</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>1031</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>1032</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>1033</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>1036</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>1037</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>1039</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>1040</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>1042</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>1043</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>1044</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>1045</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>1046</v>
+        <v>1049</v>
       </c>
     </row>
   </sheetData>
@@ -11943,7 +12004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -11961,32 +12022,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>1047</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>1048</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>1049</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>1050</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>1051</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>1052</v>
+        <v>1055</v>
       </c>
     </row>
   </sheetData>
@@ -12000,7 +12061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -12019,20 +12080,20 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>1053</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>1054</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="56" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>1056</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12100,41 +12161,41 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>1057</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="30" t="s">
-        <v>1058</v>
+        <v>1061</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>1059</v>
+        <v>1062</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>1061</v>
+        <v>1064</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>1062</v>
+        <v>1065</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>1064</v>
+        <v>1067</v>
       </c>
       <c r="H15" s="43" t="s">
-        <v>1065</v>
+        <v>1068</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="60" t="s">
-        <v>1059</v>
+        <v>1062</v>
       </c>
       <c r="B16" s="44" t="n">
         <v>0</v>
@@ -12163,7 +12224,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="60" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="B17" s="44" t="n">
         <v>125</v>
@@ -12192,7 +12253,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="60" t="s">
-        <v>1061</v>
+        <v>1064</v>
       </c>
       <c r="B18" s="44" t="n">
         <v>100</v>
@@ -12221,7 +12282,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="60" t="s">
-        <v>1062</v>
+        <v>1065</v>
       </c>
       <c r="B19" s="44" t="n">
         <v>100</v>
@@ -12250,7 +12311,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="60" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
       <c r="B20" s="44" t="n">
         <v>75</v>
@@ -12279,7 +12340,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="60" t="s">
-        <v>1064</v>
+        <v>1067</v>
       </c>
       <c r="B21" s="44" t="n">
         <v>75</v>
@@ -12308,7 +12369,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="60" t="s">
-        <v>1065</v>
+        <v>1068</v>
       </c>
       <c r="B22" s="44" t="n">
         <v>75</v>
@@ -12337,7 +12398,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="61" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
       <c r="B23" s="46" t="n">
         <v>75</v>
@@ -12366,22 +12427,22 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>1067</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>1068</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12389,10 +12450,10 @@
         <v>268</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>1072</v>
+        <v>1075</v>
       </c>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
@@ -12402,13 +12463,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="44" t="s">
-        <v>1073</v>
+        <v>1076</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
       <c r="C33" s="64" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
       <c r="D33" s="64"/>
       <c r="E33" s="64"/>
@@ -12418,13 +12479,13 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="44" t="s">
-        <v>1076</v>
+        <v>1079</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
       <c r="C34" s="64" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
       <c r="D34" s="64"/>
       <c r="E34" s="64"/>
@@ -12434,13 +12495,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="44" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B35" s="36" t="s">
         <v>1077</v>
       </c>
-      <c r="B35" s="36" t="s">
-        <v>1074</v>
-      </c>
       <c r="C35" s="64" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
       <c r="D35" s="64"/>
       <c r="E35" s="64"/>
@@ -12450,13 +12511,13 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="44" t="s">
-        <v>1078</v>
+        <v>1081</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
       <c r="D36" s="65"/>
       <c r="E36" s="65"/>
@@ -12466,13 +12527,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="44" t="s">
-        <v>1080</v>
+        <v>1083</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>1062</v>
+        <v>1065</v>
       </c>
       <c r="C37" s="64" t="s">
-        <v>1081</v>
+        <v>1084</v>
       </c>
       <c r="D37" s="64"/>
       <c r="E37" s="64"/>
@@ -12482,13 +12543,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="44" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="C38" s="64" t="s">
-        <v>1081</v>
+        <v>1084</v>
       </c>
       <c r="D38" s="64"/>
       <c r="E38" s="64"/>
@@ -12498,13 +12559,13 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="44" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="C39" s="65" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
       <c r="D39" s="65"/>
       <c r="E39" s="65"/>
@@ -12517,10 +12578,10 @@
         <v>324</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="C40" s="65" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
       <c r="D40" s="65"/>
       <c r="E40" s="65"/>
@@ -12530,13 +12591,13 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="44" t="s">
-        <v>1084</v>
+        <v>1087</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
       <c r="C41" s="65" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
@@ -12546,13 +12607,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="44" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>1064</v>
+        <v>1067</v>
       </c>
       <c r="C42" s="65" t="s">
-        <v>1087</v>
+        <v>1090</v>
       </c>
       <c r="D42" s="65"/>
       <c r="E42" s="65"/>
@@ -12562,13 +12623,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="44" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>1065</v>
+        <v>1068</v>
       </c>
       <c r="C43" s="65" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
       <c r="D43" s="65"/>
       <c r="E43" s="65"/>
@@ -12578,13 +12639,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="44" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>1091</v>
+        <v>1094</v>
       </c>
       <c r="D44" s="65"/>
       <c r="E44" s="65"/>
@@ -12594,7 +12655,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="66" t="s">
-        <v>1080</v>
+        <v>1083</v>
       </c>
       <c r="B48" s="66"/>
       <c r="C48" s="66"/>
@@ -12606,17 +12667,17 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="66" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="B52" s="66"/>
       <c r="C52" s="66"/>
@@ -12628,12 +12689,12 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>1094</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="66" t="s">
-        <v>1095</v>
+        <v>1098</v>
       </c>
       <c r="B57" s="66"/>
       <c r="C57" s="66"/>
@@ -12645,72 +12706,72 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="67" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="67" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="67" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H73" s="66" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="I73" s="66"/>
       <c r="J73" s="66"/>
@@ -12718,483 +12779,483 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="67" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="67" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>1112</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="67" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>1113</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="67" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>1114</v>
+        <v>1117</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>1115</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="67" t="s">
-        <v>1116</v>
+        <v>1119</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>1117</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="67" t="s">
-        <v>1118</v>
+        <v>1121</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>1119</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="67" t="s">
-        <v>1120</v>
+        <v>1123</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="67" t="s">
-        <v>1122</v>
+        <v>1125</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>1123</v>
+        <v>1126</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="67" t="s">
-        <v>1118</v>
+        <v>1121</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>1119</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="67" t="s">
-        <v>1125</v>
+        <v>1128</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="67" t="s">
-        <v>1126</v>
+        <v>1129</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>1127</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="67" t="s">
-        <v>1128</v>
+        <v>1131</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>1129</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="67" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>1131</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="67" t="s">
-        <v>1132</v>
+        <v>1135</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="67" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>1136</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="67" t="s">
-        <v>1137</v>
+        <v>1140</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>1138</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="67" t="s">
-        <v>1139</v>
+        <v>1142</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>1140</v>
+        <v>1143</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>1141</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="67" t="s">
-        <v>1142</v>
+        <v>1145</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="67" t="s">
-        <v>1144</v>
+        <v>1147</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="67" t="s">
-        <v>1147</v>
+        <v>1150</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>1148</v>
+        <v>1151</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>1149</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="67" t="s">
-        <v>1150</v>
+        <v>1153</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>1151</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="67" t="s">
-        <v>1152</v>
+        <v>1155</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>1153</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="67" t="s">
-        <v>1154</v>
+        <v>1157</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>1155</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="67" t="s">
-        <v>1156</v>
+        <v>1159</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>1157</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="67" t="s">
-        <v>1158</v>
+        <v>1161</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>1159</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="67" t="s">
-        <v>1160</v>
+        <v>1163</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>1162</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="67" t="s">
-        <v>1163</v>
+        <v>1166</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>1164</v>
+        <v>1167</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>1165</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="67" t="s">
-        <v>1166</v>
+        <v>1169</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>1167</v>
+        <v>1170</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>1168</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="67" t="s">
-        <v>1169</v>
+        <v>1172</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>1170</v>
+        <v>1173</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="67" t="s">
-        <v>1171</v>
+        <v>1174</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>1172</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="67" t="s">
-        <v>1173</v>
+        <v>1176</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>1174</v>
+        <v>1177</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>1175</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="67" t="s">
-        <v>1176</v>
+        <v>1179</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>1177</v>
+        <v>1180</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>1178</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="67" t="s">
-        <v>1179</v>
+        <v>1182</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>1180</v>
+        <v>1183</v>
       </c>
       <c r="H106" s="6" t="s">
-        <v>1181</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="67" t="s">
-        <v>1182</v>
+        <v>1185</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>1183</v>
+        <v>1186</v>
       </c>
       <c r="H107" s="6" t="s">
-        <v>1184</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="67" t="s">
-        <v>1185</v>
+        <v>1188</v>
       </c>
       <c r="H108" s="6" t="s">
-        <v>1172</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="67" t="s">
-        <v>1186</v>
+        <v>1189</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>1187</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="67" t="s">
-        <v>1188</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="67" t="s">
-        <v>1189</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="67" t="s">
-        <v>1190</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="67" t="s">
-        <v>1191</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="67" t="s">
-        <v>1192</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="67" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>1194</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="67" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>1196</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="67" t="s">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>1198</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="67" t="s">
-        <v>1199</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="67" t="s">
-        <v>1120</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="67" t="s">
-        <v>1122</v>
+        <v>1125</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>1200</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="67" t="s">
-        <v>1199</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="67" t="s">
-        <v>1125</v>
+        <v>1128</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>1201</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="67" t="s">
-        <v>1202</v>
+        <v>1205</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>1203</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="67" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>1194</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="67" t="s">
-        <v>1204</v>
+        <v>1207</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>1205</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="67" t="s">
-        <v>1206</v>
+        <v>1209</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="67" t="s">
-        <v>1208</v>
+        <v>1211</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>1209</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="67" t="s">
-        <v>1210</v>
+        <v>1213</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>1211</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="67" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="67" t="s">
-        <v>1213</v>
+        <v>1216</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>1214</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="67" t="s">
-        <v>1215</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="67" t="s">
-        <v>1189</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13205,78 +13266,78 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="6" t="s">
-        <v>1216</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="67" t="s">
-        <v>1217</v>
+        <v>1220</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>1218</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="67" t="s">
-        <v>1219</v>
+        <v>1222</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>1220</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="67" t="s">
-        <v>1221</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="67" t="s">
-        <v>1222</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="67" t="s">
-        <v>1223</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="67" t="s">
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="67" t="s">
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="67" t="s">
-        <v>1226</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="67" t="s">
-        <v>1227</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="67" t="s">
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="67" t="s">
-        <v>1229</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="67" t="s">
-        <v>1230</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="67" t="s">
-        <v>1189</v>
+        <v>1192</v>
       </c>
     </row>
   </sheetData>
@@ -13309,7 +13370,66 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -13328,7 +13448,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="66" t="s">
-        <v>1231</v>
+        <v>1234</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -13346,10 +13466,10 @@
         <v>268</v>
       </c>
       <c r="D2" s="68" t="s">
-        <v>1232</v>
+        <v>1235</v>
       </c>
       <c r="E2" s="68" t="s">
-        <v>1233</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13360,7 +13480,7 @@
         <v>544</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>1234</v>
+        <v>1237</v>
       </c>
       <c r="D3" s="44" t="n">
         <v>7</v>
@@ -13377,10 +13497,10 @@
         <v>549</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="D4" s="69" t="s">
-        <v>1236</v>
+        <v>1239</v>
       </c>
       <c r="E4" s="44" t="n">
         <v>6</v>
@@ -13394,10 +13514,10 @@
         <v>549</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>1237</v>
+        <v>1240</v>
       </c>
       <c r="D5" s="69" t="s">
-        <v>1236</v>
+        <v>1239</v>
       </c>
       <c r="E5" s="70" t="n">
         <v>6</v>
@@ -13411,10 +13531,10 @@
         <v>544</v>
       </c>
       <c r="C6" s="70" t="s">
-        <v>1238</v>
+        <v>1241</v>
       </c>
       <c r="D6" s="72" t="s">
-        <v>1239</v>
+        <v>1242</v>
       </c>
       <c r="E6" s="70" t="n">
         <v>1</v>
@@ -13434,66 +13554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A13"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -13508,52 +13569,52 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>1240</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>1241</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>1242</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>1243</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>1244</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>1245</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>1246</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>1247</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>1248</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>1249</v>
+        <v>1252</v>
       </c>
     </row>
   </sheetData>
@@ -13567,7 +13628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -13582,19 +13643,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="73" t="s">
-        <v>1250</v>
+        <v>1253</v>
       </c>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
       <c r="D1" s="73"/>
       <c r="E1" s="73" t="s">
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="F1" s="73"/>
       <c r="G1" s="73"/>
       <c r="H1" s="73"/>
       <c r="I1" s="73" t="s">
-        <v>1252</v>
+        <v>1255</v>
       </c>
       <c r="J1" s="73"/>
       <c r="K1" s="73"/>
@@ -13610,16 +13671,16 @@
         <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1253</v>
+        <v>1256</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>21</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>1254</v>
+        <v>1257</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>1255</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13627,10 +13688,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>1256</v>
+        <v>1259</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>1257</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13638,10 +13699,10 @@
         <v>23</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>1258</v>
+        <v>1261</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>1259</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13649,35 +13710,35 @@
         <v>24</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>1260</v>
+        <v>1263</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>1261</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="6" t="s">
-        <v>1262</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I7" s="6" t="s">
-        <v>1263</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I8" s="6" t="s">
-        <v>1264</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I9" s="6" t="s">
-        <v>1265</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I10" s="6" t="s">
-        <v>1266</v>
+        <v>1269</v>
       </c>
     </row>
   </sheetData>
@@ -13696,7 +13757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -13714,28 +13775,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1268</v>
+        <v>1271</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1269</v>
+        <v>1272</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>855</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>1270</v>
+        <v>1273</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1271</v>
+        <v>1274</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1272</v>
+        <v>1275</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>1273</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13989,7 +14050,7 @@
         <v>164</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>1274</v>
+        <v>1277</v>
       </c>
       <c r="H10" s="6" t="n">
         <v>95</v>
@@ -14071,7 +14132,7 @@
         <v>559</v>
       </c>
       <c r="G15" s="74" t="s">
-        <v>1275</v>
+        <v>1278</v>
       </c>
       <c r="H15" s="75" t="n">
         <v>35</v>
@@ -14143,7 +14204,7 @@
         <v>1329</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>1276</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14172,7 +14233,7 @@
         <v>1770</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>1277</v>
+        <v>1280</v>
       </c>
       <c r="H22" s="77" t="str">
         <f aca="false">G4</f>
@@ -14192,7 +14253,7 @@
         <v>2023</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>1278</v>
+        <v>1281</v>
       </c>
       <c r="H23" s="77" t="n">
         <f aca="false">J4</f>
@@ -14212,7 +14273,7 @@
         <v>2299</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>1279</v>
+        <v>1282</v>
       </c>
       <c r="H24" s="6" t="e">
         <f aca="false">levelfromexp(H23,VLOOKUP(H22,G2:H10,2,0))</f>
@@ -14583,7 +14644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -14601,7 +14662,7 @@
         <v>511</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1280</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14609,39 +14670,39 @@
         <v>495</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1281</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>1282</v>
+        <v>1285</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1283</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>1284</v>
+        <v>1287</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>1285</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>1286</v>
+        <v>1289</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>1287</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>1288</v>
+        <v>1291</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>1289</v>
+        <v>1292</v>
       </c>
     </row>
   </sheetData>
@@ -14655,7 +14716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -14673,7 +14734,7 @@
         <v>103</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1290</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14681,7 +14742,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1291</v>
+        <v>1294</v>
       </c>
     </row>
   </sheetData>
@@ -14695,7 +14756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -14713,7 +14774,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>1292</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14724,7 +14785,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1293</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14735,28 +14796,28 @@
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1294</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>1295</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>1296</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>1292</v>
+        <v>1295</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>1297</v>
+        <v>1300</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1298</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14783,7 +14844,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>1299</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14802,7 +14863,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1300</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14810,10 +14871,10 @@
         <v>40</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>1301</v>
+        <v>1304</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>1302</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14821,10 +14882,10 @@
         <v>37</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>1301</v>
+        <v>1304</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1302</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14832,10 +14893,10 @@
         <v>45</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>1301</v>
+        <v>1304</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1302</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14846,7 +14907,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>1303</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14859,7 +14920,7 @@
         <v>470</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>1304</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14870,7 +14931,7 @@
         <v>33.34</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1305</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14894,7 +14955,7 @@
         <v>457</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>1306</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14902,7 +14963,7 @@
         <v>472</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>1307</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14953,7 +15014,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>1308</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14969,12 +15030,12 @@
         <v>374</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>1309</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>1310</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14987,7 +15048,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>1311</v>
+        <v>1314</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>684</v>
@@ -15000,7 +15061,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>1312</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15041,7 +15102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -15059,12 +15120,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="78" t="s">
-        <v>1313</v>
+        <v>1316</v>
       </c>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
       <c r="E1" s="13" t="s">
-        <v>1314</v>
+        <v>1317</v>
       </c>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -15072,30 +15133,30 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1316</v>
+        <v>1319</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1317</v>
+        <v>1320</v>
       </c>
       <c r="E2" s="79" t="s">
         <v>268</v>
       </c>
       <c r="F2" s="79" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="G2" s="79" t="s">
-        <v>1319</v>
+        <v>1322</v>
       </c>
       <c r="H2" s="79" t="s">
-        <v>1320</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
@@ -15104,7 +15165,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>1321</v>
+        <v>1324</v>
       </c>
       <c r="F3" s="70" t="n">
         <v>5</v>
@@ -15118,7 +15179,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>1320</v>
+        <v>1323</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>6</v>
@@ -15133,7 +15194,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>1322</v>
+        <v>1325</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>5</v>
@@ -15148,7 +15209,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>1323</v>
+        <v>1326</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>3</v>
@@ -15163,7 +15224,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>2</v>
@@ -15178,7 +15239,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>1319</v>
+        <v>1322</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>0</v>
@@ -15187,7 +15248,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="80" t="s">
-        <v>1324</v>
+        <v>1327</v>
       </c>
       <c r="F8" s="80" t="n">
         <f aca="false">SUM(F3:F7)</f>
@@ -15204,7 +15265,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>1325</v>
+        <v>1328</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>5</v>
@@ -15215,7 +15276,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>5</v>
@@ -15226,7 +15287,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>1326</v>
+        <v>1329</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>20</v>
@@ -15235,7 +15296,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="80" t="s">
-        <v>1327</v>
+        <v>1330</v>
       </c>
       <c r="F11" s="80" t="n">
         <v>10</v>
@@ -15243,7 +15304,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>1328</v>
+        <v>1331</v>
       </c>
       <c r="B12" s="6" t="n">
         <v>135</v>
@@ -15252,7 +15313,7 @@
         <v>150</v>
       </c>
       <c r="E12" s="80" t="s">
-        <v>1329</v>
+        <v>1332</v>
       </c>
       <c r="F12" s="80" t="n">
         <v>7</v>
@@ -15260,7 +15321,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>1330</v>
+        <v>1333</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>2</v>
@@ -15271,7 +15332,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>1331</v>
+        <v>1334</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>5</v>
@@ -15282,7 +15343,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>1332</v>
+        <v>1335</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>15</v>
@@ -15293,7 +15354,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>1333</v>
+        <v>1336</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0</v>
@@ -15304,7 +15365,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>1334</v>
+        <v>1337</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>30</v>
@@ -15313,7 +15374,7 @@
         <v>85</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>1335</v>
+        <v>1338</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -15321,7 +15382,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>1336</v>
+        <v>1339</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0</v>
@@ -15330,21 +15391,21 @@
         <v>25</v>
       </c>
       <c r="E18" s="79" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="F18" s="79" t="s">
-        <v>1316</v>
+        <v>1319</v>
       </c>
       <c r="G18" s="79" t="s">
-        <v>1317</v>
+        <v>1320</v>
       </c>
       <c r="H18" s="79" t="s">
-        <v>1337</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>1338</v>
+        <v>1341</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>0</v>
@@ -15353,7 +15414,7 @@
         <v>99</v>
       </c>
       <c r="E19" s="70" t="s">
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="F19" s="70" t="n">
         <f aca="false">C3+C26+C34+C41+C48+C55+C63+C70+C77</f>
@@ -15370,7 +15431,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>1339</v>
+        <v>1342</v>
       </c>
       <c r="B20" s="6" t="n">
         <v>0</v>
@@ -15379,7 +15440,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="70" t="s">
-        <v>1320</v>
+        <v>1323</v>
       </c>
       <c r="F20" s="70" t="n">
         <f aca="false">B4+B29+B66+B71+(F19-B3)*(F11/2)</f>
@@ -15394,12 +15455,12 @@
         <v>300</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>1340</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>1341</v>
+        <v>1344</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>20</v>
@@ -15408,7 +15469,7 @@
         <v>60</v>
       </c>
       <c r="E21" s="70" t="s">
-        <v>1322</v>
+        <v>1325</v>
       </c>
       <c r="F21" s="70" t="n">
         <f aca="false">B5+B30+B81+(F19-B3)*(F12/2)</f>
@@ -15425,7 +15486,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>1342</v>
+        <v>1345</v>
       </c>
       <c r="B22" s="6" t="n">
         <v>0</v>
@@ -15434,7 +15495,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="70" t="s">
-        <v>1323</v>
+        <v>1326</v>
       </c>
       <c r="F22" s="70" t="n">
         <f aca="false">B6+B37+B50</f>
@@ -15451,7 +15512,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>1343</v>
+        <v>1346</v>
       </c>
       <c r="B23" s="6" t="n">
         <v>0</v>
@@ -15460,7 +15521,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="70" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="F23" s="70" t="n">
         <f aca="false">B7+B36+B56+B65+ROUNDDOWN(F25/25,0)</f>
@@ -15475,12 +15536,12 @@
         <v>25</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>1340</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="70" t="s">
-        <v>1319</v>
+        <v>1322</v>
       </c>
       <c r="F24" s="70" t="n">
         <f aca="false">B8+B42+B57+ROUNDDOWN(F29/25,0)</f>
@@ -15495,21 +15556,21 @@
         <v>22</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>1340</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>1282</v>
+        <v>1285</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1316</v>
+        <v>1319</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>1317</v>
+        <v>1320</v>
       </c>
       <c r="E25" s="70" t="s">
-        <v>1325</v>
+        <v>1328</v>
       </c>
       <c r="F25" s="70" t="n">
         <f aca="false">B9+B44+B64</f>
@@ -15526,7 +15587,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="B26" s="6" t="n">
         <v>4</v>
@@ -15535,7 +15596,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="70" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
       <c r="F26" s="70" t="n">
         <f aca="false">B10+B78</f>
@@ -15552,7 +15613,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>1330</v>
+        <v>1333</v>
       </c>
       <c r="B27" s="6" t="n">
         <v>10</v>
@@ -15561,7 +15622,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="70" t="s">
-        <v>1326</v>
+        <v>1329</v>
       </c>
       <c r="F27" s="70" t="n">
         <f aca="false">B11+B79</f>
@@ -15578,7 +15639,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>1338</v>
+        <v>1341</v>
       </c>
       <c r="B28" s="6" t="n">
         <v>20</v>
@@ -15587,7 +15648,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="70" t="s">
-        <v>1328</v>
+        <v>1331</v>
       </c>
       <c r="F28" s="70" t="n">
         <f aca="false">B12+B49</f>
@@ -15604,7 +15665,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>1320</v>
+        <v>1323</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>18</v>
@@ -15613,7 +15674,7 @@
         <v>22</v>
       </c>
       <c r="E29" s="70" t="s">
-        <v>1330</v>
+        <v>1333</v>
       </c>
       <c r="F29" s="70" t="n">
         <f aca="false">B13+B27+B58</f>
@@ -15630,7 +15691,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>1322</v>
+        <v>1325</v>
       </c>
       <c r="B30" s="6" t="n">
         <v>5</v>
@@ -15639,7 +15700,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="70" t="s">
-        <v>1331</v>
+        <v>1334</v>
       </c>
       <c r="F30" s="70" t="n">
         <f aca="false">B14+B59+B80</f>
@@ -15656,7 +15717,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="70" t="s">
-        <v>1332</v>
+        <v>1335</v>
       </c>
       <c r="F31" s="70" t="n">
         <f aca="false">B15</f>
@@ -15673,7 +15734,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="70" t="s">
-        <v>1333</v>
+        <v>1336</v>
       </c>
       <c r="F32" s="70" t="n">
         <f aca="false">B16+B35+B43+B51</f>
@@ -15693,13 +15754,13 @@
         <v>495</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1316</v>
+        <v>1319</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>1317</v>
+        <v>1320</v>
       </c>
       <c r="E33" s="70" t="s">
-        <v>1334</v>
+        <v>1337</v>
       </c>
       <c r="F33" s="70" t="n">
         <v>30</v>
@@ -15714,7 +15775,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="B34" s="6" t="n">
         <v>4</v>
@@ -15723,7 +15784,7 @@
         <v>4</v>
       